<commit_message>
Fixed comparison bar chart (still hard-coded)
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1005" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9185693F-C470-40FF-B49D-17DA731C6194}"/>
+  <xr:revisionPtr revIDLastSave="1007" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53F20CB6-804D-4540-BD16-A798BBE83D98}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -1488,7 +1488,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1730,6 +1730,9 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5796,15 +5799,15 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.88671875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -5822,7 +5825,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>133</v>
       </c>
@@ -5838,7 +5841,7 @@
       <c r="E2" s="72"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -5858,7 +5861,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>105</v>
       </c>
@@ -5879,7 +5882,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>137</v>
       </c>
@@ -5897,7 +5900,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
         <v>193</v>
       </c>
@@ -5915,7 +5918,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>192</v>
       </c>
@@ -5934,7 +5937,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="70" t="s">
         <v>91</v>
       </c>
@@ -5952,7 +5955,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A9" s="70" t="s">
         <v>92</v>
       </c>
@@ -5970,7 +5973,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>88</v>
       </c>
@@ -5986,7 +5989,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>102</v>
       </c>
@@ -6002,7 +6005,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A12" s="68" t="s">
         <v>176</v>
       </c>
@@ -6023,7 +6026,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
         <v>200</v>
       </c>
@@ -6041,7 +6044,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
         <v>175</v>
       </c>
@@ -6061,7 +6064,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
         <v>174</v>
       </c>
@@ -6081,7 +6084,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A16" s="68" t="s">
         <v>180</v>
       </c>
@@ -6099,7 +6102,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A17" s="68" t="s">
         <v>165</v>
       </c>
@@ -6116,7 +6119,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A18" s="68" t="s">
         <v>86</v>
       </c>
@@ -6134,7 +6137,7 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>93</v>
       </c>
@@ -6150,7 +6153,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>163</v>
       </c>
@@ -6166,7 +6169,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>90</v>
       </c>
@@ -6182,7 +6185,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>100</v>
       </c>
@@ -6198,7 +6201,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>98</v>
       </c>
@@ -6214,7 +6217,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>107</v>
       </c>
@@ -6230,7 +6233,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="70" t="s">
         <v>195</v>
       </c>
@@ -6248,7 +6251,7 @@
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="70" t="s">
         <v>197</v>
       </c>
@@ -6266,7 +6269,7 @@
       </c>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>99</v>
       </c>
@@ -6282,7 +6285,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>112</v>
       </c>
@@ -6297,7 +6300,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>117</v>
       </c>
@@ -6311,7 +6314,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>114</v>
       </c>
@@ -6327,23 +6330,23 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A31" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="35">
-        <v>1000</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="84">
+        <v>2500</v>
+      </c>
+      <c r="D31" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="70"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>142</v>
       </c>
@@ -6359,7 +6362,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>108</v>
       </c>
@@ -6373,7 +6376,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A34" s="68" t="s">
         <v>106</v>
       </c>
@@ -6389,7 +6392,7 @@
       <c r="E34" s="72"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="68" t="s">
         <v>101</v>
       </c>
@@ -6407,7 +6410,7 @@
       </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A36" s="68" t="s">
         <v>87</v>
       </c>
@@ -6425,7 +6428,7 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A37" s="68" t="s">
         <v>85</v>
       </c>
@@ -6444,7 +6447,7 @@
       </c>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>103</v>
       </c>
@@ -6462,7 +6465,7 @@
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>104</v>
       </c>
@@ -6478,7 +6481,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>94</v>
       </c>
@@ -6494,7 +6497,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>95</v>
       </c>
@@ -6511,7 +6514,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>96</v>
       </c>
@@ -6528,7 +6531,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>97</v>
       </c>
@@ -6544,46 +6547,46 @@
       </c>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="8"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="9"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
     </row>
@@ -6623,27 +6626,27 @@
       <selection pane="topRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="42" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.140625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" style="43" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="42" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" style="43" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="58.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
@@ -6696,7 +6699,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>58</v>
       </c>
@@ -6734,7 +6737,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -6788,7 +6791,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>201</v>
       </c>
@@ -6839,7 +6842,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="41" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="41" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>24</v>
       </c>
@@ -6909,18 +6912,18 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -6934,13 +6937,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="32"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -6960,7 +6963,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>82</v>
       </c>
@@ -6976,7 +6979,7 @@
       <c r="E4" s="81"/>
       <c r="F4" s="80"/>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>81</v>
       </c>
@@ -6988,7 +6991,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -7004,7 +7007,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -7020,7 +7023,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
@@ -7036,7 +7039,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>45</v>
       </c>
@@ -7048,13 +7051,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="32"/>
       <c r="C10" s="45"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -7068,7 +7071,7 @@
       </c>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
@@ -7082,13 +7085,13 @@
       </c>
       <c r="D12" s="37"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="33"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>73</v>
       </c>
@@ -7130,26 +7133,26 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="49" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="49" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="49"/>
-    <col min="8" max="8" width="14.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="14.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="49"/>
+    <col min="8" max="8" width="14.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="50" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="13.7109375" style="49"/>
-    <col min="26" max="26" width="18.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="13.7109375" style="49"/>
+    <col min="17" max="25" width="13.6640625" style="49"/>
+    <col min="26" max="26" width="18.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="13.6640625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>124</v>
       </c>
@@ -7160,7 +7163,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="50" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="50" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>155</v>
       </c>
@@ -7172,13 +7175,13 @@
       </c>
       <c r="F2" s="49"/>
     </row>
-    <row r="3" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="F3" s="49"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>6</v>
       </c>
@@ -7192,7 +7195,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>9</v>
       </c>
@@ -7204,7 +7207,7 @@
       </c>
       <c r="D5" s="53"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>11</v>
       </c>
@@ -7216,7 +7219,7 @@
       </c>
       <c r="D6" s="54"/>
     </row>
-    <row r="7" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
         <v>13</v>
       </c>
@@ -7230,7 +7233,7 @@
       <c r="E7" s="49"/>
       <c r="F7" s="49"/>
     </row>
-    <row r="8" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>15</v>
       </c>
@@ -7244,7 +7247,7 @@
       <c r="E8" s="49"/>
       <c r="F8" s="49"/>
     </row>
-    <row r="9" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>156</v>
       </c>
@@ -7259,7 +7262,7 @@
       <c r="F9" s="49"/>
       <c r="L9" s="49"/>
     </row>
-    <row r="10" spans="1:12" s="50" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>129</v>
       </c>
@@ -7275,7 +7278,7 @@
       <c r="F10" s="49"/>
       <c r="L10" s="49"/>
     </row>
-    <row r="11" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>125</v>
       </c>
@@ -7291,7 +7294,7 @@
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
     </row>
-    <row r="12" spans="1:12" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="50" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>126</v>
       </c>
@@ -7307,7 +7310,7 @@
       <c r="F12" s="49"/>
       <c r="G12" s="49"/>
     </row>
-    <row r="13" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
@@ -7315,10 +7318,10 @@
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="50"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="83" t="s">
         <v>130</v>
       </c>
@@ -7339,7 +7342,7 @@
       <c r="O17" s="83"/>
       <c r="P17" s="83"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="82" t="s">
         <v>121</v>
       </c>
@@ -7369,7 +7372,7 @@
       <c r="O18" s="82"/>
       <c r="P18" s="82"/>
     </row>
-    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A19" s="55" t="s">
         <v>157</v>
       </c>
@@ -7417,7 +7420,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="59">
         <v>-51.5244564886654</v>
       </c>
@@ -7473,7 +7476,7 @@
         <v>5.0730403065140095E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="59">
         <v>-89.797974315320403</v>
       </c>
@@ -7529,7 +7532,7 @@
         <v>6.5460850237780699E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="59">
         <v>-128.06720097650799</v>
       </c>
@@ -7585,7 +7588,7 @@
         <v>8.6704673566159185E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="59">
         <v>-166.34194485043901</v>
       </c>
@@ -7641,7 +7644,7 @@
         <v>1.1771856112818058E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="59">
         <v>-204.613623606179</v>
       </c>
@@ -7697,7 +7700,7 @@
         <v>1.6610145177220037E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="59">
         <v>-242.881624220091</v>
       </c>
@@ -7753,7 +7756,7 @@
         <v>2.2533996934247069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="59">
         <v>-281.15268995219299</v>
       </c>
@@ -7809,7 +7812,7 @@
         <v>3.149742423062496E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="59">
         <v>-319.427433826124</v>
       </c>
@@ -7865,7 +7868,7 @@
         <v>4.8494015452431039E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="59">
         <v>-357.69420839275898</v>
       </c>
@@ -7921,7 +7924,7 @@
         <v>7.7219536858392002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="59">
         <v>-395.96343505394702</v>
       </c>
@@ -7977,7 +7980,7 @@
         <v>0.10626191485734104</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="59">
         <v>-434.23572683332497</v>
       </c>
@@ -8033,7 +8036,7 @@
         <v>-1.8498964897695203E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="59">
         <v>-472.50188837632197</v>
       </c>
@@ -8089,7 +8092,7 @@
         <v>-1.3483050770102256E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="59">
         <v>-510.774180155701</v>
       </c>
@@ -8132,7 +8135,7 @@
       <c r="O32" s="61"/>
       <c r="P32" s="61"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="59">
         <v>-549.04095472233598</v>
       </c>
@@ -8175,7 +8178,7 @@
       <c r="O33" s="61"/>
       <c r="P33" s="61"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="59">
         <v>-587.30895533624698</v>
       </c>
@@ -8218,7 +8221,7 @@
       <c r="O34" s="61"/>
       <c r="P34" s="61"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="59">
         <v>-625.57511687924398</v>
       </c>
@@ -8261,7 +8264,7 @@
       <c r="O35" s="61"/>
       <c r="P35" s="61"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="59">
         <v>-663.84066539860203</v>
       </c>
@@ -8304,7 +8307,7 @@
       <c r="O36" s="61"/>
       <c r="P36" s="61"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="59">
         <v>-702.104987870684</v>
       </c>
@@ -8347,7 +8350,7 @@
       <c r="O37" s="61"/>
       <c r="P37" s="61"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="59">
         <v>-740.36747127185197</v>
       </c>
@@ -8390,7 +8393,7 @@
       <c r="O38" s="61"/>
       <c r="P38" s="61"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="59">
         <v>-778.62934164938099</v>
       </c>
@@ -8433,7 +8436,7 @@
       <c r="O39" s="61"/>
       <c r="P39" s="61"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="59">
         <v>-816.88814690872005</v>
       </c>
@@ -8476,7 +8479,7 @@
       <c r="O40" s="61"/>
       <c r="P40" s="61"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="59">
         <v>-855.14633914442004</v>
       </c>
@@ -8519,7 +8522,7 @@
       <c r="O41" s="61"/>
       <c r="P41" s="61"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="59">
         <v>-893.40453138012003</v>
       </c>
@@ -8562,7 +8565,7 @@
       <c r="O42" s="61"/>
       <c r="P42" s="61"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="59">
         <v>-931.65781942671504</v>
       </c>
@@ -8605,7 +8608,7 @@
       <c r="O43" s="61"/>
       <c r="P43" s="61"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="59">
         <v>-969.90988142603396</v>
       </c>
@@ -8648,7 +8651,7 @@
       <c r="O44" s="61"/>
       <c r="P44" s="61"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="59">
         <v>-1008.15397411805</v>
       </c>
@@ -8691,7 +8694,7 @@
       <c r="O45" s="61"/>
       <c r="P45" s="61"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="59">
         <v>-1046.3962277391599</v>
       </c>
@@ -8734,7 +8737,7 @@
       <c r="O46" s="61"/>
       <c r="P46" s="61"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="59">
         <v>-1084.6305120529701</v>
       </c>
@@ -8777,7 +8780,7 @@
       <c r="O47" s="61"/>
       <c r="P47" s="61"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="59">
         <v>-1122.8660224140599</v>
       </c>
@@ -8807,7 +8810,7 @@
       <c r="O48" s="61"/>
       <c r="P48" s="61"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="59">
         <v>-1161.08743323147</v>
       </c>
@@ -8837,7 +8840,7 @@
       <c r="O49" s="61"/>
       <c r="P49" s="61"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="59">
         <v>-1199.30516590705</v>
       </c>
@@ -8867,7 +8870,7 @@
       <c r="O50" s="61"/>
       <c r="P50" s="61"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="59">
         <v>-1237.5192204407999</v>
       </c>
@@ -8897,7 +8900,7 @@
       <c r="O51" s="61"/>
       <c r="P51" s="61"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="59">
         <v>-1275.72530566725</v>
       </c>
@@ -8927,7 +8930,7 @@
       <c r="O52" s="61"/>
       <c r="P52" s="61"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="59">
         <v>-1313.9283257755101</v>
       </c>
@@ -8957,7 +8960,7 @@
       <c r="O53" s="61"/>
       <c r="P53" s="61"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="59">
         <v>-1352.1258286710299</v>
       </c>
@@ -8987,7 +8990,7 @@
       <c r="O54" s="61"/>
       <c r="P54" s="61"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="59">
         <v>-1390.3306878502101</v>
       </c>
@@ -9017,7 +9020,7 @@
       <c r="O55" s="61"/>
       <c r="P55" s="61"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="59">
         <v>-1428.5300298166501</v>
       </c>
@@ -9047,7 +9050,7 @@
       <c r="O56" s="61"/>
       <c r="P56" s="61"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="59">
         <v>-1466.7189503812299</v>
       </c>
@@ -9077,7 +9080,7 @@
       <c r="O57" s="61"/>
       <c r="P57" s="61"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="59">
         <v>-1499.6968635093899</v>
       </c>
@@ -9107,7 +9110,7 @@
       <c r="O58" s="61"/>
       <c r="P58" s="61"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J62" s="63"/>
       <c r="K62" s="49"/>
       <c r="L62" s="49"/>
@@ -9116,7 +9119,7 @@
       <c r="O62" s="49"/>
       <c r="P62" s="49"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H63" s="82" t="s">
         <v>124</v>
       </c>
@@ -9129,7 +9132,7 @@
       <c r="O63" s="49"/>
       <c r="P63" s="49"/>
     </row>
-    <row r="64" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
       <c r="H64" s="64" t="s">
         <v>159</v>
       </c>
@@ -9144,7 +9147,7 @@
       <c r="O64" s="49"/>
       <c r="P64" s="49"/>
     </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H65" s="65">
         <v>2.2997934048565084E-2</v>
       </c>
@@ -9160,7 +9163,7 @@
       <c r="O65" s="49"/>
       <c r="P65" s="49"/>
     </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H66" s="65">
         <v>4.0069676396611777E-2</v>
       </c>
@@ -9176,7 +9179,7 @@
       <c r="O66" s="49"/>
       <c r="P66" s="49"/>
     </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H67" s="65">
         <v>5.7084370034302737E-2</v>
       </c>
@@ -9192,7 +9195,7 @@
       <c r="O67" s="49"/>
       <c r="P67" s="49"/>
     </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H68" s="65">
         <v>7.4140086301005395E-2</v>
       </c>
@@ -9208,7 +9211,7 @@
       <c r="O68" s="49"/>
       <c r="P68" s="49"/>
     </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H69" s="65">
         <v>9.1140638350711872E-2</v>
       </c>
@@ -9224,7 +9227,7 @@
       <c r="O69" s="49"/>
       <c r="P69" s="49"/>
     </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H70" s="65">
         <v>0.1080445517892699</v>
       </c>
@@ -9240,7 +9243,7 @@
       <c r="O70" s="49"/>
       <c r="P70" s="49"/>
     </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H71" s="65">
         <v>0.12497606826753388</v>
       </c>
@@ -9256,7 +9259,7 @@
       <c r="O71" s="49"/>
       <c r="P71" s="49"/>
     </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H72" s="65">
         <v>0.14198052165390951</v>
       </c>
@@ -9272,7 +9275,7 @@
       <c r="O72" s="49"/>
       <c r="P72" s="49"/>
     </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H73" s="65">
         <v>0.15874470475517963</v>
       </c>
@@ -9288,7 +9291,7 @@
       <c r="O73" s="49"/>
       <c r="P73" s="49"/>
     </row>
-    <row r="74" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H74" s="65">
         <v>0.17553747925232432</v>
       </c>
@@ -9304,7 +9307,7 @@
       <c r="O74" s="49"/>
       <c r="P74" s="49"/>
     </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H75" s="65">
         <v>0.19240417629290971</v>
       </c>
@@ -9320,7 +9323,7 @@
       <c r="O75" s="49"/>
       <c r="P75" s="49"/>
     </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H76" s="65">
         <v>0.20901220546271423</v>
       </c>
@@ -9336,7 +9339,7 @@
       <c r="O76" s="49"/>
       <c r="P76" s="49"/>
     </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H77" s="65">
         <v>0.22582431925537669</v>
       </c>
@@ -9352,7 +9355,7 @@
       <c r="O77" s="49"/>
       <c r="P77" s="49"/>
     </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H78" s="65">
         <v>0.24236713011424937</v>
       </c>
@@ -9368,7 +9371,7 @@
       <c r="O78" s="49"/>
       <c r="P78" s="49"/>
     </row>
-    <row r="79" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H79" s="65">
         <v>0.25891734586657894</v>
       </c>
@@ -9384,7 +9387,7 @@
       <c r="O79" s="49"/>
       <c r="P79" s="49"/>
     </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H80" s="65">
         <v>0.27532743679881172</v>
       </c>
@@ -9400,7 +9403,7 @@
       <c r="O80" s="49"/>
       <c r="P80" s="49"/>
     </row>
-    <row r="81" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H81" s="65">
         <v>0.29164753874763422</v>
       </c>
@@ -9416,7 +9419,7 @@
       <c r="O81" s="49"/>
       <c r="P81" s="49"/>
     </row>
-    <row r="82" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H82" s="65">
         <v>0.30783618288424536</v>
       </c>
@@ -9432,7 +9435,7 @@
       <c r="O82" s="49"/>
       <c r="P82" s="49"/>
     </row>
-    <row r="83" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H83" s="65">
         <v>0.32384418347196781</v>
       </c>
@@ -9448,7 +9451,7 @@
       <c r="O83" s="49"/>
       <c r="P83" s="49"/>
     </row>
-    <row r="84" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H84" s="65">
         <v>0.33973325501759533</v>
       </c>
@@ -9464,7 +9467,7 @@
       <c r="O84" s="49"/>
       <c r="P84" s="49"/>
     </row>
-    <row r="85" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H85" s="65">
         <v>0.3553317399203158</v>
       </c>
@@ -9480,7 +9483,7 @@
       <c r="O85" s="49"/>
       <c r="P85" s="49"/>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H86" s="65">
         <v>0.37078429028268828</v>
       </c>
@@ -9496,7 +9499,7 @@
       <c r="O86" s="49"/>
       <c r="P86" s="49"/>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H87" s="65">
         <v>0.38613044476352726</v>
       </c>
@@ -9512,7 +9515,7 @@
       <c r="O87" s="49"/>
       <c r="P87" s="49"/>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H88" s="65">
         <v>0.4009921758963842</v>
       </c>
@@ -9528,7 +9531,7 @@
       <c r="O88" s="49"/>
       <c r="P88" s="49"/>
     </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H89" s="65">
         <v>0.4156182923872962</v>
       </c>
@@ -9544,7 +9547,7 @@
       <c r="O89" s="49"/>
       <c r="P89" s="49"/>
     </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H90" s="65">
         <v>0.42943502667027428</v>
       </c>
@@ -9560,7 +9563,7 @@
       <c r="O90" s="49"/>
       <c r="P90" s="49"/>
     </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H91" s="65">
         <v>0.44289756776749095</v>
       </c>
@@ -9576,7 +9579,7 @@
       <c r="O91" s="49"/>
       <c r="P91" s="49"/>
     </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H92" s="65">
         <v>0.45543894715911687</v>
       </c>
@@ -9592,7 +9595,7 @@
       <c r="O92" s="49"/>
       <c r="P92" s="49"/>
     </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H93" s="65">
         <v>0.46783735943015631</v>
       </c>
@@ -9608,7 +9611,7 @@
       <c r="O93" s="49"/>
       <c r="P93" s="49"/>
     </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H94" s="65">
         <v>0.47863400366300879</v>
       </c>
@@ -9624,7 +9627,7 @@
       <c r="O94" s="49"/>
       <c r="P94" s="49"/>
     </row>
-    <row r="95" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H95" s="65">
         <v>0.48872859410433517</v>
       </c>
@@ -9640,7 +9643,7 @@
       <c r="O95" s="49"/>
       <c r="P95" s="49"/>
     </row>
-    <row r="96" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H96" s="65">
         <v>0.49808648675762501</v>
       </c>
@@ -9656,7 +9659,7 @@
       <c r="O96" s="49"/>
       <c r="P96" s="49"/>
     </row>
-    <row r="97" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H97" s="65">
         <v>0.50622094031681064</v>
       </c>
@@ -9672,7 +9675,7 @@
       <c r="O97" s="49"/>
       <c r="P97" s="49"/>
     </row>
-    <row r="98" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H98" s="65">
         <v>0.51358901063162188</v>
       </c>
@@ -9688,7 +9691,7 @@
       <c r="O98" s="49"/>
       <c r="P98" s="49"/>
     </row>
-    <row r="99" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H99" s="65">
         <v>0.51988812196851808</v>
       </c>
@@ -9704,7 +9707,7 @@
       <c r="O99" s="49"/>
       <c r="P99" s="49"/>
     </row>
-    <row r="100" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H100" s="65">
         <v>0.52654380991188665</v>
       </c>
@@ -9720,7 +9723,7 @@
       <c r="O100" s="49"/>
       <c r="P100" s="49"/>
     </row>
-    <row r="101" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H101" s="65">
         <v>0.53210746291493216</v>
       </c>
@@ -9736,7 +9739,7 @@
       <c r="O101" s="49"/>
       <c r="P101" s="49"/>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H102" s="65">
         <v>0.53593356457098895</v>
       </c>
@@ -9752,7 +9755,7 @@
       <c r="O102" s="49"/>
       <c r="P102" s="49"/>
     </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H103" s="65">
         <v>0.53837802652041589</v>
       </c>
@@ -9768,7 +9771,7 @@
       <c r="O103" s="49"/>
       <c r="P103" s="49"/>
     </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
       <c r="K104" s="49"/>
       <c r="L104" s="49"/>
       <c r="M104" s="49"/>

</xml_diff>

<commit_message>
Updated mass balance for entire flowsheet
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1007" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53F20CB6-804D-4540-BD16-A798BBE83D98}"/>
+  <xr:revisionPtr revIDLastSave="1046" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{714CD814-258F-414B-8938-B6435C8100D5}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -29,19 +29,19 @@
     <definedName name="crossover_acid">'Constants and assumptions'!#REF!</definedName>
     <definedName name="crossover_alkaline">'Constants and assumptions'!#REF!</definedName>
     <definedName name="crossover_neutral">'Constants and assumptions'!$C$8</definedName>
-    <definedName name="F">'Constants and assumptions'!$C$19</definedName>
-    <definedName name="K_to_C">'Constants and assumptions'!$C$40</definedName>
-    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$41</definedName>
-    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$42</definedName>
-    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$43</definedName>
+    <definedName name="F">'Constants and assumptions'!$C$20</definedName>
+    <definedName name="K_to_C">'Constants and assumptions'!$C$41</definedName>
+    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$42</definedName>
+    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$43</definedName>
+    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$44</definedName>
     <definedName name="mol_s_per_mA">'Kas Smith curvefit (copy)'!$B$12</definedName>
     <definedName name="mol_s_per_sccm">'Kas Smith curvefit (copy)'!$B$11</definedName>
     <definedName name="MW_CO">Products!$C$3</definedName>
-    <definedName name="P">'Constants and assumptions'!$C$27</definedName>
-    <definedName name="R_">'Constants and assumptions'!$C$20</definedName>
+    <definedName name="P">'Constants and assumptions'!$C$28</definedName>
+    <definedName name="R_">'Constants and assumptions'!$C$21</definedName>
     <definedName name="separation_efficiency">'Constants and assumptions'!$C$11</definedName>
-    <definedName name="T">'Constants and assumptions'!$C$39</definedName>
-    <definedName name="T_sep">'Constants and assumptions'!$C$38</definedName>
+    <definedName name="T">'Constants and assumptions'!$C$40</definedName>
+    <definedName name="T_sep">'Constants and assumptions'!$C$39</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="206">
   <si>
     <t>Utility</t>
   </si>
@@ -354,9 +354,6 @@
     <t>MW_O2</t>
   </si>
   <si>
-    <t>density_kgm3</t>
-  </si>
-  <si>
     <r>
       <t>kg/m</t>
     </r>
@@ -626,9 +623,6 @@
   </si>
   <si>
     <t>Crossover: neutral electrolyte</t>
-  </si>
-  <si>
-    <t>Density: salt solutions</t>
   </si>
   <si>
     <t>Faraday's constant</t>
@@ -1117,15 +1111,9 @@
     <t>Molar mass: solvent</t>
   </si>
   <si>
-    <t>MW_solvent</t>
-  </si>
-  <si>
     <t>Molar mass: supporting electrolyte</t>
   </si>
   <si>
-    <t>MW_supporting</t>
-  </si>
-  <si>
     <t>TBA perchlorate</t>
   </si>
   <si>
@@ -1139,6 +1127,24 @@
   </si>
   <si>
     <t>Jouny, Jiao I&amp;EC 2020; Guerra 2023 $0.74</t>
+  </si>
+  <si>
+    <t>MW_acetonitrile</t>
+  </si>
+  <si>
+    <t>MW_TBAClO4</t>
+  </si>
+  <si>
+    <t>Electrolyte assumption: Density</t>
+  </si>
+  <si>
+    <t>Density: aqueous solutions</t>
+  </si>
+  <si>
+    <t>electrolyte_density_kg_m3</t>
+  </si>
+  <si>
+    <t>water_density_kg_m3</t>
   </si>
 </sst>
 </file>
@@ -1488,7 +1494,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1719,6 +1725,9 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1731,7 +1740,10 @@
     <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4846,10 +4858,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E43" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:E43" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E43">
-    <sortCondition ref="A1:A43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E44" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:E44" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
+    <sortCondition ref="A1:A44"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD981D8-5D27-4DEC-AB19-B4CDEDE4E307}" name="Name" dataDxfId="38"/>
@@ -5793,21 +5805,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.88671875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -5825,121 +5837,121 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C2" s="74">
         <v>1</v>
       </c>
       <c r="D2" s="68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="72"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="9">
         <v>75</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="70" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="73">
         <f>0.0145</f>
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E4" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>138</v>
       </c>
       <c r="C5" s="35">
         <v>5000</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="70" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C6" s="73">
         <v>0.06</v>
       </c>
       <c r="D6" s="70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E6" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="B7" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C7" s="39">
         <f>340/0.05</f>
         <v>6800</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="70" t="s">
         <v>33</v>
@@ -5951,50 +5963,48 @@
         <v>17</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="70" t="s">
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="85" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="86">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="71">
-        <v>786</v>
-      </c>
-      <c r="D9" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="72" t="s">
-        <v>187</v>
-      </c>
+      <c r="E9" s="85"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="11">
         <v>0.9</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="11">
         <v>7.0000000000000007E-2</v>
@@ -6005,195 +6015,197 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="69">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" s="71">
+        <v>786</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="72" t="s">
+        <v>185</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="69">
         <f>0.75/100</f>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D13" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="70" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="F12" s="70" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="B13" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="C13" s="71">
+    </row>
+    <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="71">
         <v>6E-10</v>
       </c>
-      <c r="D13" s="68" t="s">
-        <v>178</v>
-      </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="70" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
-        <v>175</v>
-      </c>
-      <c r="B14" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="C14" s="69">
-        <v>0.89</v>
-      </c>
       <c r="D14" s="68" t="s">
-        <v>167</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>168</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="E14" s="72"/>
       <c r="F14" s="70" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B15" s="68" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C15" s="69">
         <v>0.89</v>
       </c>
       <c r="D15" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" s="70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="F15" s="70" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
-        <v>180</v>
-      </c>
-      <c r="B16" s="68" t="s">
-        <v>183</v>
-      </c>
-      <c r="C16" s="74">
+      <c r="C16" s="69">
+        <v>0.89</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="74">
         <f>0.8/10</f>
         <v>0.08</v>
       </c>
-      <c r="D16" s="68" t="s">
-        <v>181</v>
-      </c>
-      <c r="E16" s="72" t="s">
+      <c r="D17" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="72" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="B17" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="C17" s="69">
-        <v>0.22</v>
-      </c>
-      <c r="D17" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="72" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="68" t="s">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="69">
+      <c r="C19" s="69">
         <v>1.23</v>
       </c>
-      <c r="D18" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="72" t="s">
+      <c r="D19" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C20" s="8">
         <v>96485.33212331</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="5">
-        <v>8.3144720000000003</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="9">
-        <v>44.009500000000003</v>
+        <v>9</v>
+      </c>
+      <c r="C21" s="5">
+        <v>8.3144720000000003</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>75</v>
+    <row r="22" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C22" s="9">
-        <v>138.2055</v>
+        <v>44.009500000000003</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>29</v>
@@ -6201,15 +6213,15 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C23" s="9">
-        <v>31.998799999999999</v>
+        <v>138.2055</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>29</v>
@@ -6217,15 +6229,15 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
+        <v>96</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C24" s="9">
-        <v>18.015799999999999</v>
+        <v>31.998799999999999</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>29</v>
@@ -6233,379 +6245,394 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="70" t="s">
-        <v>196</v>
-      </c>
-      <c r="C25" s="75">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="9">
+        <v>18.015799999999999</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="70" t="s">
+        <v>200</v>
+      </c>
+      <c r="C26" s="75">
         <v>41.05</v>
-      </c>
-      <c r="D25" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="70" t="s">
-        <v>186</v>
-      </c>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="70" t="s">
-        <v>197</v>
-      </c>
-      <c r="B26" s="70" t="s">
-        <v>198</v>
-      </c>
-      <c r="C26" s="75">
-        <v>341.91</v>
       </c>
       <c r="D26" s="70" t="s">
         <v>29</v>
       </c>
       <c r="E26" s="70" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="70" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="70" t="s">
+        <v>201</v>
+      </c>
+      <c r="C27" s="75">
+        <v>341.91</v>
+      </c>
+      <c r="D27" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="70" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C28" s="8">
         <v>101325</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="11">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="11">
         <f>350/365</f>
         <v>0.95890410958904104</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="29">
-        <v>0</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="36">
-        <v>10</v>
-      </c>
-      <c r="D30" s="5" t="s">
         <v>116</v>
       </c>
+      <c r="C30" s="29">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="70" t="s">
+    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="36">
+        <v>10</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="80">
+        <v>2500</v>
+      </c>
+      <c r="D32" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="70" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="84">
+      <c r="E32" s="70"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="35">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="74">
         <v>2500</v>
       </c>
-      <c r="D31" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="35">
-        <v>1</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="74">
-        <v>2500</v>
-      </c>
-      <c r="D34" s="68" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="72"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="68" t="s">
+      <c r="D35" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="72"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="68">
+      <c r="C36" s="68">
         <v>10</v>
       </c>
-      <c r="D35" s="68" t="s">
+      <c r="D36" s="68" t="s">
         <v>21</v>
-      </c>
-      <c r="E35" s="72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="68">
-        <v>0.247</v>
-      </c>
-      <c r="D36" s="68" t="s">
-        <v>18</v>
       </c>
       <c r="E36" s="72" t="s">
         <v>20</v>
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A37" s="68" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B37" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="68">
+        <v>0.247</v>
+      </c>
+      <c r="D37" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="68">
+      <c r="C38" s="68">
         <f>0.041*1000</f>
         <v>41</v>
       </c>
-      <c r="D37" s="68" t="s">
-        <v>141</v>
-      </c>
-      <c r="E37" s="72" t="s">
+      <c r="D38" s="68" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="6" t="s">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C38" s="10">
-        <v>313.14999999999998</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="C39" s="10">
         <v>313.14999999999998</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="16">
-        <v>273.14999999999998</v>
-      </c>
-      <c r="D40" s="16" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="10">
+        <v>313.14999999999998</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>95</v>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="16">
+        <v>273.14999999999998</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C42" s="8">
         <f>3600</f>
         <v>3600</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" s="6" t="s">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C43" s="8">
         <f>1055870</f>
         <v>1055870</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="6" t="s">
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C44" s="8">
         <f>kJ_per_mmBtu/kJ_per_kWh</f>
         <v>293.29722222222222</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
-      <c r="B54" s="9"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E11" r:id="rId1" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
-    <hyperlink ref="E36" r:id="rId2" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
-    <hyperlink ref="E18" r:id="rId3" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
-    <hyperlink ref="E17" r:id="rId4" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
-    <hyperlink ref="E38" r:id="rId5" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
+    <hyperlink ref="E37" r:id="rId2" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
+    <hyperlink ref="E18" r:id="rId4" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
+    <hyperlink ref="E39" r:id="rId5" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
     <hyperlink ref="E3" r:id="rId6" display="IEA, average for power gen" xr:uid="{781250D3-74FF-4AAC-876D-B170419E0026}"/>
     <hyperlink ref="E4" r:id="rId7" display="Seider et al: $0.27/m3; Alerte et al: $0.0145/kg" xr:uid="{428FA07D-32E1-4E39-B95F-F3FC1495D338}"/>
     <hyperlink ref="E10" r:id="rId8" display="Brandl et al" xr:uid="{EF89FF7B-65AC-4D83-8890-C13EE030FEED}"/>
     <hyperlink ref="E5" r:id="rId9" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{13C42B5A-CBC8-4B1A-A9AB-3BCDE19ECC9C}"/>
-    <hyperlink ref="E15" r:id="rId10" xr:uid="{D0441B06-C472-48BE-94F3-D46ED457AEEA}"/>
-    <hyperlink ref="E14" r:id="rId11" xr:uid="{8B2FE28B-B8A6-4658-BE2B-A2D2A2E7068A}"/>
-    <hyperlink ref="E12" r:id="rId12" xr:uid="{3CE65C60-DA75-4595-8CAA-88F2C9A358C9}"/>
-    <hyperlink ref="E16" r:id="rId13" xr:uid="{B2106B39-835F-40BC-BDFE-DE3B87B90F64}"/>
-    <hyperlink ref="E9" r:id="rId14" xr:uid="{2792E3FF-B7C4-4474-9807-0DE4735F4ACD}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{D0441B06-C472-48BE-94F3-D46ED457AEEA}"/>
+    <hyperlink ref="E15" r:id="rId11" xr:uid="{8B2FE28B-B8A6-4658-BE2B-A2D2A2E7068A}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{3CE65C60-DA75-4595-8CAA-88F2C9A358C9}"/>
+    <hyperlink ref="E17" r:id="rId13" xr:uid="{B2106B39-835F-40BC-BDFE-DE3B87B90F64}"/>
+    <hyperlink ref="E12" r:id="rId14" xr:uid="{2792E3FF-B7C4-4474-9807-0DE4735F4ACD}"/>
     <hyperlink ref="E6" r:id="rId15" xr:uid="{5655458C-49A7-4C0B-8608-74FBB0552E76}"/>
     <hyperlink ref="E7" r:id="rId16" display="Sigma-Aldrich; acetonitrile" xr:uid="{57133E53-0E09-45A4-B177-CDDD279FC5F5}"/>
   </hyperlinks>
@@ -6626,85 +6653,85 @@
       <selection pane="topRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="42" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="20.88671875" style="43" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="4"/>
+    <col min="4" max="4" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="42" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" style="43" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="58.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="M1" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="9">
         <f>1.007947*2</f>
@@ -6737,12 +6764,12 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="9">
         <v>28.010100000000001</v>
@@ -6788,15 +6815,15 @@
         <v>20</v>
       </c>
       <c r="Q3" s="40" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C4" s="9">
         <v>46.024999999999999</v>
@@ -6839,45 +6866,45 @@
         <v>20</v>
       </c>
       <c r="Q4" s="78" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="41" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="41" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
@@ -6912,18 +6939,18 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -6937,13 +6964,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="32"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -6954,18 +6981,18 @@
         <v>50</v>
       </c>
       <c r="D3" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="81" t="s">
-        <v>151</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="F3" s="81" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="32">
         <v>2.4E-2</v>
@@ -6974,24 +7001,24 @@
         <v>20</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="80"/>
-    </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="E4" s="82"/>
+      <c r="F4" s="81"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="32">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="30" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -7004,10 +7031,10 @@
         <v>230.93061430996579</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -7020,10 +7047,10 @@
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
@@ -7036,10 +7063,10 @@
         <v>254.376</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>45</v>
       </c>
@@ -7051,13 +7078,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="32"/>
       <c r="C10" s="45"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -7071,7 +7098,7 @@
       </c>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
@@ -7085,22 +7112,22 @@
       </c>
       <c r="D12" s="37"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="33"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="32">
         <v>200</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -7133,55 +7160,55 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="49" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="49" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="49"/>
-    <col min="8" max="8" width="14.6640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="14.6640625" style="50" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="49"/>
+    <col min="8" max="8" width="14.7109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.7109375" style="50" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="50" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="13.6640625" style="49"/>
-    <col min="26" max="26" width="18.44140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="13.6640625" style="49"/>
+    <col min="17" max="25" width="13.7109375" style="49"/>
+    <col min="26" max="26" width="18.42578125" style="49" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="13.7109375" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="50" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="50" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="48"/>
       <c r="D2" s="48"/>
       <c r="E2" s="66" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F2" s="49"/>
     </row>
-    <row r="3" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="F3" s="49"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
         <v>6</v>
       </c>
@@ -7192,10 +7219,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
         <v>9</v>
       </c>
@@ -7207,7 +7234,7 @@
       </c>
       <c r="D5" s="53"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
         <v>11</v>
       </c>
@@ -7219,7 +7246,7 @@
       </c>
       <c r="D6" s="54"/>
     </row>
-    <row r="7" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="53" t="s">
         <v>13</v>
       </c>
@@ -7233,7 +7260,7 @@
       <c r="E7" s="49"/>
       <c r="F7" s="49"/>
     </row>
-    <row r="8" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
         <v>15</v>
       </c>
@@ -7247,9 +7274,9 @@
       <c r="E8" s="49"/>
       <c r="F8" s="49"/>
     </row>
-    <row r="9" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B9" s="53">
         <v>273.14999999999998</v>
@@ -7262,55 +7289,55 @@
       <c r="F9" s="49"/>
       <c r="L9" s="49"/>
     </row>
-    <row r="10" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="50" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B10" s="54">
         <f>1/60/(100^3)*P/(R_*B7+20)</f>
         <v>7.3709198831561756E-7</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="54"/>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
       <c r="L10" s="49"/>
     </row>
-    <row r="11" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="53" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11" s="53">
         <f>1/60/(100^3)*P/(R_*B7)</f>
         <v>7.4358305104930494E-7</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" s="53"/>
       <c r="E11" s="49"/>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
     </row>
-    <row r="12" spans="1:12" s="50" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="54">
         <f>1/(1000*2*F)</f>
         <v>5.182134828131088E-9</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D12" s="54"/>
       <c r="E12" s="49"/>
       <c r="F12" s="49"/>
       <c r="G12" s="49"/>
     </row>
-    <row r="13" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
@@ -7318,109 +7345,109 @@
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="50"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="83" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="H17" s="83" t="s">
-        <v>131</v>
-      </c>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
-      <c r="N17" s="83"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="83"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="82" t="s">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="H17" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="84"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="84"/>
+      <c r="P17" s="84"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="83"/>
+      <c r="C18" s="83" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" s="82"/>
+      <c r="F18" s="83"/>
       <c r="G18" s="56"/>
-      <c r="H18" s="82" t="s">
+      <c r="H18" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="83"/>
+      <c r="J18" s="83"/>
+      <c r="K18" s="83" t="s">
+        <v>120</v>
+      </c>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82" t="s">
-        <v>122</v>
-      </c>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="O18" s="82"/>
-      <c r="P18" s="82"/>
-    </row>
-    <row r="19" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="O18" s="83"/>
+      <c r="P18" s="83"/>
+    </row>
+    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F19" s="55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G19" s="56"/>
       <c r="H19" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="I19" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="J19" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="I19" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="J19" s="58" t="s">
-        <v>160</v>
-      </c>
       <c r="K19" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="M19" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="L19" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="M19" s="58" t="s">
-        <v>160</v>
-      </c>
       <c r="N19" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="O19" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="P19" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="O19" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="P19" s="58" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="59">
         <v>-51.5244564886654</v>
       </c>
@@ -7476,7 +7503,7 @@
         <v>5.0730403065140095E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="59">
         <v>-89.797974315320403</v>
       </c>
@@ -7532,7 +7559,7 @@
         <v>6.5460850237780699E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="59">
         <v>-128.06720097650799</v>
       </c>
@@ -7588,7 +7615,7 @@
         <v>8.6704673566159185E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="59">
         <v>-166.34194485043901</v>
       </c>
@@ -7644,7 +7671,7 @@
         <v>1.1771856112818058E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="59">
         <v>-204.613623606179</v>
       </c>
@@ -7700,7 +7727,7 @@
         <v>1.6610145177220037E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="59">
         <v>-242.881624220091</v>
       </c>
@@ -7756,7 +7783,7 @@
         <v>2.2533996934247069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="59">
         <v>-281.15268995219299</v>
       </c>
@@ -7812,7 +7839,7 @@
         <v>3.149742423062496E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="59">
         <v>-319.427433826124</v>
       </c>
@@ -7868,7 +7895,7 @@
         <v>4.8494015452431039E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="59">
         <v>-357.69420839275898</v>
       </c>
@@ -7924,7 +7951,7 @@
         <v>7.7219536858392002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="59">
         <v>-395.96343505394702</v>
       </c>
@@ -7980,7 +8007,7 @@
         <v>0.10626191485734104</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="59">
         <v>-434.23572683332497</v>
       </c>
@@ -8036,7 +8063,7 @@
         <v>-1.8498964897695203E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="59">
         <v>-472.50188837632197</v>
       </c>
@@ -8092,7 +8119,7 @@
         <v>-1.3483050770102256E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="59">
         <v>-510.774180155701</v>
       </c>
@@ -8135,7 +8162,7 @@
       <c r="O32" s="61"/>
       <c r="P32" s="61"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="59">
         <v>-549.04095472233598</v>
       </c>
@@ -8178,7 +8205,7 @@
       <c r="O33" s="61"/>
       <c r="P33" s="61"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="59">
         <v>-587.30895533624698</v>
       </c>
@@ -8221,7 +8248,7 @@
       <c r="O34" s="61"/>
       <c r="P34" s="61"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="59">
         <v>-625.57511687924398</v>
       </c>
@@ -8264,7 +8291,7 @@
       <c r="O35" s="61"/>
       <c r="P35" s="61"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="59">
         <v>-663.84066539860203</v>
       </c>
@@ -8307,7 +8334,7 @@
       <c r="O36" s="61"/>
       <c r="P36" s="61"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="59">
         <v>-702.104987870684</v>
       </c>
@@ -8350,7 +8377,7 @@
       <c r="O37" s="61"/>
       <c r="P37" s="61"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="59">
         <v>-740.36747127185197</v>
       </c>
@@ -8393,7 +8420,7 @@
       <c r="O38" s="61"/>
       <c r="P38" s="61"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="59">
         <v>-778.62934164938099</v>
       </c>
@@ -8436,7 +8463,7 @@
       <c r="O39" s="61"/>
       <c r="P39" s="61"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="59">
         <v>-816.88814690872005</v>
       </c>
@@ -8479,7 +8506,7 @@
       <c r="O40" s="61"/>
       <c r="P40" s="61"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="59">
         <v>-855.14633914442004</v>
       </c>
@@ -8522,7 +8549,7 @@
       <c r="O41" s="61"/>
       <c r="P41" s="61"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="59">
         <v>-893.40453138012003</v>
       </c>
@@ -8565,7 +8592,7 @@
       <c r="O42" s="61"/>
       <c r="P42" s="61"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="59">
         <v>-931.65781942671504</v>
       </c>
@@ -8608,7 +8635,7 @@
       <c r="O43" s="61"/>
       <c r="P43" s="61"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="59">
         <v>-969.90988142603396</v>
       </c>
@@ -8651,7 +8678,7 @@
       <c r="O44" s="61"/>
       <c r="P44" s="61"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="59">
         <v>-1008.15397411805</v>
       </c>
@@ -8694,7 +8721,7 @@
       <c r="O45" s="61"/>
       <c r="P45" s="61"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="59">
         <v>-1046.3962277391599</v>
       </c>
@@ -8737,7 +8764,7 @@
       <c r="O46" s="61"/>
       <c r="P46" s="61"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="59">
         <v>-1084.6305120529701</v>
       </c>
@@ -8780,7 +8807,7 @@
       <c r="O47" s="61"/>
       <c r="P47" s="61"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="59">
         <v>-1122.8660224140599</v>
       </c>
@@ -8810,7 +8837,7 @@
       <c r="O48" s="61"/>
       <c r="P48" s="61"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="59">
         <v>-1161.08743323147</v>
       </c>
@@ -8840,7 +8867,7 @@
       <c r="O49" s="61"/>
       <c r="P49" s="61"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="59">
         <v>-1199.30516590705</v>
       </c>
@@ -8870,7 +8897,7 @@
       <c r="O50" s="61"/>
       <c r="P50" s="61"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="59">
         <v>-1237.5192204407999</v>
       </c>
@@ -8900,7 +8927,7 @@
       <c r="O51" s="61"/>
       <c r="P51" s="61"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="59">
         <v>-1275.72530566725</v>
       </c>
@@ -8930,7 +8957,7 @@
       <c r="O52" s="61"/>
       <c r="P52" s="61"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="59">
         <v>-1313.9283257755101</v>
       </c>
@@ -8960,7 +8987,7 @@
       <c r="O53" s="61"/>
       <c r="P53" s="61"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="59">
         <v>-1352.1258286710299</v>
       </c>
@@ -8990,7 +9017,7 @@
       <c r="O54" s="61"/>
       <c r="P54" s="61"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="59">
         <v>-1390.3306878502101</v>
       </c>
@@ -9020,7 +9047,7 @@
       <c r="O55" s="61"/>
       <c r="P55" s="61"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="59">
         <v>-1428.5300298166501</v>
       </c>
@@ -9050,7 +9077,7 @@
       <c r="O56" s="61"/>
       <c r="P56" s="61"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="59">
         <v>-1466.7189503812299</v>
       </c>
@@ -9080,7 +9107,7 @@
       <c r="O57" s="61"/>
       <c r="P57" s="61"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="59">
         <v>-1499.6968635093899</v>
       </c>
@@ -9110,7 +9137,7 @@
       <c r="O58" s="61"/>
       <c r="P58" s="61"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J62" s="63"/>
       <c r="K62" s="49"/>
       <c r="L62" s="49"/>
@@ -9119,11 +9146,11 @@
       <c r="O62" s="49"/>
       <c r="P62" s="49"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H63" s="82" t="s">
-        <v>124</v>
-      </c>
-      <c r="I63" s="82"/>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H63" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="I63" s="83"/>
       <c r="J63" s="63"/>
       <c r="K63" s="49"/>
       <c r="L63" s="49"/>
@@ -9132,12 +9159,12 @@
       <c r="O63" s="49"/>
       <c r="P63" s="49"/>
     </row>
-    <row r="64" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="H64" s="64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I64" s="64" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J64" s="49"/>
       <c r="K64" s="49"/>
@@ -9147,7 +9174,7 @@
       <c r="O64" s="49"/>
       <c r="P64" s="49"/>
     </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H65" s="65">
         <v>2.2997934048565084E-2</v>
       </c>
@@ -9163,7 +9190,7 @@
       <c r="O65" s="49"/>
       <c r="P65" s="49"/>
     </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H66" s="65">
         <v>4.0069676396611777E-2</v>
       </c>
@@ -9179,7 +9206,7 @@
       <c r="O66" s="49"/>
       <c r="P66" s="49"/>
     </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H67" s="65">
         <v>5.7084370034302737E-2</v>
       </c>
@@ -9195,7 +9222,7 @@
       <c r="O67" s="49"/>
       <c r="P67" s="49"/>
     </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H68" s="65">
         <v>7.4140086301005395E-2</v>
       </c>
@@ -9211,7 +9238,7 @@
       <c r="O68" s="49"/>
       <c r="P68" s="49"/>
     </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H69" s="65">
         <v>9.1140638350711872E-2</v>
       </c>
@@ -9227,7 +9254,7 @@
       <c r="O69" s="49"/>
       <c r="P69" s="49"/>
     </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H70" s="65">
         <v>0.1080445517892699</v>
       </c>
@@ -9243,7 +9270,7 @@
       <c r="O70" s="49"/>
       <c r="P70" s="49"/>
     </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H71" s="65">
         <v>0.12497606826753388</v>
       </c>
@@ -9259,7 +9286,7 @@
       <c r="O71" s="49"/>
       <c r="P71" s="49"/>
     </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H72" s="65">
         <v>0.14198052165390951</v>
       </c>
@@ -9275,7 +9302,7 @@
       <c r="O72" s="49"/>
       <c r="P72" s="49"/>
     </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H73" s="65">
         <v>0.15874470475517963</v>
       </c>
@@ -9291,7 +9318,7 @@
       <c r="O73" s="49"/>
       <c r="P73" s="49"/>
     </row>
-    <row r="74" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H74" s="65">
         <v>0.17553747925232432</v>
       </c>
@@ -9307,7 +9334,7 @@
       <c r="O74" s="49"/>
       <c r="P74" s="49"/>
     </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H75" s="65">
         <v>0.19240417629290971</v>
       </c>
@@ -9323,7 +9350,7 @@
       <c r="O75" s="49"/>
       <c r="P75" s="49"/>
     </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H76" s="65">
         <v>0.20901220546271423</v>
       </c>
@@ -9339,7 +9366,7 @@
       <c r="O76" s="49"/>
       <c r="P76" s="49"/>
     </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H77" s="65">
         <v>0.22582431925537669</v>
       </c>
@@ -9355,7 +9382,7 @@
       <c r="O77" s="49"/>
       <c r="P77" s="49"/>
     </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H78" s="65">
         <v>0.24236713011424937</v>
       </c>
@@ -9371,7 +9398,7 @@
       <c r="O78" s="49"/>
       <c r="P78" s="49"/>
     </row>
-    <row r="79" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H79" s="65">
         <v>0.25891734586657894</v>
       </c>
@@ -9387,7 +9414,7 @@
       <c r="O79" s="49"/>
       <c r="P79" s="49"/>
     </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H80" s="65">
         <v>0.27532743679881172</v>
       </c>
@@ -9403,7 +9430,7 @@
       <c r="O80" s="49"/>
       <c r="P80" s="49"/>
     </row>
-    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H81" s="65">
         <v>0.29164753874763422</v>
       </c>
@@ -9419,7 +9446,7 @@
       <c r="O81" s="49"/>
       <c r="P81" s="49"/>
     </row>
-    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H82" s="65">
         <v>0.30783618288424536</v>
       </c>
@@ -9435,7 +9462,7 @@
       <c r="O82" s="49"/>
       <c r="P82" s="49"/>
     </row>
-    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H83" s="65">
         <v>0.32384418347196781</v>
       </c>
@@ -9451,7 +9478,7 @@
       <c r="O83" s="49"/>
       <c r="P83" s="49"/>
     </row>
-    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H84" s="65">
         <v>0.33973325501759533</v>
       </c>
@@ -9467,7 +9494,7 @@
       <c r="O84" s="49"/>
       <c r="P84" s="49"/>
     </row>
-    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H85" s="65">
         <v>0.3553317399203158</v>
       </c>
@@ -9483,7 +9510,7 @@
       <c r="O85" s="49"/>
       <c r="P85" s="49"/>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H86" s="65">
         <v>0.37078429028268828</v>
       </c>
@@ -9499,7 +9526,7 @@
       <c r="O86" s="49"/>
       <c r="P86" s="49"/>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H87" s="65">
         <v>0.38613044476352726</v>
       </c>
@@ -9515,7 +9542,7 @@
       <c r="O87" s="49"/>
       <c r="P87" s="49"/>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H88" s="65">
         <v>0.4009921758963842</v>
       </c>
@@ -9531,7 +9558,7 @@
       <c r="O88" s="49"/>
       <c r="P88" s="49"/>
     </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H89" s="65">
         <v>0.4156182923872962</v>
       </c>
@@ -9547,7 +9574,7 @@
       <c r="O89" s="49"/>
       <c r="P89" s="49"/>
     </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H90" s="65">
         <v>0.42943502667027428</v>
       </c>
@@ -9563,7 +9590,7 @@
       <c r="O90" s="49"/>
       <c r="P90" s="49"/>
     </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H91" s="65">
         <v>0.44289756776749095</v>
       </c>
@@ -9579,7 +9606,7 @@
       <c r="O91" s="49"/>
       <c r="P91" s="49"/>
     </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H92" s="65">
         <v>0.45543894715911687</v>
       </c>
@@ -9595,7 +9622,7 @@
       <c r="O92" s="49"/>
       <c r="P92" s="49"/>
     </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H93" s="65">
         <v>0.46783735943015631</v>
       </c>
@@ -9611,7 +9638,7 @@
       <c r="O93" s="49"/>
       <c r="P93" s="49"/>
     </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H94" s="65">
         <v>0.47863400366300879</v>
       </c>
@@ -9627,7 +9654,7 @@
       <c r="O94" s="49"/>
       <c r="P94" s="49"/>
     </row>
-    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H95" s="65">
         <v>0.48872859410433517</v>
       </c>
@@ -9643,7 +9670,7 @@
       <c r="O95" s="49"/>
       <c r="P95" s="49"/>
     </row>
-    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H96" s="65">
         <v>0.49808648675762501</v>
       </c>
@@ -9659,7 +9686,7 @@
       <c r="O96" s="49"/>
       <c r="P96" s="49"/>
     </row>
-    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H97" s="65">
         <v>0.50622094031681064</v>
       </c>
@@ -9675,7 +9702,7 @@
       <c r="O97" s="49"/>
       <c r="P97" s="49"/>
     </row>
-    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H98" s="65">
         <v>0.51358901063162188</v>
       </c>
@@ -9691,7 +9718,7 @@
       <c r="O98" s="49"/>
       <c r="P98" s="49"/>
     </row>
-    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H99" s="65">
         <v>0.51988812196851808</v>
       </c>
@@ -9707,7 +9734,7 @@
       <c r="O99" s="49"/>
       <c r="P99" s="49"/>
     </row>
-    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H100" s="65">
         <v>0.52654380991188665</v>
       </c>
@@ -9723,7 +9750,7 @@
       <c r="O100" s="49"/>
       <c r="P100" s="49"/>
     </row>
-    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H101" s="65">
         <v>0.53210746291493216</v>
       </c>
@@ -9739,7 +9766,7 @@
       <c r="O101" s="49"/>
       <c r="P101" s="49"/>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H102" s="65">
         <v>0.53593356457098895</v>
       </c>
@@ -9755,7 +9782,7 @@
       <c r="O102" s="49"/>
       <c r="P102" s="49"/>
     </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H103" s="65">
         <v>0.53837802652041589</v>
       </c>
@@ -9771,7 +9798,7 @@
       <c r="O103" s="49"/>
       <c r="P103" s="49"/>
     </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.2">
       <c r="K104" s="49"/>
       <c r="L104" s="49"/>
       <c r="M104" s="49"/>

</xml_diff>

<commit_message>
Updated file names and calls to single_run_nonaq
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1229" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2BF5957-06A7-4CEE-A973-C07D4CC75FB7}"/>
+  <xr:revisionPtr revIDLastSave="1236" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC3D5572-464F-47C8-9C7F-7AFCCCA70AF3}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -31,19 +31,19 @@
     <definedName name="crossover_acid">'Constants and assumptions'!#REF!</definedName>
     <definedName name="crossover_alkaline">'Constants and assumptions'!#REF!</definedName>
     <definedName name="crossover_neutral">'Constants and assumptions'!$C$7</definedName>
-    <definedName name="F">'Constants and assumptions'!$C$14</definedName>
-    <definedName name="K_to_C">'Constants and assumptions'!$C$33</definedName>
-    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$34</definedName>
-    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$35</definedName>
-    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$36</definedName>
+    <definedName name="F">'Constants and assumptions'!$C$15</definedName>
+    <definedName name="K_to_C">'Constants and assumptions'!$C$34</definedName>
+    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$35</definedName>
+    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$36</definedName>
+    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$37</definedName>
     <definedName name="mol_s_per_mA">'Kas Smith curvefit (copy)'!$B$12</definedName>
     <definedName name="mol_s_per_sccm">'Kas Smith curvefit (copy)'!$B$11</definedName>
     <definedName name="MW_CO">Products!$C$3</definedName>
-    <definedName name="P">'Constants and assumptions'!$C$20</definedName>
-    <definedName name="R_">'Constants and assumptions'!$C$15</definedName>
-    <definedName name="separation_efficiency">'Constants and assumptions'!$C$10</definedName>
-    <definedName name="T">'Constants and assumptions'!$C$32</definedName>
-    <definedName name="T_sep">'Constants and assumptions'!$C$31</definedName>
+    <definedName name="P">'Constants and assumptions'!$C$21</definedName>
+    <definedName name="R_">'Constants and assumptions'!$C$16</definedName>
+    <definedName name="separation_efficiency">'Constants and assumptions'!$C$11</definedName>
+    <definedName name="T">'Constants and assumptions'!$C$33</definedName>
+    <definedName name="T_sep">'Constants and assumptions'!$C$32</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="204">
   <si>
     <t>Utility</t>
   </si>
@@ -1138,6 +1138,9 @@
   </si>
   <si>
     <t>Business Analytiq (accessed 2024)</t>
+  </si>
+  <si>
+    <t>LL_second_law_efficiency</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1499,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1753,6 +1756,9 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5184,10 +5190,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E36" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <autoFilter ref="A1:E36" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
-    <sortCondition ref="A1:A36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E37" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A1:E37" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
+    <sortCondition ref="A1:A37"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD981D8-5D27-4DEC-AB19-B4CDEDE4E307}" name="Name" dataDxfId="53"/>
@@ -6165,10 +6171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6343,125 +6349,123 @@
         <v>100</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="89">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C11" s="11">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="24" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C12" s="29">
         <f>0.8/10</f>
         <v>0.08</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E12" s="24" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0.22</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C14" s="10">
         <v>1.23</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E14" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C15" s="8">
         <v>96485.33212331</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="5">
-        <v>8.3144720000000003</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="9">
-        <v>44.009500000000003</v>
+        <v>9</v>
+      </c>
+      <c r="C16" s="5">
+        <v>8.3144720000000003</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>74</v>
+      <c r="A17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C17" s="9">
-        <v>138.2055</v>
+        <v>44.009500000000003</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>29</v>
@@ -6470,14 +6474,14 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>96</v>
+      <c r="A18" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C18" s="9">
-        <v>31.998799999999999</v>
+        <v>138.2055</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>29</v>
@@ -6485,15 +6489,15 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>44</v>
+        <v>96</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="9">
-        <v>18.015799999999999</v>
+        <v>31.998799999999999</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>29</v>
@@ -6503,44 +6507,46 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="8">
-        <v>101325</v>
+        <v>44</v>
+      </c>
+      <c r="C20" s="9">
+        <v>18.015799999999999</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="8">
+        <v>101325</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C22" s="11">
         <f>350/365</f>
         <v>0.95890410958904104</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="29">
-        <v>0</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -6548,112 +6554,108 @@
     </row>
     <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="36">
-        <v>10</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>114</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C23" s="29">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="36">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="B25" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="76">
+      <c r="C25" s="76">
         <v>2500</v>
       </c>
-      <c r="D24" s="69" t="s">
+      <c r="D25" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="69"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="E25" s="69"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C26" s="35">
         <v>1</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C27" s="11">
         <v>0.05</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="29">
-        <v>2500</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="D27" s="6"/>
       <c r="E27" s="24"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="6">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="C28" s="29">
+        <v>2500</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>20</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E28" s="24"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C29" s="6">
-        <v>0.247</v>
+        <v>10</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>20</v>
@@ -6662,126 +6664,140 @@
     </row>
     <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.247</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C31" s="6">
         <f>0.041*1000</f>
         <v>41</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E31" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C31" s="10">
-        <v>313.14999999999998</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="C32" s="10">
         <v>313.14999999999998</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="16">
-        <v>273.14999999999998</v>
-      </c>
-      <c r="D33" s="16" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="10">
+        <v>313.14999999999998</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="16">
+        <v>273.14999999999998</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C35" s="8">
         <f>3600</f>
         <v>3600</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C36" s="8">
         <f>1055870</f>
         <v>1055870</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C37" s="8">
         <f>kJ_per_mmBtu/kJ_per_kWh</f>
         <v>293.29722222222222</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -6810,33 +6826,36 @@
       <c r="A45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="A46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
-      <c r="B47" s="9"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{B2106B39-835F-40BC-BDFE-DE3B87B90F64}"/>
+    <hyperlink ref="E12" r:id="rId1" xr:uid="{B2106B39-835F-40BC-BDFE-DE3B87B90F64}"/>
     <hyperlink ref="E6" r:id="rId2" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{13C42B5A-CBC8-4B1A-A9AB-3BCDE19ECC9C}"/>
     <hyperlink ref="E9" r:id="rId3" display="Brandl et al" xr:uid="{EF89FF7B-65AC-4D83-8890-C13EE030FEED}"/>
     <hyperlink ref="E5" r:id="rId4" display="Seider et al: $0.27/m3; Alerte et al: $0.0145/kg" xr:uid="{428FA07D-32E1-4E39-B95F-F3FC1495D338}"/>
     <hyperlink ref="E4" r:id="rId5" display="IEA, average for power gen" xr:uid="{781250D3-74FF-4AAC-876D-B170419E0026}"/>
-    <hyperlink ref="E31" r:id="rId6" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
-    <hyperlink ref="E12" r:id="rId7" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
-    <hyperlink ref="E13" r:id="rId8" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
-    <hyperlink ref="E29" r:id="rId9" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
-    <hyperlink ref="E10" r:id="rId10" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
+    <hyperlink ref="E32" r:id="rId6" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
+    <hyperlink ref="E13" r:id="rId7" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
+    <hyperlink ref="E30" r:id="rId9" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -7332,7 +7351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8976AAB6-E21A-42F8-BEF8-70CDE446E133}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -7349,7 +7368,7 @@
     <col min="9" max="9" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="s">
         <v>187</v>
       </c>

</xml_diff>

<commit_message>
Fixed comparison plots to be generalized on tick titles
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1236" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC3D5572-464F-47C8-9C7F-7AFCCCA70AF3}"/>
+  <xr:revisionPtr revIDLastSave="1257" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05748941-0862-450C-900A-F9F8B1A9125C}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -1153,7 +1153,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1315,13 +1315,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial Nova"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1712,9 +1705,6 @@
     <xf numFmtId="1" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1745,6 +1735,12 @@
     <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="23" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1756,9 +1752,6 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="23" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6173,8 +6166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6262,7 +6255,7 @@
       <c r="B5" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="77">
+      <c r="C5" s="76">
         <f>0.0145</f>
         <v>1.4500000000000001E-2</v>
       </c>
@@ -6351,7 +6344,7 @@
       <c r="B10" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="89">
+      <c r="C10" s="84">
         <v>0.3</v>
       </c>
       <c r="D10" s="6"/>
@@ -6589,7 +6582,7 @@
       <c r="B25" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="76">
+      <c r="C25" s="75">
         <v>2500</v>
       </c>
       <c r="D25" s="69" t="s">
@@ -6869,9 +6862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7023,14 +7016,14 @@
       <c r="L3" s="66">
         <v>10</v>
       </c>
-      <c r="M3" s="75">
+      <c r="M3" s="74">
         <v>0.8</v>
       </c>
       <c r="N3" s="72">
         <v>0.7</v>
       </c>
-      <c r="O3" s="73">
-        <v>150</v>
+      <c r="O3" s="85">
+        <v>853.8</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>20</v>
@@ -7039,7 +7032,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>176</v>
       </c>
@@ -7074,7 +7067,7 @@
       <c r="L4" s="66">
         <v>10</v>
       </c>
-      <c r="M4" s="75">
+      <c r="M4" s="74">
         <v>0.9</v>
       </c>
       <c r="N4" s="72">
@@ -7083,10 +7076,10 @@
       <c r="O4" s="73">
         <v>100</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="Q4" s="39" t="s">
         <v>178</v>
       </c>
     </row>
@@ -7110,29 +7103,29 @@
       <c r="G5" s="9">
         <v>0.7</v>
       </c>
-      <c r="H5" s="78">
+      <c r="H5" s="77">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="I5" s="78">
+      <c r="I5" s="77">
         <v>-0.12</v>
       </c>
-      <c r="J5" s="75">
+      <c r="J5" s="74">
         <v>-0.71199999999999997</v>
       </c>
-      <c r="K5" s="75">
+      <c r="K5" s="74">
         <v>-416</v>
       </c>
-      <c r="L5" s="75">
+      <c r="L5" s="74">
         <v>10</v>
       </c>
-      <c r="M5" s="75">
+      <c r="M5" s="74">
         <v>0.9</v>
       </c>
       <c r="N5" s="72">
         <v>0.7</v>
       </c>
-      <c r="O5" s="73">
-        <v>100</v>
+      <c r="O5" s="85">
+        <v>850.2</v>
       </c>
       <c r="P5" s="24" t="s">
         <v>202</v>
@@ -7225,7 +7218,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="82" t="s">
         <v>185</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -7251,13 +7244,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>171</v>
       </c>
       <c r="B2" s="9">
         <v>41.05</v>
       </c>
-      <c r="C2" s="77">
+      <c r="C2" s="76">
         <v>0.06</v>
       </c>
       <c r="D2" s="8">
@@ -7277,55 +7270,55 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="79" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="77">
         <v>102.09</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="77">
         <v>10</v>
       </c>
-      <c r="D3" s="75">
+      <c r="D3" s="74">
         <v>1200</v>
       </c>
-      <c r="E3" s="75">
+      <c r="E3" s="74">
         <v>2.5</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="74" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="80" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="77">
         <v>78.13</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="77">
         <v>50</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="74">
         <v>1095</v>
       </c>
-      <c r="E4" s="75">
+      <c r="E4" s="74">
         <v>1.99</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="74" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="26"/>
@@ -7369,7 +7362,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="82" t="s">
         <v>187</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -7395,13 +7388,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>175</v>
       </c>
       <c r="B2" s="9">
         <v>341.91</v>
       </c>
-      <c r="C2" s="76">
+      <c r="C2" s="75">
         <f>340/0.05</f>
         <v>6800</v>
       </c>
@@ -7426,53 +7419,53 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="79" t="s">
         <v>197</v>
       </c>
       <c r="B3" s="9">
         <v>329.27</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="77">
         <f>548/0.025</f>
         <v>21920</v>
       </c>
-      <c r="D3" s="75">
+      <c r="D3" s="74">
         <v>0.01</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="75"/>
+      <c r="F3" s="74"/>
       <c r="G3" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="H3" s="75"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="66"/>
     </row>
     <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="79" t="s">
         <v>198</v>
       </c>
       <c r="B4" s="9">
         <v>217.06</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="77">
         <f>116/0.025</f>
         <v>4640</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="74">
         <v>0.01</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="75"/>
+      <c r="F4" s="74"/>
       <c r="G4" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="H4" s="75"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="66"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="66"/>
       <c r="E5" s="26"/>
       <c r="F5" s="66"/>
@@ -7547,10 +7540,10 @@
       <c r="D3" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="87" t="s">
         <v>148</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="86" t="s">
         <v>149</v>
       </c>
     </row>
@@ -7567,8 +7560,8 @@
       <c r="D4" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="86"/>
-      <c r="F4" s="85"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="86"/>
     </row>
     <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -7913,55 +7906,55 @@
       <c r="B14" s="49"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="88"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="H17" s="88" t="s">
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="H17" s="89" t="s">
         <v>129</v>
       </c>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="88"/>
-      <c r="N17" s="88"/>
-      <c r="O17" s="88"/>
-      <c r="P17" s="88"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
+      <c r="P17" s="89"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87" t="s">
+      <c r="B18" s="88"/>
+      <c r="C18" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87" t="s">
+      <c r="D18" s="88"/>
+      <c r="E18" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="87"/>
+      <c r="F18" s="88"/>
       <c r="G18" s="55"/>
-      <c r="H18" s="87" t="s">
+      <c r="H18" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87" t="s">
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87" t="s">
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="O18" s="87"/>
-      <c r="P18" s="87"/>
+      <c r="O18" s="88"/>
+      <c r="P18" s="88"/>
     </row>
     <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="54" t="s">
@@ -9711,10 +9704,10 @@
       <c r="P62" s="48"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H63" s="87" t="s">
+      <c r="H63" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="I63" s="87"/>
+      <c r="I63" s="88"/>
       <c r="J63" s="62"/>
       <c r="K63" s="48"/>
       <c r="L63" s="48"/>

</xml_diff>

<commit_message>
Updated separations capital costs
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1321" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C993D0A-A534-4482-BF5E-EE1EFEA4AE0B}"/>
+  <xr:revisionPtr revIDLastSave="1357" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCAC03C0-C783-4A55-B552-A13AAB437AAE}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -30,20 +30,20 @@
     <definedName name="cost_heat">Utilities!$B$12</definedName>
     <definedName name="crossover_acid">'Constants and assumptions'!#REF!</definedName>
     <definedName name="crossover_alkaline">'Constants and assumptions'!#REF!</definedName>
-    <definedName name="crossover_neutral">'Constants and assumptions'!$C$7</definedName>
-    <definedName name="F">'Constants and assumptions'!$C$15</definedName>
-    <definedName name="K_to_C">'Constants and assumptions'!$C$34</definedName>
-    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$35</definedName>
-    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$36</definedName>
-    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$37</definedName>
+    <definedName name="crossover_neutral">'Constants and assumptions'!$C$9</definedName>
+    <definedName name="F">'Constants and assumptions'!$C$17</definedName>
+    <definedName name="K_to_C">'Constants and assumptions'!$C$36</definedName>
+    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$37</definedName>
+    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$38</definedName>
+    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$39</definedName>
     <definedName name="mol_s_per_mA">'Kas Smith curvefit (copy)'!$B$12</definedName>
     <definedName name="mol_s_per_sccm">'Kas Smith curvefit (copy)'!$B$11</definedName>
     <definedName name="MW_CO">Products!$C$3</definedName>
-    <definedName name="P">'Constants and assumptions'!$C$21</definedName>
-    <definedName name="R_">'Constants and assumptions'!$C$16</definedName>
-    <definedName name="separation_efficiency">'Constants and assumptions'!$C$11</definedName>
-    <definedName name="T">'Constants and assumptions'!$C$33</definedName>
-    <definedName name="T_sep">'Constants and assumptions'!$C$32</definedName>
+    <definedName name="P">'Constants and assumptions'!$C$23</definedName>
+    <definedName name="R_">'Constants and assumptions'!$C$18</definedName>
+    <definedName name="separation_efficiency">'Constants and assumptions'!$C$13</definedName>
+    <definedName name="T">'Constants and assumptions'!$C$35</definedName>
+    <definedName name="T_sep">'Constants and assumptions'!$C$34</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="210">
   <si>
     <t>Utility</t>
   </si>
@@ -1228,6 +1228,43 @@
       </rPr>
       <t>/ mol solvent)</t>
     </r>
+  </si>
+  <si>
+    <t>Cost: PSA</t>
+  </si>
+  <si>
+    <t>Cost: L/L</t>
+  </si>
+  <si>
+    <t>PSA_capex_USD_1000m3_hr</t>
+  </si>
+  <si>
+    <t>LL_capex_USD_1000m3_hr</t>
+  </si>
+  <si>
+    <r>
+      <t>$/(1000 m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Arial Nova"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial Nova"/>
+        <family val="2"/>
+      </rPr>
+      <t>/hr)</t>
+    </r>
+  </si>
+  <si>
+    <t>$/(1000 mol/s)</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1616,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1842,6 +1879,9 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5253,10 +5293,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E37" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="A1:E37" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
-    <sortCondition ref="A1:A37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E39" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:E39" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E39">
+    <sortCondition ref="A1:A39"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD981D8-5D27-4DEC-AB19-B4CDEDE4E307}" name="Name" dataDxfId="52"/>
@@ -6252,16 +6292,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="4" customWidth="1"/>
     <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -6359,16 +6399,16 @@
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>133</v>
+        <v>204</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="35">
-        <v>5000</v>
+        <v>206</v>
+      </c>
+      <c r="C6" s="25">
+        <v>1989043</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>135</v>
+        <v>208</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>142</v>
@@ -6377,208 +6417,212 @@
     </row>
     <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="25">
+        <v>3349999.9967999998</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>171</v>
+        <v>209</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="25">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C10" s="8">
         <v>1000</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C11" s="11">
         <v>0.9</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C10" s="84">
-        <v>0.3</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="11">
-        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" s="84">
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C14" s="10">
         <f>0.8/10</f>
         <v>0.08</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E14" s="24" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="15" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C15" s="10">
         <v>0.22</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E15" s="24" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C16" s="10">
         <v>1.23</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E16" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C17" s="8">
         <v>96485.33212331</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="5">
-        <v>8.3144720000000003</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="9">
-        <v>44.009500000000003</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="9">
-        <v>138.2055</v>
+    <row r="18" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5">
+        <v>8.3144720000000003</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>46</v>
+        <v>88</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C19" s="9">
-        <v>31.998799999999999</v>
+        <v>44.009500000000003</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>29</v>
@@ -6586,15 +6630,15 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>44</v>
+    <row r="20" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="C20" s="9">
-        <v>18.015799999999999</v>
+        <v>138.2055</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>29</v>
@@ -6602,92 +6646,92 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8">
-        <v>101325</v>
+        <v>95</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="9">
+        <v>31.998799999999999</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="9">
+        <v>18.015799999999999</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="8">
+        <v>101325</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C24" s="11">
         <f>350/365</f>
         <v>0.95890410958904104</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="29">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="36">
-        <v>10</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>113</v>
-      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="69" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="75">
-        <v>2500</v>
-      </c>
-      <c r="D25" s="69" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="69"/>
+      <c r="A25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="29">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="35">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="36">
+        <v>10</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>113</v>
@@ -6695,201 +6739,227 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="75">
+        <v>2500</v>
+      </c>
+      <c r="D27" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="69"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="35">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C29" s="11">
         <v>0.05</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="29">
-        <v>2500</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="6">
-        <v>10</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>20</v>
-      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="6">
-        <v>0.247</v>
+        <v>74</v>
+      </c>
+      <c r="C30" s="29">
+        <v>2500</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>20</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E30" s="24"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="6">
+        <v>10</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.247</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C33" s="6">
         <f>0.041*1000</f>
         <v>41</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E33" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C34" s="10">
         <v>313.14999999999998</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E34" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C35" s="10">
         <v>313.14999999999998</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C36" s="16">
         <v>273.14999999999998</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D36" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C37" s="8">
         <f>3600</f>
         <v>3600</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C38" s="8">
         <f>1055870</f>
         <v>1055870</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C39" s="8">
         <f>kJ_per_mmBtu/kJ_per_kWh</f>
         <v>293.29722222222222</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
@@ -6910,38 +6980,46 @@
       <c r="A46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="A47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="5"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1" xr:uid="{B2106B39-835F-40BC-BDFE-DE3B87B90F64}"/>
-    <hyperlink ref="E6" r:id="rId2" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{13C42B5A-CBC8-4B1A-A9AB-3BCDE19ECC9C}"/>
-    <hyperlink ref="E9" r:id="rId3" display="Brandl et al" xr:uid="{EF89FF7B-65AC-4D83-8890-C13EE030FEED}"/>
+    <hyperlink ref="E14" r:id="rId1" xr:uid="{B2106B39-835F-40BC-BDFE-DE3B87B90F64}"/>
+    <hyperlink ref="E8" r:id="rId2" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{13C42B5A-CBC8-4B1A-A9AB-3BCDE19ECC9C}"/>
+    <hyperlink ref="E11" r:id="rId3" display="Brandl et al" xr:uid="{EF89FF7B-65AC-4D83-8890-C13EE030FEED}"/>
     <hyperlink ref="E5" r:id="rId4" display="Seider et al: $0.27/m3; Alerte et al: $0.0145/kg" xr:uid="{428FA07D-32E1-4E39-B95F-F3FC1495D338}"/>
     <hyperlink ref="E4" r:id="rId5" display="IEA, average for power gen" xr:uid="{781250D3-74FF-4AAC-876D-B170419E0026}"/>
-    <hyperlink ref="E32" r:id="rId6" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
-    <hyperlink ref="E13" r:id="rId7" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
-    <hyperlink ref="E14" r:id="rId8" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
-    <hyperlink ref="E30" r:id="rId9" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
+    <hyperlink ref="E34" r:id="rId6" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
+    <hyperlink ref="E15" r:id="rId7" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
+    <hyperlink ref="E16" r:id="rId8" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
+    <hyperlink ref="E32" r:id="rId9" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
+    <hyperlink ref="E6" r:id="rId11" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{B305148C-D46E-4A68-A9BE-7CDAF5B30D3F}"/>
+    <hyperlink ref="E7" r:id="rId12" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{063033EA-CFBF-459E-876F-914E3FE1C3B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6950,9 +7028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7059,7 +7137,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
@@ -7089,7 +7167,7 @@
         <v>-2.4870000000000001</v>
       </c>
       <c r="J3" s="5">
-        <v>-375</v>
+        <v>-182</v>
       </c>
       <c r="K3" s="5">
         <v>1</v>
@@ -7136,8 +7214,8 @@
       <c r="I4" s="66">
         <v>-0.71199999999999997</v>
       </c>
-      <c r="J4" s="66">
-        <v>-416</v>
+      <c r="J4" s="5">
+        <v>-182</v>
       </c>
       <c r="K4" s="66">
         <v>10</v>
@@ -7271,8 +7349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4385D70-1AE4-4A35-988B-BBC4298D1C90}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7426,8 +7504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8976AAB6-E21A-42F8-BEF8-70CDE446E133}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7479,7 +7557,7 @@
       <c r="C2" s="86">
         <v>250</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="91">
         <f>0.75/100</f>
         <v>7.4999999999999997E-3</v>
       </c>
@@ -7509,7 +7587,7 @@
       <c r="C3" s="86">
         <v>250</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D3" s="72">
         <v>0.01</v>
       </c>
       <c r="E3" s="5"/>
@@ -7530,7 +7608,7 @@
       <c r="C4" s="86">
         <v>250</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D4" s="72">
         <v>0.01</v>
       </c>
       <c r="E4" s="6"/>

</xml_diff>

<commit_message>
Updated solvent cost etc
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1372" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7573D18C-0561-446C-B4E6-3C4DB0CE5B63}"/>
+  <xr:revisionPtr revIDLastSave="1418" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE25F94A-D602-4A9D-868E-26129E46B096}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14580" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -32,18 +32,18 @@
     <definedName name="crossover_alkaline">'Constants and assumptions'!#REF!</definedName>
     <definedName name="crossover_neutral">'Constants and assumptions'!$C$9</definedName>
     <definedName name="F">'Constants and assumptions'!$C$17</definedName>
-    <definedName name="K_to_C">'Constants and assumptions'!$C$36</definedName>
-    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$37</definedName>
-    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$38</definedName>
-    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$39</definedName>
+    <definedName name="K_to_C">'Constants and assumptions'!$C$37</definedName>
+    <definedName name="kJ_per_kWh">'Constants and assumptions'!$C$38</definedName>
+    <definedName name="kJ_per_mmBtu">'Constants and assumptions'!$C$39</definedName>
+    <definedName name="kWh_per_mmBtu">'Constants and assumptions'!$C$40</definedName>
     <definedName name="mol_s_per_mA">'Kas Smith curvefit (copy)'!$B$12</definedName>
     <definedName name="mol_s_per_sccm">'Kas Smith curvefit (copy)'!$B$11</definedName>
     <definedName name="MW_CO">Products!$C$3</definedName>
     <definedName name="P">'Constants and assumptions'!$C$23</definedName>
     <definedName name="R_">'Constants and assumptions'!$C$18</definedName>
     <definedName name="separation_efficiency">'Constants and assumptions'!$C$13</definedName>
-    <definedName name="T">'Constants and assumptions'!$C$35</definedName>
-    <definedName name="T_sep">'Constants and assumptions'!$C$34</definedName>
+    <definedName name="T">'Constants and assumptions'!$C$36</definedName>
+    <definedName name="T_sep">'Constants and assumptions'!$C$35</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -115,6 +115,53 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={ECC5778C-B306-4101-9455-D2B811F9E1B3}</author>
+    <author>tc={168996AD-382A-4647-91D8-9337C1109D7E}</author>
+    <author>tc={317D1D06-DBFE-4387-B801-D2EDD5F30074}</author>
+    <author>tc={BF97B819-C241-44FC-AA8D-937FDD0CF315}</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{ECC5778C-B306-4101-9455-D2B811F9E1B3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.intratec.us/chemical-markets/acetonitrile-price</t>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="1" shapeId="0" xr:uid="{168996AD-382A-4647-91D8-9337C1109D7E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.imarcgroup.com/propylene-carbonate-pricing-report</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="2" shapeId="0" xr:uid="{317D1D06-DBFE-4387-B801-D2EDD5F30074}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://doi.org/10.1016/j.jct.2019.106017
+Fig 4</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="3" shapeId="0" xr:uid="{BF97B819-C241-44FC-AA8D-937FDD0CF315}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.imarcgroup.com/dimethyl-sulfoxide-pricing-report
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={07BD2C0B-3DD0-40BC-AD52-A79697FDE249}</author>
   </authors>
   <commentList>
@@ -153,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="215">
   <si>
     <t>Utility</t>
   </si>
@@ -1268,6 +1315,18 @@
   </si>
   <si>
     <t>Kinematic viscosity (mm^2/s)</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>Ratio: Solvent feed vs product rate</t>
+  </si>
+  <si>
+    <t>excess_solvent_ratio</t>
+  </si>
+  <si>
+    <t>mol/s solvent per mol/s CO2</t>
   </si>
 </sst>
 </file>
@@ -1841,9 +1900,6 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1875,6 +1931,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5299,10 +5358,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E39" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="A1:E39" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E39">
-    <sortCondition ref="A1:A39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E40" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:E40" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
+    <sortCondition ref="A1:A40"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD981D8-5D27-4DEC-AB19-B4CDEDE4E307}" name="Name" dataDxfId="52"/>
@@ -6291,6 +6350,49 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C2" dT="2024-12-03T18:32:44.07" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{ECC5778C-B306-4101-9455-D2B811F9E1B3}">
+    <text>https://www.intratec.us/chemical-markets/acetonitrile-price</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3329351198</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="59" url="https://www.intratec.us/chemical-markets/acetonitrile-price"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="C3" dT="2024-12-03T18:30:41.82" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{168996AD-382A-4647-91D8-9337C1109D7E}">
+    <text>https://www.imarcgroup.com/propylene-carbonate-pricing-report</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>2517436472</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="61" url="https://www.imarcgroup.com/propylene-carbonate-pricing-report"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="H3" dT="2024-12-03T18:25:05.42" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{317D1D06-DBFE-4387-B801-D2EDD5F30074}">
+    <text>https://doi.org/10.1016/j.jct.2019.106017
+Fig 4</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3672286581</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="41" url="https://doi.org/10.1016/j.jct.2019.106017"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="C4" dT="2024-12-03T18:29:32.47" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{BF97B819-C241-44FC-AA8D-937FDD0CF315}">
+    <text xml:space="preserve">https://www.imarcgroup.com/dimethyl-sulfoxide-pricing-report
+</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3022425215</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="60" url="https://www.imarcgroup.com/dimethyl-sulfoxide-pricing-report"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="C2" dT="2024-11-11T22:11:30.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{07BD2C0B-3DD0-40BC-AD52-A79697FDE249}">
     <text>From Chen Hallett Green Chem 2014</text>
   </threadedComment>
@@ -6299,10 +6401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6476,7 +6578,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>178</v>
       </c>
@@ -6515,7 +6617,7 @@
       <c r="B12" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="84">
+      <c r="C12" s="83">
         <v>0.3</v>
       </c>
       <c r="D12" s="6"/>
@@ -6572,7 +6674,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>84</v>
       </c>
@@ -6793,51 +6895,49 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" s="67" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="88">
+        <v>100</v>
+      </c>
+      <c r="D30" s="67" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="71"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="29">
+      <c r="C31" s="88">
         <v>2500</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="E30" s="24"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="6">
-        <v>10</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>20</v>
-      </c>
+      <c r="E31" s="71"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C32" s="6">
-        <v>0.247</v>
+        <v>10</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>20</v>
@@ -6846,130 +6946,145 @@
     </row>
     <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.247</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C34" s="6">
         <f>0.041*1000</f>
         <v>41</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E34" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C34" s="10">
-        <v>313.14999999999998</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="C35" s="10">
         <v>313.14999999999998</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="16">
-        <v>273.14999999999998</v>
-      </c>
-      <c r="D36" s="16" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="10">
+        <v>313.14999999999998</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="16">
+        <v>273.14999999999998</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C38" s="8">
         <f>3600</f>
         <v>3600</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C39" s="8">
         <f>1055870</f>
         <v>1055870</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C40" s="8">
         <f>kJ_per_mmBtu/kJ_per_kWh</f>
         <v>293.29722222222222</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
@@ -6993,20 +7108,23 @@
       <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
-      <c r="B50" s="9"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7015,10 +7133,10 @@
     <hyperlink ref="E11" r:id="rId3" display="Brandl et al" xr:uid="{EF89FF7B-65AC-4D83-8890-C13EE030FEED}"/>
     <hyperlink ref="E5" r:id="rId4" display="Seider et al: $0.27/m3; Alerte et al: $0.0145/kg" xr:uid="{428FA07D-32E1-4E39-B95F-F3FC1495D338}"/>
     <hyperlink ref="E4" r:id="rId5" display="IEA, average for power gen" xr:uid="{781250D3-74FF-4AAC-876D-B170419E0026}"/>
-    <hyperlink ref="E34" r:id="rId6" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
+    <hyperlink ref="E35" r:id="rId6" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
     <hyperlink ref="E15" r:id="rId7" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
     <hyperlink ref="E16" r:id="rId8" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
-    <hyperlink ref="E32" r:id="rId9" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
+    <hyperlink ref="E33" r:id="rId9" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
     <hyperlink ref="E13" r:id="rId10" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
     <hyperlink ref="E6" r:id="rId11" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{B305148C-D46E-4A68-A9BE-7CDAF5B30D3F}"/>
     <hyperlink ref="E7" r:id="rId12" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{063033EA-CFBF-459E-876F-914E3FE1C3B5}"/>
@@ -7035,9 +7153,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N3" sqref="N3"/>
+      <selection pane="topRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7185,8 +7303,8 @@
       <c r="M3" s="72">
         <v>0.7</v>
       </c>
-      <c r="N3" s="85">
-        <v>336.2</v>
+      <c r="N3" s="84">
+        <v>337</v>
       </c>
       <c r="O3" s="24" t="s">
         <v>20</v>
@@ -7282,8 +7400,8 @@
       <c r="M5" s="72">
         <v>0.7</v>
       </c>
-      <c r="N5" s="85">
-        <v>331.6</v>
+      <c r="N5" s="84">
+        <v>332.4</v>
       </c>
       <c r="O5" s="24" t="s">
         <v>201</v>
@@ -7353,11 +7471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4385D70-1AE4-4A35-988B-BBC4298D1C90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4385D70-1AE4-4A35-988B-BBC4298D1C90}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7375,7 +7493,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>184</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -7396,7 +7514,7 @@
       <c r="G1" s="67" t="s">
         <v>188</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="6" t="s">
         <v>203</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -7407,14 +7525,14 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="77" t="s">
         <v>170</v>
       </c>
       <c r="B2" s="9">
         <v>41.05</v>
       </c>
-      <c r="C2" s="76">
-        <v>0.06</v>
+      <c r="C2" s="9">
+        <v>2.7</v>
       </c>
       <c r="D2" s="8">
         <v>786</v>
@@ -7422,11 +7540,12 @@
       <c r="E2" s="10">
         <v>0.89</v>
       </c>
-      <c r="F2" s="88">
+      <c r="F2" s="87">
         <f>(Products6[[#This Row],[Viscosity (cP)]]/100)/Products6[[#This Row],[Density (kg/m3)]]*10000</f>
         <v>0.11323155216284986</v>
       </c>
       <c r="G2" s="68">
+        <f>Products6[[#This Row],[Viscosity (cP)]]</f>
         <v>0.89</v>
       </c>
       <c r="H2" s="68">
@@ -7440,73 +7559,73 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="78" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="77">
+      <c r="B3" s="9">
         <v>102.09</v>
       </c>
-      <c r="C3" s="77">
-        <v>10</v>
-      </c>
-      <c r="D3" s="74">
+      <c r="C3" s="9">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="D3" s="8">
         <v>1200</v>
       </c>
-      <c r="E3" s="74">
-        <v>2.5</v>
-      </c>
-      <c r="F3" s="88">
+      <c r="E3" s="10">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="F3" s="87">
         <f>(Products6[[#This Row],[Viscosity (cP)]]/100)/Products6[[#This Row],[Density (kg/m3)]]*100</f>
-        <v>2.0833333333333337E-3</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="68">
-        <v>0.15</v>
-      </c>
-      <c r="I3" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="J3" s="74" t="s">
-        <v>195</v>
-      </c>
+        <v>2.1083333333333332E-3</v>
+      </c>
+      <c r="G3" s="68">
+        <f>Products6[[#This Row],[Viscosity (cP)]]</f>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="H3" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="79" t="s">
         <v>194</v>
       </c>
-      <c r="B4" s="77">
+      <c r="B4" s="9">
         <v>78.13</v>
       </c>
-      <c r="C4" s="77">
-        <v>50</v>
-      </c>
-      <c r="D4" s="74">
+      <c r="C4" s="9">
+        <v>2.66</v>
+      </c>
+      <c r="D4" s="8">
         <v>1095</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="10">
         <v>1.99</v>
       </c>
-      <c r="F4" s="88">
+      <c r="F4" s="87">
         <f>(Products6[[#This Row],[Viscosity (cP)]]/100)/Products6[[#This Row],[Density (kg/m3)]]*100</f>
         <v>1.817351598173516E-3</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="68">
+        <f>Products6[[#This Row],[Viscosity (cP)]]</f>
+        <v>1.99</v>
+      </c>
       <c r="H4" s="68"/>
-      <c r="I4" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="J4" s="74" t="s">
-        <v>195</v>
-      </c>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
       <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="G5" s="26" t="s">
+        <v>211</v>
+      </c>
       <c r="H5" s="26"/>
       <c r="J5" s="26"/>
     </row>
@@ -7518,8 +7637,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7546,7 +7666,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -7572,16 +7692,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="77" t="s">
         <v>174</v>
       </c>
       <c r="B2" s="9">
         <v>341.91</v>
       </c>
-      <c r="C2" s="86">
+      <c r="C2" s="85">
         <v>250</v>
       </c>
-      <c r="D2" s="87">
+      <c r="D2" s="86">
         <f>0.75/100</f>
         <v>7.4999999999999997E-3</v>
       </c>
@@ -7602,13 +7722,13 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="78" t="s">
         <v>196</v>
       </c>
       <c r="B3" s="9">
         <v>329.27</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="85">
         <v>250</v>
       </c>
       <c r="D3" s="72">
@@ -7623,13 +7743,13 @@
       <c r="I3" s="66"/>
     </row>
     <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="78" t="s">
         <v>197</v>
       </c>
       <c r="B4" s="9">
         <v>217.06</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="85">
         <v>250</v>
       </c>
       <c r="D4" s="72">
@@ -7644,9 +7764,9 @@
       <c r="I4" s="66"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="66"/>
       <c r="E5" s="26"/>
       <c r="F5" s="66"/>

</xml_diff>

<commit_message>
Removed reference electrolyte properties
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1420" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48EFFCB3-38D5-41B5-B4F0-027EEC1CEC35}"/>
+  <xr:revisionPtr revIDLastSave="1492" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4DBFBA7-6A74-49B7-A14F-E8BEFF95F929}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="4" activeTab="5" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="219">
   <si>
     <t>Utility</t>
   </si>
@@ -657,12 +657,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Optimal SPC @ 7.6 c/kWh, Hawks model</t>
-  </si>
-  <si>
-    <t>Optimal j @ 7.6 c/kWh, Hawks model</t>
-  </si>
-  <si>
     <t>Electricity - wind + storage</t>
   </si>
   <si>
@@ -1105,9 +1099,6 @@
     <t>Gas constant</t>
   </si>
   <si>
-    <t>George (Kirk-Othmer Encyclopedia 2001)</t>
-  </si>
-  <si>
     <t>Electrolyzer assumption: Membrane ohmic resistance</t>
   </si>
   <si>
@@ -1327,6 +1318,29 @@
   </si>
   <si>
     <t>mol/s solvent per mol/s CO2</t>
+  </si>
+  <si>
+    <t>Boor, Ramdin (Ind. Eng. Chem. 2022)</t>
+  </si>
+  <si>
+    <t>CEPCI 2021: 773.1
+CEPCI 2024: ~800 (https://toweringskills.com/financial-analysis/cost-indices/)</t>
+  </si>
+  <si>
+    <t>CEPCI 2020: 596.2
+CEPCI 2024: ~800 (https://toweringskills.com/financial-analysis/cost-indices/)</t>
+  </si>
+  <si>
+    <t>U.S. Energy Information Administration (2024 Jan - Jun average) - industrial retail; GREET (2022)</t>
+  </si>
+  <si>
+    <t>George (Kirk-Othmer Encyclopedia 2001) adjusted by 1% inflation; but $0.1 (syngas?) in Guerra, Hodge (Joule, 2023)</t>
+  </si>
+  <si>
+    <t>Optimal j @ 8.2 c/kWh, no tradeoff</t>
+  </si>
+  <si>
+    <t>Chosen SPC, no tradeoff</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1692,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1933,6 +1947,9 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1944,12 +1961,6 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5393,8 +5404,8 @@
     <tableColumn id="8" xr3:uid="{63FE646D-E5BD-46A5-B63F-54D7C89DFC20}" name="Tafel slope (mV/dec)" dataDxfId="36"/>
     <tableColumn id="7" xr3:uid="{8762D60F-6494-4D48-BF71-09EE6526135E}" name="Reference current density (mA/cm2)" dataDxfId="35"/>
     <tableColumn id="15" xr3:uid="{C96EBEF2-D837-4395-8D46-7E2BC536E261}" name="FECO2R at SPC = 0" dataDxfId="34"/>
-    <tableColumn id="16" xr3:uid="{F3E3F633-1F65-481C-8C36-D0FBD783D2AB}" name="Optimal SPC @ 7.6 c/kWh, Hawks model" dataDxfId="33"/>
-    <tableColumn id="17" xr3:uid="{06806002-8BCC-442F-99A4-15A00506143C}" name="Optimal j @ 7.6 c/kWh, Hawks model" dataDxfId="32"/>
+    <tableColumn id="16" xr3:uid="{F3E3F633-1F65-481C-8C36-D0FBD783D2AB}" name="Chosen SPC, no tradeoff" dataDxfId="33"/>
+    <tableColumn id="17" xr3:uid="{06806002-8BCC-442F-99A4-15A00506143C}" name="Optimal j @ 8.2 c/kWh, no tradeoff" dataDxfId="32"/>
     <tableColumn id="4" xr3:uid="{EA53ED90-0A02-4FC0-8D2F-B62ACD3411A0}" name="References" dataDxfId="31"/>
     <tableColumn id="10" xr3:uid="{15AF80F1-11B7-4792-895F-6EC0B2B7A7A4}" name="References 2" dataDxfId="30"/>
   </tableColumns>
@@ -6406,15 +6417,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" style="4" customWidth="1"/>
-    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
+    <col min="3" max="5" width="21.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="29" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -6438,10 +6450,10 @@
     </row>
     <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" s="29">
         <v>1</v>
@@ -6454,10 +6466,10 @@
     </row>
     <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C3" s="29">
         <v>1</v>
@@ -6468,9 +6480,9 @@
       <c r="E3" s="24"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>68</v>
@@ -6482,90 +6494,99 @@
         <v>69</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" s="76">
         <f>0.0145</f>
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E5" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="C6" s="25">
+        <f>5000*800/773.1</f>
+        <v>5173.9749062217043</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="25">
+        <f>36703.01902*800/596.2</f>
+        <v>49249.27074136195</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="25">
+        <f>1989043*800/596.2</f>
+        <v>2668960.7514256961</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="25">
-        <v>1989043</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C7" s="25">
-        <v>36703.01902</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="25">
-        <v>5000</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="E8" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>33</v>
@@ -6577,16 +6598,16 @@
         <v>17</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C10" s="8">
         <v>1000</v>
@@ -6599,26 +6620,26 @@
     </row>
     <row r="11" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="11">
         <v>0.9</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C12" s="82">
         <v>0.3</v>
@@ -6629,7 +6650,7 @@
     </row>
     <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>66</v>
@@ -6644,28 +6665,28 @@
     </row>
     <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="C14" s="10">
         <f>0.8/10</f>
         <v>0.08</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C15" s="10">
         <v>0.22</v>
@@ -6674,12 +6695,12 @@
         <v>22</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>34</v>
@@ -6696,7 +6717,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -6710,9 +6731,9 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>9</v>
@@ -6728,7 +6749,7 @@
     </row>
     <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>43</v>
@@ -6744,7 +6765,7 @@
     </row>
     <row r="20" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>73</v>
@@ -6760,7 +6781,7 @@
     </row>
     <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>46</v>
@@ -6776,7 +6797,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>44</v>
@@ -6792,7 +6813,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>15</v>
@@ -6808,10 +6829,10 @@
     </row>
     <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C24" s="11">
         <f>350/365</f>
@@ -6823,10 +6844,10 @@
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C25" s="29">
         <v>0</v>
@@ -6837,55 +6858,55 @@
     </row>
     <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C26" s="36">
         <v>10</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C27" s="75">
         <v>2500</v>
       </c>
       <c r="D27" s="69" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E27" s="69"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C28" s="35">
         <v>1</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>75</v>
@@ -6899,23 +6920,23 @@
     </row>
     <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="67" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B30" s="67" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C30" s="87">
         <v>100</v>
       </c>
       <c r="D30" s="67" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E30" s="71"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B31" s="67" t="s">
         <v>74</v>
@@ -6924,14 +6945,14 @@
         <v>2500</v>
       </c>
       <c r="D31" s="67" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E31" s="71"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>37</v>
@@ -6949,7 +6970,7 @@
     </row>
     <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>35</v>
@@ -6967,7 +6988,7 @@
     </row>
     <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>36</v>
@@ -6977,7 +6998,7 @@
         <v>41</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>20</v>
@@ -6986,7 +7007,7 @@
     </row>
     <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>38</v>
@@ -7004,10 +7025,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C36" s="10">
         <v>313.14999999999998</v>
@@ -7020,7 +7041,7 @@
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>39</v>
@@ -7036,7 +7057,7 @@
     </row>
     <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>40</v>
@@ -7053,7 +7074,7 @@
     </row>
     <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>42</v>
@@ -7070,7 +7091,7 @@
     </row>
     <row r="40" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>41</v>
@@ -7132,22 +7153,24 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E14" r:id="rId1" xr:uid="{B2106B39-835F-40BC-BDFE-DE3B87B90F64}"/>
-    <hyperlink ref="E8" r:id="rId2" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{13C42B5A-CBC8-4B1A-A9AB-3BCDE19ECC9C}"/>
-    <hyperlink ref="E11" r:id="rId3" display="Brandl et al" xr:uid="{EF89FF7B-65AC-4D83-8890-C13EE030FEED}"/>
-    <hyperlink ref="E5" r:id="rId4" display="Seider et al: $0.27/m3; Alerte et al: $0.0145/kg" xr:uid="{428FA07D-32E1-4E39-B95F-F3FC1495D338}"/>
-    <hyperlink ref="E4" r:id="rId5" display="IEA, average for power gen" xr:uid="{781250D3-74FF-4AAC-876D-B170419E0026}"/>
-    <hyperlink ref="E35" r:id="rId6" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
-    <hyperlink ref="E15" r:id="rId7" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
-    <hyperlink ref="E16" r:id="rId8" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
-    <hyperlink ref="E33" r:id="rId9" xr:uid="{214EAADB-058E-4DBA-880F-727E021F35A8}"/>
-    <hyperlink ref="E13" r:id="rId10" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
-    <hyperlink ref="E6" r:id="rId11" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{B305148C-D46E-4A68-A9BE-7CDAF5B30D3F}"/>
-    <hyperlink ref="E7" r:id="rId12" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{063033EA-CFBF-459E-876F-914E3FE1C3B5}"/>
+    <hyperlink ref="E11" r:id="rId2" display="Brandl et al" xr:uid="{EF89FF7B-65AC-4D83-8890-C13EE030FEED}"/>
+    <hyperlink ref="E5" r:id="rId3" display="Seider et al: $0.27/m3; Alerte et al: $0.0145/kg" xr:uid="{428FA07D-32E1-4E39-B95F-F3FC1495D338}"/>
+    <hyperlink ref="E4" r:id="rId4" display="IEA, average for power gen" xr:uid="{781250D3-74FF-4AAC-876D-B170419E0026}"/>
+    <hyperlink ref="E35" r:id="rId5" xr:uid="{1D582B49-C9A3-4464-96C4-7694D2F23D8F}"/>
+    <hyperlink ref="E15" r:id="rId6" display="Chemours 2024; Nafion N117" xr:uid="{C255EE5C-FBDD-4176-A67A-8F3FD3120E2E}"/>
+    <hyperlink ref="E16" r:id="rId7" xr:uid="{C621EBC1-D2D7-4FBE-8E4B-BC10DF4928D4}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{2C690385-64CC-452A-875C-728C51C7F159}"/>
+    <hyperlink ref="E6" r:id="rId9" location="fig2" display="Badgett, Cortright (J Cleaner Prod 2022)" xr:uid="{13C42B5A-CBC8-4B1A-A9AB-3BCDE19ECC9C}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{02516210-4A57-4505-9BB9-81760639675F}"/>
+    <hyperlink ref="E33" r:id="rId11" xr:uid="{4036FC5E-2405-4C4F-9382-95746ACACF99}"/>
+    <hyperlink ref="E32" r:id="rId12" xr:uid="{A2BA9811-CE47-4570-9C89-3F1B13200BAB}"/>
+    <hyperlink ref="E34" r:id="rId13" xr:uid="{D6C65685-0DF2-44D6-9321-5CE49E794532}"/>
+    <hyperlink ref="E8" r:id="rId14" xr:uid="{BD6E9C34-DA45-404C-A535-A5E941272F90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7156,9 +7179,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7218,10 +7241,10 @@
         <v>72</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>78</v>
+        <v>217</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>24</v>
@@ -7265,7 +7288,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
@@ -7285,7 +7308,8 @@
         <v>10160</v>
       </c>
       <c r="G3" s="9">
-        <v>0.6</v>
+        <f>0.6*(1.015^(2024-2001))</f>
+        <v>0.84502629276592345</v>
       </c>
       <c r="H3" s="10">
         <v>-0.06</v>
@@ -7307,21 +7331,21 @@
         <v>0.7</v>
       </c>
       <c r="N3" s="83">
-        <v>337</v>
+        <v>329.4</v>
       </c>
       <c r="O3" s="24" t="s">
         <v>20</v>
       </c>
       <c r="P3" s="39" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C4" s="9">
         <v>46.024999999999999</v>
@@ -7361,15 +7385,15 @@
         <v>20</v>
       </c>
       <c r="P4" s="39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="40" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C5" s="10">
         <v>90.03</v>
@@ -7404,13 +7428,13 @@
         <v>0.7</v>
       </c>
       <c r="N5" s="83">
-        <v>332.4</v>
+        <v>324.89999999999998</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="P5" s="72" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="57" x14ac:dyDescent="0.2">
@@ -7424,7 +7448,7 @@
         <v>65</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>65</v>
@@ -7436,7 +7460,7 @@
         <v>70</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>56</v>
@@ -7449,7 +7473,7 @@
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
+      <c r="N6" s="83"/>
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
     </row>
@@ -7461,8 +7485,8 @@
     <hyperlink ref="H6" r:id="rId3" display="Bui Weber Chem Rev 2022" xr:uid="{D54C8481-3AD6-4B97-878B-D2C90AD4D097}"/>
     <hyperlink ref="O4" r:id="rId4" xr:uid="{8DCF1B3E-E4C0-4519-B0A4-B9CFE6918586}"/>
     <hyperlink ref="O5" r:id="rId5" xr:uid="{42FBBE18-D944-424A-B062-2455F7054E13}"/>
-    <hyperlink ref="P3" r:id="rId6" display="Jouny, Jiao I&amp;EC 2018" xr:uid="{10B5C8FC-32D4-41B8-BAEB-C077AC9722AB}"/>
-    <hyperlink ref="O3" r:id="rId7" xr:uid="{A4F65FF6-C6EC-40B1-9701-93F5858A18BD}"/>
+    <hyperlink ref="O3" r:id="rId6" xr:uid="{A4F65FF6-C6EC-40B1-9701-93F5858A18BD}"/>
+    <hyperlink ref="P3" r:id="rId7" display="Jouny, Jiao I&amp;EC 2018" xr:uid="{055CF2D0-A5B8-4CD1-86AB-6306FD0BDCB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -7478,7 +7502,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7497,28 +7521,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="67" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>188</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>24</v>
@@ -7529,7 +7553,7 @@
     </row>
     <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2" s="9">
         <v>41.05</v>
@@ -7555,15 +7579,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I2" s="71" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="92" t="s">
-        <v>193</v>
+      <c r="A3" s="77" t="s">
+        <v>190</v>
       </c>
       <c r="B3" s="9">
         <v>102.09</v>
@@ -7592,8 +7616,8 @@
       <c r="J3" s="74"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
-        <v>194</v>
+      <c r="A4" s="88" t="s">
+        <v>191</v>
       </c>
       <c r="B4" s="9">
         <v>78.13</v>
@@ -7625,9 +7649,11 @@
       <c r="C5" s="27"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
+      <c r="F5" s="26" t="s">
+        <v>208</v>
+      </c>
       <c r="G5" s="26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H5" s="26"/>
       <c r="J5" s="26"/>
@@ -7670,22 +7696,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E1" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="67" t="s">
         <v>188</v>
-      </c>
-      <c r="F1" s="67" t="s">
-        <v>191</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>24</v>
@@ -7696,7 +7722,7 @@
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B2" s="9">
         <v>341.91</v>
@@ -7715,18 +7741,18 @@
         <v>6E-10</v>
       </c>
       <c r="G2" s="71" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H2" s="71" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I2" s="69" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A3" s="78" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B3" s="9">
         <v>329.27</v>
@@ -7740,14 +7766,14 @@
       <c r="E3" s="69"/>
       <c r="F3" s="74"/>
       <c r="G3" s="71" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H3" s="74"/>
       <c r="I3" s="66"/>
     </row>
-    <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A4" s="78" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B4" s="9">
         <v>217.06</v>
@@ -7761,7 +7787,7 @@
       <c r="E4" s="67"/>
       <c r="F4" s="74"/>
       <c r="G4" s="71" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H4" s="74"/>
       <c r="I4" s="66"/>
@@ -7797,8 +7823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7843,18 +7869,18 @@
         <v>50</v>
       </c>
       <c r="D3" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="E3" s="89" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="88" t="s">
-        <v>148</v>
+      <c r="F3" s="89" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="32">
         <v>2.4E-2</v>
@@ -7863,21 +7889,21 @@
         <v>20</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="88"/>
+        <v>143</v>
+      </c>
+      <c r="E4" s="90"/>
+      <c r="F4" s="89"/>
     </row>
     <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="32">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
@@ -7893,23 +7919,23 @@
         <v>230.93061430996579</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="32">
-        <f>7.62/100</f>
-        <v>7.6200000000000004E-2</v>
+        <f>8.19/100</f>
+        <v>8.1900000000000001E-2</v>
       </c>
       <c r="C7" s="43" cm="1">
         <f t="array" ref="C7">[1]!Electricity_upstream_fuel_CO2/kWh_per_mmBtu</f>
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>149</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
@@ -7925,7 +7951,7 @@
         <v>254.376</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -7952,7 +7978,7 @@
       </c>
       <c r="B11" s="32">
         <f>B7</f>
-        <v>7.6200000000000004E-2</v>
+        <v>8.1900000000000001E-2</v>
       </c>
       <c r="C11" s="44">
         <f>C7</f>
@@ -7989,7 +8015,7 @@
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -8004,7 +8030,7 @@
     <hyperlink ref="D14" r:id="rId4" xr:uid="{AE632364-779F-4089-A88D-F487214F42B4}"/>
     <hyperlink ref="D4" r:id="rId5" display="Lazard April 2023; GREET 2022" xr:uid="{001DDBDA-9A42-4028-A4C3-DD34E948B14B}"/>
     <hyperlink ref="D6" r:id="rId6" xr:uid="{EEDCFB93-E59F-403A-99E8-154836C00872}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{2B223392-32B3-448A-811F-60ABD0999D47}"/>
+    <hyperlink ref="D7" r:id="rId7" display="U.S. Energy Information Administration (April 2023) - industrial retail; GREET (2022)" xr:uid="{2B223392-32B3-448A-811F-60ABD0999D47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -8018,7 +8044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F67CF3A-7D65-46DF-B766-523F8464614A}">
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -8043,24 +8069,24 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
       <c r="E1" s="48" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="49" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" s="46"/>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
       <c r="E2" s="65" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F2" s="48"/>
     </row>
@@ -8081,7 +8107,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -8138,7 +8164,7 @@
     </row>
     <row r="9" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" s="52">
         <v>273.14999999999998</v>
@@ -8153,14 +8179,14 @@
     </row>
     <row r="10" spans="1:12" s="49" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="53" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" s="53">
         <f>1/60/(100^3)*P/(R_*B7+20)</f>
         <v>7.3709198831561756E-7</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D10" s="53"/>
       <c r="E10" s="48"/>
@@ -8169,14 +8195,14 @@
     </row>
     <row r="11" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" s="52">
         <f>1/60/(100^3)*P/(R_*B7)</f>
         <v>7.4358305104930494E-7</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D11" s="52"/>
       <c r="E11" s="48"/>
@@ -8185,14 +8211,14 @@
     </row>
     <row r="12" spans="1:12" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" s="53">
         <f>1/(1000*2*F)</f>
         <v>5.182134828131088E-9</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D12" s="53"/>
       <c r="E12" s="48"/>
@@ -8211,102 +8237,102 @@
       <c r="B14" s="49"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="91" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="H17" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="91"/>
-      <c r="M17" s="91"/>
-      <c r="N17" s="91"/>
-      <c r="O17" s="91"/>
-      <c r="P17" s="91"/>
+      <c r="A17" s="92" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
+      <c r="H17" s="92" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="90" t="s">
+      <c r="A18" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="91"/>
+      <c r="C18" s="91" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="90"/>
-      <c r="C18" s="90" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="90"/>
+      <c r="F18" s="91"/>
       <c r="G18" s="55"/>
-      <c r="H18" s="90" t="s">
+      <c r="H18" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="91"/>
+      <c r="J18" s="91"/>
+      <c r="K18" s="91" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="91"/>
+      <c r="M18" s="91"/>
+      <c r="N18" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90" t="s">
-        <v>119</v>
-      </c>
-      <c r="L18" s="90"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
+      <c r="O18" s="91"/>
+      <c r="P18" s="91"/>
     </row>
     <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F19" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G19" s="55"/>
       <c r="H19" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="J19" s="57" t="s">
         <v>154</v>
       </c>
-      <c r="I19" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="J19" s="57" t="s">
-        <v>156</v>
-      </c>
       <c r="K19" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="L19" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="M19" s="57" t="s">
         <v>154</v>
       </c>
-      <c r="L19" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="M19" s="57" t="s">
-        <v>156</v>
-      </c>
       <c r="N19" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="O19" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="P19" s="57" t="s">
         <v>154</v>
-      </c>
-      <c r="O19" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="P19" s="57" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
@@ -10009,10 +10035,10 @@
       <c r="P62" s="48"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H63" s="90" t="s">
-        <v>121</v>
-      </c>
-      <c r="I63" s="90"/>
+      <c r="H63" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="I63" s="91"/>
       <c r="J63" s="62"/>
       <c r="K63" s="48"/>
       <c r="L63" s="48"/>
@@ -10023,10 +10049,10 @@
     </row>
     <row r="64" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="H64" s="63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I64" s="63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J64" s="48"/>
       <c r="K64" s="48"/>

</xml_diff>

<commit_message>
Updated amount of catholyte to match anolyte
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1878" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32B5B696-E557-43B4-B535-412BB9C5BA04}"/>
+  <xr:revisionPtr revIDLastSave="1879" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE8A266C-D20D-4C64-813B-AAAF954BE05D}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21585" windowHeight="11295" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -1574,7 +1574,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1727,12 +1727,6 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Nova"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2120,29 +2114,6 @@
   <dxfs count="52">
     <dxf>
       <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial Nova"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2538,6 +2509,29 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3291,10 +3285,10 @@
     <tableColumn id="3" xr3:uid="{CCFBA968-B535-4D6B-82F9-71090461EE43}" name="Density (kg/m3)"/>
     <tableColumn id="4" xr3:uid="{6DE0BEDB-FDAC-4FA2-8AC5-B102FC6EEC22}" name="Viscosity (cP)" dataDxfId="20"/>
     <tableColumn id="11" xr3:uid="{7E968132-802A-4590-8623-AF835C5600CC}" name="Henry's constant at 298K, CO2 (mole fraction/atm)" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{4B98493F-7EF6-4DC3-A55A-0A71F419BBB2}" name="CO2 solubility, 10 bar (mol CO2/ mol solvent)" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{1008D39B-F74C-44B5-9C39-9094D52EB44D}" name="Boiling point (K)" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{4E983CB5-D8FE-442A-8A07-6298EE4689D9}" name="Vapor pressure (Pa)" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{57ADEF7D-1DC8-4D29-B0B1-B07EDD74B7FC}" name="Solubility in water" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{4B98493F-7EF6-4DC3-A55A-0A71F419BBB2}" name="CO2 solubility, 10 bar (mol CO2/ mol solvent)" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{1008D39B-F74C-44B5-9C39-9094D52EB44D}" name="Boiling point (K)" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{4E983CB5-D8FE-442A-8A07-6298EE4689D9}" name="Vapor pressure (Pa)" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{57ADEF7D-1DC8-4D29-B0B1-B07EDD74B7FC}" name="Solubility in water" dataDxfId="15"/>
     <tableColumn id="7" xr3:uid="{A94104E3-BA24-4CBD-8D8E-9581768AC69A}" name="References"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3302,30 +3296,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0BE243CA-C135-4CB6-B37F-4749B7F8C437}" name="Products67" displayName="Products67" ref="A1:H5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0BE243CA-C135-4CB6-B37F-4749B7F8C437}" name="Products67" displayName="Products67" ref="A1:H5" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:H5" xr:uid="{0BE243CA-C135-4CB6-B37F-4749B7F8C437}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5E12D873-28F4-4BAA-A124-01ED2F10306F}" name="Supporting electrolyte" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{8BFB1102-BA9E-4FA2-8287-970DFEAD7F45}" name="Molecular weight (g/mol)" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{40345891-0EC3-4D4A-9A2E-09812C6C59BF}" name="Cost ($/kg supporting)" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{5E12D873-28F4-4BAA-A124-01ED2F10306F}" name="Supporting electrolyte" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{8BFB1102-BA9E-4FA2-8287-970DFEAD7F45}" name="Molecular weight (g/mol)" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{40345891-0EC3-4D4A-9A2E-09812C6C59BF}" name="Cost ($/kg supporting)" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{580C116E-F5E0-41C5-8884-D2C8E1385F89}" name="Conductivity (S/cm)"/>
     <tableColumn id="6" xr3:uid="{C9659692-EF7D-4190-B767-6AC28EF23541}" name="Reference viscosity (cP)"/>
-    <tableColumn id="4" xr3:uid="{F0A415E1-CFAE-4B45-AF57-6D3EEBC72369}" name="Molar conductivity (S/cm.mol)" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{BF9F5B6E-2598-43D5-ABA7-189814842EF4}" name="References" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{0EA10F76-7695-4288-8BC9-D38255B25BBB}" name="References 2" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{F0A415E1-CFAE-4B45-AF57-6D3EEBC72369}" name="Molar conductivity (S/cm.mol)" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{BF9F5B6E-2598-43D5-ABA7-189814842EF4}" name="References" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{0EA10F76-7695-4288-8BC9-D38255B25BBB}" name="References 2" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F90A0C8F-F9A6-4BD9-BE38-37BCD437C167}" name="Utility_sources" displayName="Utility_sources" ref="A1:D14" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F90A0C8F-F9A6-4BD9-BE38-37BCD437C167}" name="Utility_sources" displayName="Utility_sources" ref="A1:D14" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:D14" xr:uid="{F90A0C8F-F9A6-4BD9-BE38-37BCD437C167}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{019A737E-EC43-437D-A256-C18EEEE61274}" name="Utility" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{339E3BF5-AD63-4805-BC84-16828025960D}" name="Cost ($/kWh)" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{5BD4A003-8709-44FE-A299-AB3C44A1C92B}" name="CO2 emissions (g CO2/kWh)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{106C8FDA-1A54-408F-9E45-6177A2EA926F}" name="References" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{019A737E-EC43-437D-A256-C18EEEE61274}" name="Utility" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{339E3BF5-AD63-4805-BC84-16828025960D}" name="Cost ($/kWh)" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{5BD4A003-8709-44FE-A299-AB3C44A1C92B}" name="CO2 emissions (g CO2/kWh)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{106C8FDA-1A54-408F-9E45-6177A2EA926F}" name="References" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3870,8 +3864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4383,7 +4377,7 @@
         <v>182</v>
       </c>
       <c r="C30" s="54">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>197</v>

</xml_diff>

<commit_message>
Updated the evaporation rate, but it is still not a function of volatility
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1879" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE8A266C-D20D-4C64-813B-AAAF954BE05D}"/>
+  <xr:revisionPtr revIDLastSave="1885" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC6EEBF0-38F0-4A4F-9250-E89348F173E4}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21585" windowHeight="11295" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21585" windowHeight="11295" activeTab="3" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -501,7 +501,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    From Chen Hallett Green Chem 2014</t>
+    From Chen Hallett Green Chem 2014
+Reply:
+    https://pubs.acs.org/doi/10.1021/acssuschemeng.0c03061 $10-40 / kg IL (AHAs)</t>
       </text>
     </comment>
   </commentList>
@@ -1894,7 +1896,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2039,9 +2041,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3857,6 +3856,15 @@
   <threadedComment ref="C2" dT="2024-11-11T22:11:30.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{07BD2C0B-3DD0-40BC-AD52-A79697FDE249}">
     <text>From Chen Hallett Green Chem 2014</text>
   </threadedComment>
+  <threadedComment ref="C2" dT="2025-01-21T21:36:02.14" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{D1FD7102-0BB2-45B8-8328-65159D4EFE0F}" parentId="{07BD2C0B-3DD0-40BC-AD52-A79697FDE249}">
+    <text>https://pubs.acs.org/doi/10.1021/acssuschemeng.0c03061 $10-40 / kg IL (AHAs)</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>4006977529</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="54" url="https://pubs.acs.org/doi/10.1021/acssuschemeng.0c03061"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -3864,8 +3872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4000,7 +4008,7 @@
       <c r="B7" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="64">
+      <c r="C7" s="63">
         <f>36703.01902*800/596.2</f>
         <v>49249.27074136195</v>
       </c>
@@ -4092,7 +4100,7 @@
       <c r="B12" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="C12" s="63">
+      <c r="C12" s="62">
         <v>0.3</v>
       </c>
       <c r="D12" s="40"/>
@@ -4376,7 +4384,7 @@
       <c r="B30" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="C30" s="54">
+      <c r="C30" s="53">
         <v>500</v>
       </c>
       <c r="D30" s="38" t="s">
@@ -4773,23 +4781,23 @@
       <c r="H3" s="10">
         <v>-0.06</v>
       </c>
-      <c r="I3" s="68">
+      <c r="I3" s="67">
         <f>-2.35-0.197-Products[[#This Row],[Standard potential, pH = 0 (V vs SHE)]]</f>
         <v>-2.4870000000000001</v>
       </c>
       <c r="J3" s="40">
         <v>-182</v>
       </c>
-      <c r="K3" s="68">
+      <c r="K3" s="67">
         <v>1</v>
       </c>
       <c r="L3" s="10">
         <v>0.9</v>
       </c>
-      <c r="M3" s="66">
+      <c r="M3" s="65">
         <v>0.66700000000000004</v>
       </c>
-      <c r="N3" s="69">
+      <c r="N3" s="68">
         <v>312.39999999999998</v>
       </c>
       <c r="O3" s="22" t="s">
@@ -4816,7 +4824,7 @@
       <c r="E4" s="5">
         <v>2</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="66">
         <v>10000</v>
       </c>
       <c r="G4" s="9">
@@ -4825,7 +4833,7 @@
       <c r="H4" s="10">
         <v>-0.51</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="67">
         <f>-1.8+0.197-Products[[#This Row],[Standard potential, pH = 0 (V vs SHE)]]</f>
         <v>-1.093</v>
       </c>
@@ -4833,16 +4841,16 @@
         <f>0.2*1000/(3.2-5.2)</f>
         <v>-100</v>
       </c>
-      <c r="K4" s="68">
+      <c r="K4" s="67">
         <v>5.6</v>
       </c>
       <c r="L4" s="6">
         <v>0.7</v>
       </c>
-      <c r="M4" s="66">
+      <c r="M4" s="65">
         <v>0.66700000000000004</v>
       </c>
-      <c r="N4" s="69">
+      <c r="N4" s="68">
         <v>314</v>
       </c>
       <c r="O4" s="22" t="s">
@@ -4871,7 +4879,7 @@
       <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="63">
         <v>5400</v>
       </c>
       <c r="G5" s="9">
@@ -4880,13 +4888,13 @@
       <c r="H5" s="10">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
       <c r="L5" s="6">
         <v>0.74</v>
       </c>
-      <c r="M5" s="66">
+      <c r="M5" s="65">
         <v>0.66700000000000004</v>
       </c>
       <c r="N5" s="44"/>
@@ -4970,7 +4978,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5091,7 +5099,7 @@
         <f>0.05*1000</f>
         <v>50</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="64" t="s">
         <v>209</v>
       </c>
       <c r="K3" s="42" t="s">
@@ -5099,7 +5107,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="54" t="s">
         <v>167</v>
       </c>
       <c r="B4" s="9">
@@ -5138,7 +5146,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="54" t="s">
         <v>190</v>
       </c>
       <c r="B5" s="9">
@@ -5177,7 +5185,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="69" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5202,8 +5210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8976AAB6-E21A-42F8-BEF8-70CDE446E133}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5252,10 +5260,10 @@
       <c r="B2" s="9">
         <v>341.91</v>
       </c>
-      <c r="C2" s="52">
-        <v>250</v>
-      </c>
-      <c r="D2" s="53">
+      <c r="C2" s="9">
+        <v>10</v>
+      </c>
+      <c r="D2" s="52">
         <f>0.75/100</f>
         <v>7.4999999999999997E-3</v>
       </c>
@@ -5282,8 +5290,8 @@
       <c r="B3" s="9">
         <v>329.27</v>
       </c>
-      <c r="C3" s="52">
-        <v>250</v>
+      <c r="C3" s="9">
+        <v>10</v>
       </c>
       <c r="D3" s="43">
         <v>0.01</v>
@@ -5303,8 +5311,8 @@
       <c r="B4" s="9">
         <v>217.06</v>
       </c>
-      <c r="C4" s="52">
-        <v>250</v>
+      <c r="C4" s="9">
+        <v>10</v>
       </c>
       <c r="D4" s="43">
         <v>0.01</v>
@@ -5355,8 +5363,8 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="57" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
@@ -5367,10 +5375,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5379,27 +5387,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="58">
         <v>2.4E-2</v>
       </c>
-      <c r="C3" s="60">
+      <c r="C3" s="59">
         <v>50</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="70" t="s">
         <v>133</v>
       </c>
     </row>
@@ -5407,26 +5415,26 @@
       <c r="A4" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <v>2.4E-2</v>
       </c>
-      <c r="C4" s="60">
+      <c r="C4" s="59">
         <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="28" t="s">
         <v>131</v>
       </c>
@@ -5435,11 +5443,11 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <f>16.05/100</f>
         <v>0.1605</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="59">
         <v>230.93061430996579</v>
       </c>
       <c r="D6" s="28" t="s">
@@ -5450,11 +5458,11 @@
       <c r="A7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="58">
         <f>8.19/100</f>
         <v>8.1900000000000001E-2</v>
       </c>
-      <c r="C7" s="60">
+      <c r="C7" s="59">
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="28" t="s">
@@ -5465,11 +5473,11 @@
       <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="58">
         <f>2.22/kWh_per_mmBtu</f>
         <v>7.5691136219420956E-3</v>
       </c>
-      <c r="C8" s="60">
+      <c r="C8" s="59">
         <f>70.66/1000*kJ_per_kWh</f>
         <v>254.376</v>
       </c>
@@ -5481,29 +5489,29 @@
       <c r="A9" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="59">
+      <c r="B9" s="58">
         <v>0.03</v>
       </c>
-      <c r="C9" s="61"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="61"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="59">
+      <c r="B11" s="58">
         <f>B7</f>
         <v>8.1900000000000001E-2</v>
       </c>
-      <c r="C11" s="61">
+      <c r="C11" s="60">
         <f>C7</f>
         <v>414.10433834299573</v>
       </c>
@@ -5513,11 +5521,11 @@
       <c r="A12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="62">
+      <c r="B12" s="61">
         <f>B8</f>
         <v>7.5691136219420956E-3</v>
       </c>
-      <c r="C12" s="61">
+      <c r="C12" s="60">
         <f>C8</f>
         <v>254.376</v>
       </c>
@@ -5525,18 +5533,18 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="60"/>
       <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="59">
+      <c r="B14" s="58">
         <v>200</v>
       </c>
-      <c r="C14" s="61"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="32" t="s">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
Updated histograms for MC
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2005" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9826AC14-58E3-45F1-AC25-57A9829A727D}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8928" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8928" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -4752,8 +4752,8 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N4" sqref="N4"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated effect of CO2 solubility on seps, handling of solvents
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2019" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAD83AE8-ECFB-4FBB-BCB4-E9FADB1F5013}"/>
+  <xr:revisionPtr revIDLastSave="2058" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6067A9E6-005E-4C4B-BC70-A6B3534049B6}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1290" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="15990" windowHeight="15585" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -96,9 +96,11 @@
     <author>tc={E6E48448-0E21-41A5-B06E-F65140C42E87}</author>
     <author>tc={D9B01A9E-9FFA-448D-A0A9-79E915973C3A}</author>
     <author>tc={9C7BA66E-4710-4766-B736-DAB2C4C5EA8C}</author>
+    <author>tc={F0232A46-C9BF-49E2-A4AA-DE559C7A6D71}</author>
     <author>tc={38772031-2712-4E60-AF4C-BC7506EB126A}</author>
     <author>tc={19966830-0D20-46F0-AE3D-88797573DA5E}</author>
     <author>tc={61AD334A-127F-49E9-826D-132D83D54FFE}</author>
+    <author>tc={D3F419E4-0AC2-42D8-AE74-03450151D28F}</author>
     <author>tc={CF7FF991-BD99-42BD-BE0C-DD9BF8B9A73E}</author>
     <author>tc={F3E0BD3F-9F26-4F73-B97C-92F5976365D6}</author>
   </authors>
@@ -143,7 +145,15 @@
     Average for top 25 datapoints making CO</t>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{38772031-2712-4E60-AF4C-BC7506EB126A}">
+    <comment ref="N3" authorId="5" shapeId="0" xr:uid="{F0232A46-C9BF-49E2-A4AA-DE559C7A6D71}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In DMF</t>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="6" shapeId="0" xr:uid="{38772031-2712-4E60-AF4C-BC7506EB126A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -151,7 +161,7 @@
     Saveant - RT over Hg in ACN</t>
       </text>
     </comment>
-    <comment ref="K4" authorId="6" shapeId="0" xr:uid="{19966830-0D20-46F0-AE3D-88797573DA5E}">
+    <comment ref="K4" authorId="7" shapeId="0" xr:uid="{19966830-0D20-46F0-AE3D-88797573DA5E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -161,7 +171,7 @@
     DMF, 0.2 M TEACl, Pb vs Al, undivided cell</t>
       </text>
     </comment>
-    <comment ref="L4" authorId="7" shapeId="0" xr:uid="{61AD334A-127F-49E9-826D-132D83D54FFE}">
+    <comment ref="L4" authorId="8" shapeId="0" xr:uid="{61AD334A-127F-49E9-826D-132D83D54FFE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -169,7 +179,15 @@
     Average for top 50 datapoints making any oxalates or OA</t>
       </text>
     </comment>
-    <comment ref="F5" authorId="8" shapeId="0" xr:uid="{CF7FF991-BD99-42BD-BE0C-DD9BF8B9A73E}">
+    <comment ref="N4" authorId="9" shapeId="0" xr:uid="{D3F419E4-0AC2-42D8-AE74-03450151D28F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In DMSO</t>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="10" shapeId="0" xr:uid="{CF7FF991-BD99-42BD-BE0C-DD9BF8B9A73E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -179,7 +197,7 @@
     Should be able to just calculate from thermo of water condensation</t>
       </text>
     </comment>
-    <comment ref="L5" authorId="9" shapeId="0" xr:uid="{F3E0BD3F-9F26-4F73-B97C-92F5976365D6}">
+    <comment ref="L5" authorId="11" shapeId="0" xr:uid="{F3E0BD3F-9F26-4F73-B97C-92F5976365D6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -271,7 +289,7 @@
     https://doi.org/10.1016/0022-0728(90)87217-8 60.7</t>
       </text>
     </comment>
-    <comment ref="H2" authorId="5" shapeId="0" xr:uid="{CCFAFA67-1AB3-4E10-B472-4734839B5FB8}">
+    <comment ref="I2" authorId="5" shapeId="0" xr:uid="{CCFAFA67-1AB3-4E10-B472-4734839B5FB8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -279,7 +297,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="I2" authorId="6" shapeId="0" xr:uid="{7E768D53-988A-46AE-8800-331D2B19C4CA}">
+    <comment ref="J2" authorId="6" shapeId="0" xr:uid="{7E768D53-988A-46AE-8800-331D2B19C4CA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -287,7 +305,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="K2" authorId="7" shapeId="0" xr:uid="{F72D791D-203F-48D2-BBE6-FB8C410089E4}">
+    <comment ref="L2" authorId="7" shapeId="0" xr:uid="{F72D791D-203F-48D2-BBE6-FB8C410089E4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -335,7 +353,7 @@
     https://doi.org/10.1016/0378-3812(88)80106-7</t>
       </text>
     </comment>
-    <comment ref="H3" authorId="13" shapeId="0" xr:uid="{8C14FDD1-22B7-4F70-B01E-C665917CE3E4}">
+    <comment ref="I3" authorId="13" shapeId="0" xr:uid="{8C14FDD1-22B7-4F70-B01E-C665917CE3E4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -343,7 +361,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="I3" authorId="14" shapeId="0" xr:uid="{0182AE5B-5F63-4940-956C-D441191E1036}">
+    <comment ref="J3" authorId="14" shapeId="0" xr:uid="{0182AE5B-5F63-4940-956C-D441191E1036}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -394,7 +412,7 @@
     https://doi.org/10.1016/0022-0728(90)87217-8 101.6</t>
       </text>
     </comment>
-    <comment ref="H4" authorId="20" shapeId="0" xr:uid="{1983A994-3FCC-4917-A080-32AC954B27A3}">
+    <comment ref="I4" authorId="20" shapeId="0" xr:uid="{1983A994-3FCC-4917-A080-32AC954B27A3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -402,7 +420,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="I4" authorId="21" shapeId="0" xr:uid="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
+    <comment ref="J4" authorId="21" shapeId="0" xr:uid="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -410,7 +428,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="K4" authorId="22" shapeId="0" xr:uid="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
+    <comment ref="L4" authorId="22" shapeId="0" xr:uid="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -462,7 +480,7 @@
     https://doi.org/10.1016/0022-0728(90)87217-8 65.3</t>
       </text>
     </comment>
-    <comment ref="H5" authorId="28" shapeId="0" xr:uid="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
+    <comment ref="I5" authorId="28" shapeId="0" xr:uid="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -470,7 +488,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="I5" authorId="29" shapeId="0" xr:uid="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
+    <comment ref="J5" authorId="29" shapeId="0" xr:uid="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -478,7 +496,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="K5" authorId="30" shapeId="0" xr:uid="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
+    <comment ref="L5" authorId="30" shapeId="0" xr:uid="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -586,7 +604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="208">
   <si>
     <t>Utility</t>
   </si>
@@ -1477,9 +1495,6 @@
     <t>excess_solvent_ratio</t>
   </si>
   <si>
-    <t>Boor, Ramdin (Ind. Eng. Chem. 2022)</t>
-  </si>
-  <si>
     <t>CEPCI 2021: 773.1
 CEPCI 2024: ~800 (https://toweringskills.com/financial-analysis/cost-indices/)</t>
   </si>
@@ -1494,9 +1509,6 @@
     <t>George (Kirk-Othmer Encyclopedia 2001) adjusted by 1% inflation; but $0.1 (syngas?) in Guerra, Hodge (Joule, 2023)</t>
   </si>
   <si>
-    <t>Optimal j @ 8.2 c/kWh, no tradeoff</t>
-  </si>
-  <si>
     <t>Chosen SPC, no tradeoff</t>
   </si>
   <si>
@@ -1609,9 +1621,6 @@
     <t>Solvent loss fraction ((mol/s offgas)/ (mol/s solvent))</t>
   </si>
   <si>
-    <t>Conductivity, 0.3 M (S/cm)</t>
-  </si>
-  <si>
     <t>TEACl</t>
   </si>
   <si>
@@ -1625,6 +1634,26 @@
   </si>
   <si>
     <t>TBABF$_4$</t>
+  </si>
+  <si>
+    <t>Rantakyla, 2004</t>
+  </si>
+  <si>
+    <t>Base case assumes mol/h of acetonitrile
+CEPCI 2004: 444.2
+CEPCI 2024: ~800 (https://toweringskills.com/financial-analysis/cost-indices/)</t>
+  </si>
+  <si>
+    <t>Conductivity in ACN, 0.3 M (S/cm)</t>
+  </si>
+  <si>
+    <t>Conductivity factor relative to ACN</t>
+  </si>
+  <si>
+    <t>JM's estimate: 0.010 - 0.020 S/cm</t>
+  </si>
+  <si>
+    <t>Optimal j @ 8.2 c/kWh, no tradeoff (mA/cm2)</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1665,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1789,6 +1818,12 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Nova"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2156,7 +2191,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="54">
     <dxf>
       <font>
         <b val="0"/>
@@ -2609,6 +2644,26 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color auto="1"/>
         <name val="Arial Nova"/>
         <family val="2"/>
@@ -3277,58 +3332,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E40" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}" name="Constants" displayName="Constants" ref="A1:E40" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:E40" xr:uid="{4573E0AF-4F91-4E0C-A0FD-4101785DA193}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
     <sortCondition ref="A1:A40"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0CD981D8-5D27-4DEC-AB19-B4CDEDE4E307}" name="Name" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{447AB61C-D6A8-4C69-B914-F84CC2DD3D7F}" name="Variable name" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{8D0B10A0-AAB3-497D-AACC-B47886E623F4}" name="Value" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{13805BE1-5D36-4E51-B5A1-6DAB8482D1CA}" name="Unit" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{D9E6851E-6681-4B84-8DD9-9DC84337FA8D}" name="References" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{0CD981D8-5D27-4DEC-AB19-B4CDEDE4E307}" name="Name" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{447AB61C-D6A8-4C69-B914-F84CC2DD3D7F}" name="Variable name" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{8D0B10A0-AAB3-497D-AACC-B47886E623F4}" name="Value" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{13805BE1-5D36-4E51-B5A1-6DAB8482D1CA}" name="Unit" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{D9E6851E-6681-4B84-8DD9-9DC84337FA8D}" name="References" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89323130-A0D1-49F6-A5DF-27B490E4A7F3}" name="Products" displayName="Products" ref="A1:Q6" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89323130-A0D1-49F6-A5DF-27B490E4A7F3}" name="Products" displayName="Products" ref="A1:Q6" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:Q6" xr:uid="{89323130-A0D1-49F6-A5DF-27B490E4A7F3}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{3C50D7C6-76ED-4D16-B177-C24A6EDEF5E8}" name="Product" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{E3E543EF-1CAC-4E7C-917B-9F6A2A12C5A5}" name="Phase" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{60087321-E31A-4465-97EA-5E82B4930DEF}" name="Molecular weight (g/mol)" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{73F411CA-0C00-43A6-8E8A-2C96DEBEAE56}" name="n (mol e-/ mol product)" dataDxfId="40"/>
-    <tableColumn id="12" xr3:uid="{35098869-B8D6-4322-9A6F-55D84BD00AAD}" name="z (mol CO2/ mol product)" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{42FF57EE-C82B-4BEE-B6E3-5CDCD61D73F4}" name="LHV (kJ/kg product)" dataDxfId="38"/>
-    <tableColumn id="14" xr3:uid="{E9D086E2-203C-4567-AACC-7D8FDCBCFD52}" name="Cost ($/kg product)" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{F6536296-A5EF-4707-BAA4-8ED36A0299FD}" name="Standard potential, pH = 0 (V vs SHE)" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{44F64A4D-679B-4F83-A0F1-9FD50BE9A102}" name="Reference overpotential (V)" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{63FE646D-E5BD-46A5-B63F-54D7C89DFC20}" name="Tafel slope (mV/dec)" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{8762D60F-6494-4D48-BF71-09EE6526135E}" name="Reference current density (mA/cm2)" dataDxfId="33"/>
-    <tableColumn id="15" xr3:uid="{C96EBEF2-D837-4395-8D46-7E2BC536E261}" name="FECO2R at SPC = 0" dataDxfId="32"/>
-    <tableColumn id="16" xr3:uid="{F3E3F633-1F65-481C-8C36-D0FBD783D2AB}" name="Chosen SPC, no tradeoff" dataDxfId="31"/>
-    <tableColumn id="17" xr3:uid="{06806002-8BCC-442F-99A4-15A00506143C}" name="Optimal j @ 8.2 c/kWh, no tradeoff" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{EA53ED90-0A02-4FC0-8D2F-B62ACD3411A0}" name="References" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{15AF80F1-11B7-4792-895F-6EC0B2B7A7A4}" name="References 2" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{F302EFF0-A13D-4A4C-8A0B-F721AD1E47B9}" name="References 3" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{3C50D7C6-76ED-4D16-B177-C24A6EDEF5E8}" name="Product" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{E3E543EF-1CAC-4E7C-917B-9F6A2A12C5A5}" name="Phase" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{60087321-E31A-4465-97EA-5E82B4930DEF}" name="Molecular weight (g/mol)" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{73F411CA-0C00-43A6-8E8A-2C96DEBEAE56}" name="n (mol e-/ mol product)" dataDxfId="41"/>
+    <tableColumn id="12" xr3:uid="{35098869-B8D6-4322-9A6F-55D84BD00AAD}" name="z (mol CO2/ mol product)" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{42FF57EE-C82B-4BEE-B6E3-5CDCD61D73F4}" name="LHV (kJ/kg product)" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{E9D086E2-203C-4567-AACC-7D8FDCBCFD52}" name="Cost ($/kg product)" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{F6536296-A5EF-4707-BAA4-8ED36A0299FD}" name="Standard potential, pH = 0 (V vs SHE)" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{44F64A4D-679B-4F83-A0F1-9FD50BE9A102}" name="Reference overpotential (V)" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{63FE646D-E5BD-46A5-B63F-54D7C89DFC20}" name="Tafel slope (mV/dec)" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{8762D60F-6494-4D48-BF71-09EE6526135E}" name="Reference current density (mA/cm2)" dataDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{C96EBEF2-D837-4395-8D46-7E2BC536E261}" name="FECO2R at SPC = 0" dataDxfId="33"/>
+    <tableColumn id="16" xr3:uid="{F3E3F633-1F65-481C-8C36-D0FBD783D2AB}" name="Chosen SPC, no tradeoff" dataDxfId="32"/>
+    <tableColumn id="17" xr3:uid="{06806002-8BCC-442F-99A4-15A00506143C}" name="Optimal j @ 8.2 c/kWh, no tradeoff (mA/cm2)" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{EA53ED90-0A02-4FC0-8D2F-B62ACD3411A0}" name="References" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{15AF80F1-11B7-4792-895F-6EC0B2B7A7A4}" name="References 2" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{F302EFF0-A13D-4A4C-8A0B-F721AD1E47B9}" name="References 3" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}" name="Products6" displayName="Products6" ref="A1:L5" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:L5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{996983E7-48A1-4F2C-AAE8-BB6499F82011}" name="Solvent" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{7587D408-6B96-4220-A9BE-2B71A4248C30}" name="Molecular weight (g/mol)" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{8CB95F86-8F61-4051-8BEA-3EA0B1243627}" name="Cost ($/kg solvent)" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{CCFBA968-B535-4D6B-82F9-71090461EE43}" name="Density (kg/m3)" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{6DE0BEDB-FDAC-4FA2-8AC5-B102FC6EEC22}" name="Viscosity (cP)" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{7E968132-802A-4590-8623-AF835C5600CC}" name="Henry's constant at 298K, CO2 (mole fraction/atm)" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}" name="Products6" displayName="Products6" ref="A1:M5" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:M5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{996983E7-48A1-4F2C-AAE8-BB6499F82011}" name="Solvent" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{7587D408-6B96-4220-A9BE-2B71A4248C30}" name="Molecular weight (g/mol)" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{8CB95F86-8F61-4051-8BEA-3EA0B1243627}" name="Cost ($/kg solvent)" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{CCFBA968-B535-4D6B-82F9-71090461EE43}" name="Density (kg/m3)" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{6DE0BEDB-FDAC-4FA2-8AC5-B102FC6EEC22}" name="Viscosity (cP)" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{7E968132-802A-4590-8623-AF835C5600CC}" name="Henry's constant at 298K, CO2 (mole fraction/atm)" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{C14326B4-157A-4FBF-9FD5-58F36F9782B3}" name="Conductivity factor relative to ACN" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{4B98493F-7EF6-4DC3-A55A-0A71F419BBB2}" name="CO2 solubility, 10 bar (mol CO2/ mol solvent)" dataDxfId="18"/>
     <tableColumn id="6" xr3:uid="{1008D39B-F74C-44B5-9C39-9094D52EB44D}" name="Boiling point (K)" dataDxfId="17"/>
     <tableColumn id="9" xr3:uid="{4E983CB5-D8FE-442A-8A07-6298EE4689D9}" name="Vapor pressure (Pa)" dataDxfId="16"/>
@@ -3347,7 +3403,7 @@
     <tableColumn id="1" xr3:uid="{5E12D873-28F4-4BAA-A124-01ED2F10306F}" name="Supporting electrolyte" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{8BFB1102-BA9E-4FA2-8287-970DFEAD7F45}" name="Molecular weight (g/mol)" dataDxfId="10"/>
     <tableColumn id="14" xr3:uid="{40345891-0EC3-4D4A-9A2E-09812C6C59BF}" name="Cost ($/kg supporting)" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{580C116E-F5E0-41C5-8884-D2C8E1385F89}" name="Conductivity, 0.3 M (S/cm)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{580C116E-F5E0-41C5-8884-D2C8E1385F89}" name="Conductivity in ACN, 0.3 M (S/cm)" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{BF9F5B6E-2598-43D5-ABA7-189814842EF4}" name="References" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3690,6 +3746,9 @@
   <threadedComment ref="L3" dT="2024-11-11T19:54:36.26" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{9C7BA66E-4710-4766-B736-DAB2C4C5EA8C}">
     <text>Average for top 25 datapoints making CO</text>
   </threadedComment>
+  <threadedComment ref="N3" dT="2025-02-07T23:53:30.60" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{F0232A46-C9BF-49E2-A4AA-DE559C7A6D71}">
+    <text>In DMF</text>
+  </threadedComment>
   <threadedComment ref="J4" dT="2025-01-15T16:47:50.62" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{38772031-2712-4E60-AF4C-BC7506EB126A}">
     <text>Saveant - RT over Hg in ACN</text>
   </threadedComment>
@@ -3701,6 +3760,9 @@
   </threadedComment>
   <threadedComment ref="L4" dT="2025-01-15T15:40:12.85" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{61AD334A-127F-49E9-826D-132D83D54FFE}">
     <text>Average for top 50 datapoints making any oxalates or OA</text>
+  </threadedComment>
+  <threadedComment ref="N4" dT="2025-02-07T23:53:39.13" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{D3F419E4-0AC2-42D8-AE74-03450151D28F}">
+    <text>In DMSO</text>
   </threadedComment>
   <threadedComment ref="F5" dT="2025-01-15T16:01:46.09" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{CF7FF991-BD99-42BD-BE0C-DD9BF8B9A73E}">
     <text xml:space="preserve">Muller Stolten J CO2 Util 2025 </text>
@@ -3755,13 +3817,13 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="H2" dT="2025-01-20T21:27:20.62" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{CCFAFA67-1AB3-4E10-B472-4734839B5FB8}">
+  <threadedComment ref="I2" dT="2025-01-20T21:27:20.62" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{CCFAFA67-1AB3-4E10-B472-4734839B5FB8}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="I2" dT="2025-01-20T21:27:35.11" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{7E768D53-988A-46AE-8800-331D2B19C4CA}">
+  <threadedComment ref="J2" dT="2025-01-20T21:27:35.11" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{7E768D53-988A-46AE-8800-331D2B19C4CA}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="K2" dT="2025-01-20T21:27:50.71" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{F72D791D-203F-48D2-BBE6-FB8C410089E4}">
+  <threadedComment ref="L2" dT="2025-01-20T21:27:50.71" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{F72D791D-203F-48D2-BBE6-FB8C410089E4}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
   <threadedComment ref="B3" dT="2025-01-20T21:26:20.62" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{46705330-D6EB-4863-A1A8-B104F2E8D6B3}">
@@ -3791,10 +3853,10 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="H3" dT="2025-01-20T21:27:23.98" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{8C14FDD1-22B7-4F70-B01E-C665917CE3E4}">
+  <threadedComment ref="I3" dT="2025-01-20T21:27:23.98" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{8C14FDD1-22B7-4F70-B01E-C665917CE3E4}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="I3" dT="2025-01-20T21:27:38.80" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{0182AE5B-5F63-4940-956C-D441191E1036}">
+  <threadedComment ref="J3" dT="2025-01-20T21:27:38.80" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{0182AE5B-5F63-4940-956C-D441191E1036}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
   <threadedComment ref="B4" dT="2025-01-20T21:26:24.25" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{DD06A995-3E0B-473D-8CCE-79C9FDD92985}">
@@ -3834,13 +3896,13 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="H4" dT="2025-01-20T21:27:27.28" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{1983A994-3FCC-4917-A080-32AC954B27A3}">
+  <threadedComment ref="I4" dT="2025-01-20T21:27:27.28" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{1983A994-3FCC-4917-A080-32AC954B27A3}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="I4" dT="2025-01-20T21:27:42.09" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
+  <threadedComment ref="J4" dT="2025-01-20T21:27:42.09" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="K4" dT="2025-01-20T21:27:55.05" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
+  <threadedComment ref="L4" dT="2025-01-20T21:27:55.05" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
   <threadedComment ref="B5" dT="2025-01-20T21:26:28.19" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{918158CC-13D0-4406-9FA6-83AE98F2FB61}">
@@ -3882,13 +3944,13 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="H5" dT="2025-01-20T21:27:30.00" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
+  <threadedComment ref="I5" dT="2025-01-20T21:27:30.00" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="I5" dT="2025-01-20T21:27:46.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
+  <threadedComment ref="J5" dT="2025-01-20T21:27:46.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="K5" dT="2025-01-20T21:27:59.71" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
+  <threadedComment ref="L5" dT="2025-01-20T21:27:59.71" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
 </ThreadedComments>
@@ -3990,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4112,28 +4174,28 @@
         <v>127</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="56">
-        <f>36703.01902*800/596.2</f>
-        <v>49249.27074136195</v>
-      </c>
-      <c r="D7" s="38" t="s">
+      <c r="C7" s="23">
+        <f>1.3*950000*1.24*(800/444.2)*((1000)/(2160/(Solvents!H2*C19/1000)))^0.7</f>
+        <v>57368.495093584941</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E7" s="39" t="s">
-        <v>173</v>
+      <c r="E7" s="22" t="s">
+        <v>202</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -4154,7 +4216,7 @@
         <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -4502,7 +4564,7 @@
         <v>500</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="5"/>
@@ -4754,9 +4816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4817,10 +4879,10 @@
         <v>70</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>23</v>
@@ -4829,7 +4891,7 @@
         <v>59</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
@@ -4911,13 +4973,13 @@
         <v>0.66700000000000004</v>
       </c>
       <c r="N3" s="61">
-        <v>196.3</v>
+        <v>198.8</v>
       </c>
       <c r="O3" s="22" t="s">
         <v>19</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q3" s="5"/>
     </row>
@@ -4964,16 +5026,16 @@
         <v>0.66700000000000004</v>
       </c>
       <c r="N4" s="61">
-        <v>197.1</v>
+        <v>168.6</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Q4" s="22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="34" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -5015,10 +5077,10 @@
         <v>19</v>
       </c>
       <c r="P5" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q5" s="22" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
@@ -5038,7 +5100,7 @@
         <v>63</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>68</v>
@@ -5088,10 +5150,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4385D70-1AE4-4A35-988B-BBC4298D1C90}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5101,12 +5163,12 @@
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="8" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="74.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="74.25" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>155</v>
       </c>
@@ -5117,34 +5179,37 @@
         <v>156</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>158</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>198</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>145</v>
       </c>
@@ -5165,28 +5230,31 @@
         <v>1.6474464579901153E-2</v>
       </c>
       <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
         <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
         <v>0.19415787278579127</v>
       </c>
-      <c r="H2" s="10">
+      <c r="I2" s="10">
         <f>273.15+81.6</f>
         <v>354.75</v>
       </c>
-      <c r="I2" s="8">
+      <c r="J2" s="8">
         <f>11.9*1000</f>
         <v>11900</v>
       </c>
-      <c r="J2" s="63">
+      <c r="K2" s="63">
         <v>1E-4</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="M2" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="L2" s="39" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>160</v>
       </c>
@@ -5207,28 +5275,32 @@
         <v>1.2180267965895251E-2</v>
       </c>
       <c r="G3" s="10">
+        <f>1.59/5.69</f>
+        <v>0.27943760984182775</v>
+      </c>
+      <c r="H3" s="10">
         <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
         <v>0.13663423359564064</v>
       </c>
-      <c r="H3" s="10">
+      <c r="I3" s="10">
         <f>273.15+241.6</f>
         <v>514.75</v>
       </c>
-      <c r="I3" s="8">
+      <c r="J3" s="8">
         <f>0.05*1000</f>
         <v>50</v>
       </c>
-      <c r="J3" s="63">
+      <c r="K3" s="63">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="K3" s="57" t="s">
-        <v>197</v>
-      </c>
-      <c r="L3" s="39" t="s">
+      <c r="L3" s="57" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="M3" s="39" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>161</v>
       </c>
@@ -5249,30 +5321,34 @@
         <v>9.8425196850393699E-3</v>
       </c>
       <c r="G4" s="10">
+        <f>2.36/5.69</f>
+        <v>0.41476274165202104</v>
+      </c>
+      <c r="H4" s="10">
         <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
         <v>0.10758872701426347</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="10">
         <f>273.15+191.9</f>
         <v>465.04999999999995</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J4" s="8">
         <f>0.084*1000</f>
         <v>84</v>
       </c>
-      <c r="J4" s="63">
+      <c r="K4" s="63">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="L4" s="39" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="L4" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B5" s="9">
         <v>73.093999999999994</v>
@@ -5291,52 +5367,56 @@
         <v>1.5313935681470138E-2</v>
       </c>
       <c r="G5" s="10">
+        <f>3.34/5.69</f>
+        <v>0.58699472759226712</v>
+      </c>
+      <c r="H5" s="10">
         <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
         <v>0.17804541879244029</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="10">
         <f>273.15+152.8</f>
         <v>425.95</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J5" s="8">
         <f>0.439*1000</f>
         <v>439</v>
       </c>
-      <c r="J5" s="63">
+      <c r="K5" s="63">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="M5" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="L5" s="39" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" ht="57" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
-        <v>201</v>
-      </c>
-      <c r="H7" s="64"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="64"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H9" s="64"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H10" s="64"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H11" s="64"/>
+        <v>198</v>
+      </c>
+      <c r="I7" s="64"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I8" s="64"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I9" s="64"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I10" s="64"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I11" s="64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" display="Izutsu (Wiley 2009)" xr:uid="{3CE65C60-DA75-4595-8CAA-88F2C9A358C9}"/>
-    <hyperlink ref="L3" r:id="rId2" display="Izutsu (Wiley 2009)" xr:uid="{6B0DA7F9-0782-4596-8B42-F9EBE5175294}"/>
-    <hyperlink ref="L4" r:id="rId3" display="Izutsu (Wiley 2009)" xr:uid="{55B29BD6-B10F-4DCF-93BE-7B2953D8D605}"/>
-    <hyperlink ref="L5" r:id="rId4" display="Izutsu (Wiley 2009)" xr:uid="{A3AEBAE1-B668-4BB3-9056-8F0FA6D1359D}"/>
+    <hyperlink ref="M2" r:id="rId1" display="Izutsu (Wiley 2009)" xr:uid="{3CE65C60-DA75-4595-8CAA-88F2C9A358C9}"/>
+    <hyperlink ref="M3" r:id="rId2" display="Izutsu (Wiley 2009)" xr:uid="{6B0DA7F9-0782-4596-8B42-F9EBE5175294}"/>
+    <hyperlink ref="M4" r:id="rId3" display="Izutsu (Wiley 2009)" xr:uid="{55B29BD6-B10F-4DCF-93BE-7B2953D8D605}"/>
+    <hyperlink ref="M5" r:id="rId4" display="Izutsu (Wiley 2009)" xr:uid="{A3AEBAE1-B668-4BB3-9056-8F0FA6D1359D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -5349,10 +5429,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8976AAB6-E21A-42F8-BEF8-70CDE446E133}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5363,9 +5443,10 @@
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>157</v>
       </c>
@@ -5376,15 +5457,15 @@
         <v>159</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B2" s="9">
         <v>341.91</v>
@@ -5393,17 +5474,20 @@
         <v>10</v>
       </c>
       <c r="D2" s="58">
-        <f>AVERAGE(5.69,3.34,2.36,1.59)/1000</f>
-        <v>3.2450000000000001E-3</v>
+        <f>5.69/1000</f>
+        <v>5.6900000000000006E-3</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B3" s="9">
         <v>229.74</v>
@@ -5412,15 +5496,14 @@
         <v>10</v>
       </c>
       <c r="D3" s="58">
-        <f>3/5*1000/1000000*0.3*172.3*(1-2.08*SQRT(0.3)+2.4*(0.3))</f>
-        <v>1.8010979811192335E-2</v>
+        <f>1000/1000000*0.3*172.3*(1-2.08*SQRT(0.3)+2.4*(0.3))</f>
+        <v>3.0018299685320562E-2</v>
       </c>
       <c r="E3" s="22"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B4" s="9">
         <v>329.27</v>
@@ -5429,15 +5512,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="40">
-        <f>3/5*1000/1000000*0.3*172.3*(1-2.08*SQRT(0.3)+2.4*(0.3))</f>
-        <v>1.8010979811192335E-2</v>
+        <f>1000/1000000*0.3*172.3*(1-2.08*SQRT(0.3)+2.4*(0.3))</f>
+        <v>3.0018299685320562E-2</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="65"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B5" s="9">
         <v>165.74</v>
@@ -5446,8 +5529,8 @@
         <v>10</v>
       </c>
       <c r="D5" s="58">
-        <f>3/5*1000/1000000*0.3*169.6*(1-2.1*SQRT(0.3)+10*(0.3))</f>
-        <v>8.6998164105412792E-2</v>
+        <f>1000/1000000*0.3*169.6*(1-2.1*SQRT(0.3)+10*(0.3))</f>
+        <v>0.14499694017568801</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="65"/>
@@ -5577,7 +5660,7 @@
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated rate of solvent loss
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2058" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6067A9E6-005E-4C4B-BC70-A6B3534049B6}"/>
+  <xr:revisionPtr revIDLastSave="2065" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F6427A4-2FA9-4A2B-9296-5CAB2FCB92C5}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="15990" windowHeight="15585" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="2265" yWindow="2595" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -1665,7 +1665,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1818,12 +1818,6 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Nova"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4052,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="B16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4206,8 +4200,8 @@
         <v>167</v>
       </c>
       <c r="C8" s="23">
-        <f>1989043*800/596.2</f>
-        <v>2668960.7514256961</v>
+        <f>1.3*1989043*800/596.2</f>
+        <v>3469648.9768534047</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>168</v>
@@ -4816,9 +4810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J3" sqref="J3"/>
+      <selection pane="topRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5152,8 +5146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4385D70-1AE4-4A35-988B-BBC4298D1C90}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5291,7 +5285,7 @@
         <v>50</v>
       </c>
       <c r="K3" s="63">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="L3" s="57" t="s">
         <v>195</v>
@@ -5337,7 +5331,7 @@
         <v>84</v>
       </c>
       <c r="K4" s="63">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>194</v>

</xml_diff>

<commit_message>
Updated solvent conductivity data
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Non-aqueous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2065" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F6427A4-2FA9-4A2B-9296-5CAB2FCB92C5}"/>
+  <xr:revisionPtr revIDLastSave="2169" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{953E0BFD-604D-4FE7-A6BC-7C55099AAECB}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2595" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="4" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -217,6 +217,7 @@
     <author>tc={F67C249D-9E0C-448B-A8C7-01734972A047}</author>
     <author>tc={1A47F35F-C8C5-428F-B841-B07DB6CB6586}</author>
     <author>tc={1F00EE09-7981-4B53-A2FE-8E9564200CBF}</author>
+    <author>tc={0A555575-C1EC-476A-AE97-9AC131832B8A}</author>
     <author>tc={CCFAFA67-1AB3-4E10-B472-4734839B5FB8}</author>
     <author>tc={7E768D53-988A-46AE-8800-331D2B19C4CA}</author>
     <author>tc={F72D791D-203F-48D2-BBE6-FB8C410089E4}</author>
@@ -227,22 +228,24 @@
     <author>tc={44C8D15E-D18E-42F7-B8B2-A65CC53CBB8C}</author>
     <author>tc={8C14FDD1-22B7-4F70-B01E-C665917CE3E4}</author>
     <author>tc={0182AE5B-5F63-4940-956C-D441191E1036}</author>
+    <author>tc={918158CC-13D0-4406-9FA6-83AE98F2FB61}</author>
+    <author>tc={5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}</author>
+    <author>tc={7EC05627-69D0-4FD7-BD41-0D34F6398A4A}</author>
+    <author>tc={86D5D7AE-BF34-4CC2-BAB5-EB71EAF53309}</author>
+    <author>tc={3A5F5CB1-C285-495B-87E8-AE2A789DD37B}</author>
+    <author>tc={46A38827-0DE9-44F3-AF17-F0D80DDB9CEE}</author>
+    <author>tc={4E6C45D9-A547-4A85-8E31-46455E39B2F7}</author>
+    <author>tc={C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}</author>
+    <author>tc={699871B5-28D8-4F74-810A-11C06F2FFAC4}</author>
     <author>tc={DD06A995-3E0B-473D-8CCE-79C9FDD92985}</author>
     <author>tc={BF97B819-C241-44FC-AA8D-937FDD0CF315}</author>
     <author>tc={24A6F79D-F1B1-486E-8E16-0DF2EB3ECD76}</author>
     <author>tc={3E35980D-20DB-4345-B9FE-BEA0317F7EBB}</author>
     <author>tc={A557D283-8D16-4ED2-AC97-8D87D241B088}</author>
+    <author>tc={82FB6557-34EB-402A-8FFE-EEA21AD195C0}</author>
     <author>tc={1983A994-3FCC-4917-A080-32AC954B27A3}</author>
     <author>tc={F163D6D5-0931-443B-A93F-1C0E825E55FE}</author>
     <author>tc={5EA6F35C-447A-4F92-B17C-594D64D62197}</author>
-    <author>tc={918158CC-13D0-4406-9FA6-83AE98F2FB61}</author>
-    <author>tc={5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}</author>
-    <author>tc={7EC05627-69D0-4FD7-BD41-0D34F6398A4A}</author>
-    <author>tc={86D5D7AE-BF34-4CC2-BAB5-EB71EAF53309}</author>
-    <author>tc={3A5F5CB1-C285-495B-87E8-AE2A789DD37B}</author>
-    <author>tc={4E6C45D9-A547-4A85-8E31-46455E39B2F7}</author>
-    <author>tc={C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}</author>
-    <author>tc={699871B5-28D8-4F74-810A-11C06F2FFAC4}</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{E5AC3F3D-5F46-4C07-9B89-304D65BB0E75}">
@@ -289,15 +292,23 @@
     https://doi.org/10.1016/0022-0728(90)87217-8 60.7</t>
       </text>
     </comment>
-    <comment ref="I2" authorId="5" shapeId="0" xr:uid="{CCFAFA67-1AB3-4E10-B472-4734839B5FB8}">
+    <comment ref="G2" authorId="5" shapeId="0" xr:uid="{0A555575-C1EC-476A-AE97-9AC131832B8A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
+    Schmelzer Farad Soc Trans 1990; Emerson manual https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf</t>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="6" shapeId="0" xr:uid="{CCFAFA67-1AB3-4E10-B472-4734839B5FB8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="J2" authorId="6" shapeId="0" xr:uid="{7E768D53-988A-46AE-8800-331D2B19C4CA}">
+    <comment ref="J2" authorId="7" shapeId="0" xr:uid="{7E768D53-988A-46AE-8800-331D2B19C4CA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -305,7 +316,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="L2" authorId="7" shapeId="0" xr:uid="{F72D791D-203F-48D2-BBE6-FB8C410089E4}">
+    <comment ref="L2" authorId="8" shapeId="0" xr:uid="{F72D791D-203F-48D2-BBE6-FB8C410089E4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -313,7 +324,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="B3" authorId="8" shapeId="0" xr:uid="{46705330-D6EB-4863-A1A8-B104F2E8D6B3}">
+    <comment ref="B3" authorId="9" shapeId="0" xr:uid="{46705330-D6EB-4863-A1A8-B104F2E8D6B3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -321,7 +332,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="C3" authorId="9" shapeId="0" xr:uid="{168996AD-382A-4647-91D8-9337C1109D7E}">
+    <comment ref="C3" authorId="10" shapeId="0" xr:uid="{168996AD-382A-4647-91D8-9337C1109D7E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -329,7 +340,7 @@
     https://www.imarcgroup.com/propylene-carbonate-pricing-report</t>
       </text>
     </comment>
-    <comment ref="D3" authorId="10" shapeId="0" xr:uid="{64FBC311-9AC9-4A86-9F4C-B513D1E820CD}">
+    <comment ref="D3" authorId="11" shapeId="0" xr:uid="{64FBC311-9AC9-4A86-9F4C-B513D1E820CD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -337,7 +348,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="E3" authorId="11" shapeId="0" xr:uid="{03642210-2394-46F4-A4C6-05E5974668C8}">
+    <comment ref="E3" authorId="12" shapeId="0" xr:uid="{03642210-2394-46F4-A4C6-05E5974668C8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -345,7 +356,7 @@
     Izutsu 2009 Table 1.1</t>
       </text>
     </comment>
-    <comment ref="F3" authorId="12" shapeId="0" xr:uid="{44C8D15E-D18E-42F7-B8B2-A65CC53CBB8C}">
+    <comment ref="F3" authorId="13" shapeId="0" xr:uid="{44C8D15E-D18E-42F7-B8B2-A65CC53CBB8C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -353,7 +364,7 @@
     https://doi.org/10.1016/0378-3812(88)80106-7</t>
       </text>
     </comment>
-    <comment ref="I3" authorId="13" shapeId="0" xr:uid="{8C14FDD1-22B7-4F70-B01E-C665917CE3E4}">
+    <comment ref="I3" authorId="14" shapeId="0" xr:uid="{8C14FDD1-22B7-4F70-B01E-C665917CE3E4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -361,7 +372,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="J3" authorId="14" shapeId="0" xr:uid="{0182AE5B-5F63-4940-956C-D441191E1036}">
+    <comment ref="J3" authorId="15" shapeId="0" xr:uid="{0182AE5B-5F63-4940-956C-D441191E1036}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -369,7 +380,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="B4" authorId="15" shapeId="0" xr:uid="{DD06A995-3E0B-473D-8CCE-79C9FDD92985}">
+    <comment ref="B4" authorId="16" shapeId="0" xr:uid="{918158CC-13D0-4406-9FA6-83AE98F2FB61}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -377,74 +388,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="C4" authorId="16" shapeId="0" xr:uid="{BF97B819-C241-44FC-AA8D-937FDD0CF315}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    https://www.imarcgroup.com/dimethyl-sulfoxide-pricing-report
-</t>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="17" shapeId="0" xr:uid="{24A6F79D-F1B1-486E-8E16-0DF2EB3ECD76}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CRC Handbook of Chem and Phys 105th Ed.</t>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="18" shapeId="0" xr:uid="{3E35980D-20DB-4345-B9FE-BEA0317F7EBB}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CRC Handbook of Chem and Phys 105th Ed.</t>
-      </text>
-    </comment>
-    <comment ref="F4" authorId="19" shapeId="0" xr:uid="{A557D283-8D16-4ED2-AC97-8D87D241B088}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Table 3 in https://www.sciencedirect.com/science/article/pii/S0021961419306883#f0030
-Reply:
-    https://doi.org/10.1016/0022-0728(90)87217-8 101.6</t>
-      </text>
-    </comment>
-    <comment ref="I4" authorId="20" shapeId="0" xr:uid="{1983A994-3FCC-4917-A080-32AC954B27A3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CRC Handbook of Chem and Phys 105th Ed.</t>
-      </text>
-    </comment>
-    <comment ref="J4" authorId="21" shapeId="0" xr:uid="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CRC Handbook of Chem and Phys 105th Ed.</t>
-      </text>
-    </comment>
-    <comment ref="L4" authorId="22" shapeId="0" xr:uid="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CRC Handbook of Chem and Phys 105th Ed.</t>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="23" shapeId="0" xr:uid="{918158CC-13D0-4406-9FA6-83AE98F2FB61}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CRC Handbook of Chem and Phys 105th Ed.</t>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="24" shapeId="0" xr:uid="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
+    <comment ref="C4" authorId="17" shapeId="0" xr:uid="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -456,7 +400,7 @@
     Averaged the above roughly</t>
       </text>
     </comment>
-    <comment ref="D5" authorId="25" shapeId="0" xr:uid="{7EC05627-69D0-4FD7-BD41-0D34F6398A4A}">
+    <comment ref="D4" authorId="18" shapeId="0" xr:uid="{7EC05627-69D0-4FD7-BD41-0D34F6398A4A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -464,7 +408,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="E5" authorId="26" shapeId="0" xr:uid="{86D5D7AE-BF34-4CC2-BAB5-EB71EAF53309}">
+    <comment ref="E4" authorId="19" shapeId="0" xr:uid="{86D5D7AE-BF34-4CC2-BAB5-EB71EAF53309}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -472,7 +416,7 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="F5" authorId="27" shapeId="0" xr:uid="{3A5F5CB1-C285-495B-87E8-AE2A789DD37B}">
+    <comment ref="F4" authorId="20" shapeId="0" xr:uid="{3A5F5CB1-C285-495B-87E8-AE2A789DD37B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -480,15 +424,23 @@
     https://doi.org/10.1016/0022-0728(90)87217-8 65.3</t>
       </text>
     </comment>
-    <comment ref="I5" authorId="28" shapeId="0" xr:uid="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
+    <comment ref="G4" authorId="21" shapeId="0" xr:uid="{46A38827-0DE9-44F3-AF17-F0D80DDB9CEE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
+    Schmelzer Farad Soc Trans 1990; Shinkle Monroe J Power Sources 2014</t>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="22" shapeId="0" xr:uid="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="J5" authorId="29" shapeId="0" xr:uid="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
+    <comment ref="J4" authorId="23" shapeId="0" xr:uid="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -496,7 +448,82 @@
     CRC Handbook of Chem and Phys 105th Ed.</t>
       </text>
     </comment>
-    <comment ref="L5" authorId="30" shapeId="0" xr:uid="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
+    <comment ref="L4" authorId="24" shapeId="0" xr:uid="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CRC Handbook of Chem and Phys 105th Ed.</t>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="25" shapeId="0" xr:uid="{DD06A995-3E0B-473D-8CCE-79C9FDD92985}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CRC Handbook of Chem and Phys 105th Ed.</t>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="26" shapeId="0" xr:uid="{BF97B819-C241-44FC-AA8D-937FDD0CF315}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.imarcgroup.com/dimethyl-sulfoxide-pricing-report
+</t>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="27" shapeId="0" xr:uid="{24A6F79D-F1B1-486E-8E16-0DF2EB3ECD76}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CRC Handbook of Chem and Phys 105th Ed.</t>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="28" shapeId="0" xr:uid="{3E35980D-20DB-4345-B9FE-BEA0317F7EBB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CRC Handbook of Chem and Phys 105th Ed.</t>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="29" shapeId="0" xr:uid="{A557D283-8D16-4ED2-AC97-8D87D241B088}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Table 3 in https://www.sciencedirect.com/science/article/pii/S0021961419306883#f0030
+Reply:
+    https://doi.org/10.1016/0022-0728(90)87217-8 101.6</t>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="30" shapeId="0" xr:uid="{82FB6557-34EB-402A-8FFE-EEA21AD195C0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Schmelzer Farad Soc Trans 1990; Emerson manual https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf</t>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="31" shapeId="0" xr:uid="{1983A994-3FCC-4917-A080-32AC954B27A3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CRC Handbook of Chem and Phys 105th Ed.</t>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="32" shapeId="0" xr:uid="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CRC Handbook of Chem and Phys 105th Ed.</t>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="33" shapeId="0" xr:uid="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -512,13 +539,17 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={07BD2C0B-3DD0-40BC-AD52-A79697FDE249}</author>
-    <author>tc={12C0EC02-9084-4697-8B56-C3293339F20B}</author>
+    <author>tc={43B59BBE-E29D-41F7-8430-AA47C246E708}</author>
+    <author>tc={8D382F3B-8433-4D50-AD8B-3CDB4C5E2091}</author>
     <author>tc={18ECACC2-E30B-407C-B2EF-2D02470F19E2}</author>
     <author>tc={224EC866-413C-4C24-91AC-D4B821D21361}</author>
+    <author>tc={99B3EF73-D9AF-4165-9BAA-2D78D6A936A3}</author>
     <author>tc={2EA54DCB-79E7-4A67-94B1-01E68FDD14D9}</author>
-    <author>tc={24EDBDE4-89F6-4893-A249-65F70D6F4EB5}</author>
+    <author>tc={E8DB58D9-FECA-44B0-A45F-2D6CD01B8C82}</author>
+    <author>tc={BCA5F20C-1DCE-4C25-8CA7-13042C65B6D7}</author>
     <author>tc={FE69842F-8058-427E-A379-A3530412D42F}</author>
     <author>tc={D8A725FE-F27F-4CE0-B881-3504A580D1E3}</author>
+    <author>tc={47E6C014-E881-40B4-899B-38C111AE0A6F}</author>
   </authors>
   <commentList>
     <comment ref="C2" authorId="0" shapeId="0" xr:uid="{07BD2C0B-3DD0-40BC-AD52-A79697FDE249}">
@@ -531,15 +562,23 @@
     https://pubs.acs.org/doi/10.1021/acssuschemeng.0c03061 $10-40 / kg IL (AHAs)</t>
       </text>
     </comment>
-    <comment ref="D2" authorId="1" shapeId="0" xr:uid="{12C0EC02-9084-4697-8B56-C3293339F20B}">
+    <comment ref="D2" authorId="1" shapeId="0" xr:uid="{43B59BBE-E29D-41F7-8430-AA47C246E708}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Darling Brushett Energy Env Sci 2014, 0.1 M, averaging all solvents</t>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="2" shapeId="0" xr:uid="{18ECACC2-E30B-407C-B2EF-2D02470F19E2}">
+    Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</t>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="2" shapeId="0" xr:uid="{8D382F3B-8433-4D50-AD8B-3CDB4C5E2091}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</t>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="3" shapeId="0" xr:uid="{18ECACC2-E30B-407C-B2EF-2D02470F19E2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -549,17 +588,23 @@
     https://pubs.acs.org/doi/10.1021/acssuschemeng.0c03061 $10-40 / kg IL (AHAs)</t>
       </text>
     </comment>
-    <comment ref="D3" authorId="3" shapeId="0" xr:uid="{224EC866-413C-4C24-91AC-D4B821D21361}">
+    <comment ref="D3" authorId="4" shapeId="0" xr:uid="{224EC866-413C-4C24-91AC-D4B821D21361}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf - Pr4NClO4 in ACN
-Reply:
-    Factor of ⅗ to correct for multiple solvents being averaged</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="4" shapeId="0" xr:uid="{2EA54DCB-79E7-4A67-94B1-01E68FDD14D9}">
+    Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</t>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="5" shapeId="0" xr:uid="{99B3EF73-D9AF-4165-9BAA-2D78D6A936A3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="6" shapeId="0" xr:uid="{2EA54DCB-79E7-4A67-94B1-01E68FDD14D9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -569,17 +614,25 @@
     https://pubs.acs.org/doi/10.1021/acssuschemeng.0c03061 $10-40 / kg IL (AHAs)</t>
       </text>
     </comment>
-    <comment ref="D4" authorId="5" shapeId="0" xr:uid="{24EDBDE4-89F6-4893-A249-65F70D6F4EB5}">
+    <comment ref="D4" authorId="7" shapeId="0" xr:uid="{E8DB58D9-FECA-44B0-A45F-2D6CD01B8C82}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf - Pr4NClO4 in ACN
-Reply:
-    Factor of ⅗ to correct for multiple solvents being averaged</t>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="6" shapeId="0" xr:uid="{FE69842F-8058-427E-A379-A3530412D42F}">
+    Ue Mori JECS 1994 - https://iopscience.iop.org/article/10.1149/1.2059270
+In DMF and ACN, 0.1 M: Shinkle Monroe J Power Sources 2014 -https://doi.org/10.1016/j.jpowsour.2013.10.034
+In PC, any concentration: Ue Mori JECS 1994 - https://iopscience.iop.org/article/10.1149/1.2059270</t>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="8" shapeId="0" xr:uid="{BCA5F20C-1DCE-4C25-8CA7-13042C65B6D7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Gong Yan EES 2015 - https://doi.org/10.1039/C5EE02341F</t>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="9" shapeId="0" xr:uid="{FE69842F-8058-427E-A379-A3530412D42F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -589,7 +642,7 @@
     https://pubs.acs.org/doi/10.1021/acssuschemeng.0c03061 $10-40 / kg IL (AHAs)</t>
       </text>
     </comment>
-    <comment ref="D5" authorId="7" shapeId="0" xr:uid="{D8A725FE-F27F-4CE0-B881-3504A580D1E3}">
+    <comment ref="D5" authorId="10" shapeId="0" xr:uid="{D8A725FE-F27F-4CE0-B881-3504A580D1E3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -597,6 +650,14 @@
     https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf - Pr4NI in ACN
 Reply:
     Factor of ⅗ to correct for multiple solvents being averaged</t>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="11" shapeId="0" xr:uid="{47E6C014-E881-40B4-899B-38C111AE0A6F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</t>
       </text>
     </comment>
   </commentList>
@@ -604,7 +665,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="205">
   <si>
     <t>Utility</t>
   </si>
@@ -1349,9 +1410,6 @@
     <t>Chemours 2024; Nafion N117 180 um</t>
   </si>
   <si>
-    <t>Tried Pathania et al, but gives very high conductivity</t>
-  </si>
-  <si>
     <t>Acetonitrile</t>
   </si>
   <si>
@@ -1609,9 +1667,6 @@
     </r>
   </si>
   <si>
-    <t>Izutsu (Wiley 2009); CRC Handbook</t>
-  </si>
-  <si>
     <t>Soluble</t>
   </si>
   <si>
@@ -1622,9 +1677,6 @@
   </si>
   <si>
     <t>TEACl</t>
-  </si>
-  <si>
-    <t>Others: THF, DME, acetone, sulfolane</t>
   </si>
   <si>
     <t>TBAClO$_4$</t>
@@ -1644,16 +1696,37 @@
 CEPCI 2024: ~800 (https://toweringskills.com/financial-analysis/cost-indices/)</t>
   </si>
   <si>
-    <t>Conductivity in ACN, 0.3 M (S/cm)</t>
-  </si>
-  <si>
-    <t>Conductivity factor relative to ACN</t>
-  </si>
-  <si>
-    <t>JM's estimate: 0.010 - 0.020 S/cm</t>
-  </si>
-  <si>
     <t>Optimal j @ 8.2 c/kWh, no tradeoff (mA/cm2)</t>
+  </si>
+  <si>
+    <t>Conductivity in PC, 0.3 M (S/cm)</t>
+  </si>
+  <si>
+    <t>Conductivity factor relative to PC</t>
+  </si>
+  <si>
+    <r>
+      <t>Limiting molar conductivity in PC (S cm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Nova"/>
+        <family val="2"/>
+      </rPr>
+      <t>/mol)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1665,7 +1738,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1820,6 +1893,12 @@
       <name val="Arial Nova"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1841,7 +1920,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1967,17 +2046,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2096,9 +2164,6 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2150,9 +2215,6 @@
     <xf numFmtId="2" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2162,14 +2224,20 @@
     <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2186,6 +2254,26 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="54">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial Nova"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2351,14 +2439,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3369,22 +3449,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}" name="Products6" displayName="Products6" ref="A1:M5" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:M5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}" name="Products6" displayName="Products6" ref="A1:L5" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:L5" xr:uid="{FDE89AE4-9617-4085-AD63-8D726E2ECE27}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{996983E7-48A1-4F2C-AAE8-BB6499F82011}" name="Solvent" dataDxfId="25"/>
     <tableColumn id="5" xr3:uid="{7587D408-6B96-4220-A9BE-2B71A4248C30}" name="Molecular weight (g/mol)" dataDxfId="24"/>
     <tableColumn id="14" xr3:uid="{8CB95F86-8F61-4051-8BEA-3EA0B1243627}" name="Cost ($/kg solvent)" dataDxfId="23"/>
     <tableColumn id="3" xr3:uid="{CCFBA968-B535-4D6B-82F9-71090461EE43}" name="Density (kg/m3)" dataDxfId="22"/>
     <tableColumn id="4" xr3:uid="{6DE0BEDB-FDAC-4FA2-8AC5-B102FC6EEC22}" name="Viscosity (cP)" dataDxfId="21"/>
     <tableColumn id="11" xr3:uid="{7E968132-802A-4590-8623-AF835C5600CC}" name="Henry's constant at 298K, CO2 (mole fraction/atm)" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{C14326B4-157A-4FBF-9FD5-58F36F9782B3}" name="Conductivity factor relative to ACN" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{C14326B4-157A-4FBF-9FD5-58F36F9782B3}" name="Conductivity factor relative to PC" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{4B98493F-7EF6-4DC3-A55A-0A71F419BBB2}" name="CO2 solubility, 10 bar (mol CO2/ mol solvent)" dataDxfId="18"/>
     <tableColumn id="6" xr3:uid="{1008D39B-F74C-44B5-9C39-9094D52EB44D}" name="Boiling point (K)" dataDxfId="17"/>
     <tableColumn id="9" xr3:uid="{4E983CB5-D8FE-442A-8A07-6298EE4689D9}" name="Vapor pressure (Pa)" dataDxfId="16"/>
     <tableColumn id="10" xr3:uid="{57E55551-0CF1-45DA-9F74-4502CD642FB0}" name="Solvent loss fraction ((mol/s offgas)/ (mol/s solvent))" dataDxfId="15"/>
     <tableColumn id="8" xr3:uid="{57ADEF7D-1DC8-4D29-B0B1-B07EDD74B7FC}" name="Solubility in water" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{A94104E3-BA24-4CBD-8D8E-9581768AC69A}" name="References"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3397,21 +3476,21 @@
     <tableColumn id="1" xr3:uid="{5E12D873-28F4-4BAA-A124-01ED2F10306F}" name="Supporting electrolyte" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{8BFB1102-BA9E-4FA2-8287-970DFEAD7F45}" name="Molecular weight (g/mol)" dataDxfId="10"/>
     <tableColumn id="14" xr3:uid="{40345891-0EC3-4D4A-9A2E-09812C6C59BF}" name="Cost ($/kg supporting)" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{580C116E-F5E0-41C5-8884-D2C8E1385F89}" name="Conductivity in ACN, 0.3 M (S/cm)" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{BF9F5B6E-2598-43D5-ABA7-189814842EF4}" name="References" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{580C116E-F5E0-41C5-8884-D2C8E1385F89}" name="Conductivity in PC, 0.3 M (S/cm)" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{71DE59C7-7F1E-4C7B-9873-8A66974BE6BD}" name="Limiting molar conductivity in PC (S cm2/mol)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F90A0C8F-F9A6-4BD9-BE38-37BCD437C167}" name="Utility_sources" displayName="Utility_sources" ref="A1:D14" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F90A0C8F-F9A6-4BD9-BE38-37BCD437C167}" name="Utility_sources" displayName="Utility_sources" ref="A1:D14" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:D14" xr:uid="{F90A0C8F-F9A6-4BD9-BE38-37BCD437C167}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{019A737E-EC43-437D-A256-C18EEEE61274}" name="Utility" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{339E3BF5-AD63-4805-BC84-16828025960D}" name="Cost ($/kWh)" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{5BD4A003-8709-44FE-A299-AB3C44A1C92B}" name="CO2 emissions (g CO2/kWh)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{106C8FDA-1A54-408F-9E45-6177A2EA926F}" name="References" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{019A737E-EC43-437D-A256-C18EEEE61274}" name="Utility" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{339E3BF5-AD63-4805-BC84-16828025960D}" name="Cost ($/kWh)" dataDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{5BD4A003-8709-44FE-A299-AB3C44A1C92B}" name="CO2 emissions (g CO2/kWh)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{106C8FDA-1A54-408F-9E45-6177A2EA926F}" name="References" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3811,6 +3890,15 @@
       </x:ext>
     </extLst>
   </threadedComment>
+  <threadedComment ref="G2" dT="2025-02-27T00:04:38.96" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{0A555575-C1EC-476A-AE97-9AC131832B8A}">
+    <text>Schmelzer Farad Soc Trans 1990; Emerson manual https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>2220198763</xltc2:checksum>
+        <xltc2:hyperlink startIndex="47" length="119" url="https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
   <threadedComment ref="I2" dT="2025-01-20T21:27:20.62" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{CCFAFA67-1AB3-4E10-B472-4734839B5FB8}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
@@ -3853,10 +3941,61 @@
   <threadedComment ref="J3" dT="2025-01-20T21:27:38.80" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{0182AE5B-5F63-4940-956C-D441191E1036}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="B4" dT="2025-01-20T21:26:24.25" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{DD06A995-3E0B-473D-8CCE-79C9FDD92985}">
+  <threadedComment ref="B4" dT="2025-01-20T21:26:28.19" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{918158CC-13D0-4406-9FA6-83AE98F2FB61}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="C4" dT="2024-12-03T18:29:32.47" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{BF97B819-C241-44FC-AA8D-937FDD0CF315}">
+  <threadedComment ref="C4" dT="2025-01-15T16:55:54.83" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
+    <text>https://businessanalytiq.com/procurementanalytics/index/dimethylformamide-dmf-price-index/</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>2903401631</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="90" url="https://businessanalytiq.com/procurementanalytics/index/dimethylformamide-dmf-price-index/"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="C4" dT="2025-01-15T16:57:54.36" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{2116F162-FBCC-4461-8DF2-BA5FD59EB428}" parentId="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
+    <text>https://www.procurementresource.com/resource-center/dmf-dimethylformamide-price-trends</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3253514027</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="86" url="https://www.procurementresource.com/resource-center/dmf-dimethylformamide-price-trends"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="C4" dT="2025-01-15T16:58:00.41" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{0F76214F-3170-4DB8-9A38-572C212649EE}" parentId="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
+    <text>Averaged the above roughly</text>
+  </threadedComment>
+  <threadedComment ref="D4" dT="2025-01-20T21:27:00.06" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{7EC05627-69D0-4FD7-BD41-0D34F6398A4A}">
+    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
+  </threadedComment>
+  <threadedComment ref="E4" dT="2025-01-20T21:27:11.44" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{86D5D7AE-BF34-4CC2-BAB5-EB71EAF53309}">
+    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
+  </threadedComment>
+  <threadedComment ref="F4" dT="2025-01-20T21:04:12.01" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{3A5F5CB1-C285-495B-87E8-AE2A789DD37B}">
+    <text>https://doi.org/10.1016/0022-0728(90)87217-8 65.3</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>693612592</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="44" url="https://doi.org/10.1016/0022-0728(90)87217-8"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="G4" dT="2025-02-27T00:06:38.71" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{46A38827-0DE9-44F3-AF17-F0D80DDB9CEE}">
+    <text>Schmelzer Farad Soc Trans 1990; Shinkle Monroe J Power Sources 2014</text>
+  </threadedComment>
+  <threadedComment ref="I4" dT="2025-01-20T21:27:30.00" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
+    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
+  </threadedComment>
+  <threadedComment ref="J4" dT="2025-01-20T21:27:46.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
+    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
+  </threadedComment>
+  <threadedComment ref="L4" dT="2025-01-20T21:27:59.71" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
+    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
+  </threadedComment>
+  <threadedComment ref="B5" dT="2025-01-20T21:26:24.25" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{DD06A995-3E0B-473D-8CCE-79C9FDD92985}">
+    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
+  </threadedComment>
+  <threadedComment ref="C5" dT="2024-12-03T18:29:32.47" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{BF97B819-C241-44FC-AA8D-937FDD0CF315}">
     <text xml:space="preserve">https://www.imarcgroup.com/dimethyl-sulfoxide-pricing-report
 </text>
     <extLst>
@@ -3866,13 +4005,13 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="D4" dT="2025-01-20T21:26:45.46" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{24A6F79D-F1B1-486E-8E16-0DF2EB3ECD76}">
+  <threadedComment ref="D5" dT="2025-01-20T21:26:45.46" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{24A6F79D-F1B1-486E-8E16-0DF2EB3ECD76}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="E4" dT="2025-01-20T21:27:07.86" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{3E35980D-20DB-4345-B9FE-BEA0317F7EBB}">
+  <threadedComment ref="E5" dT="2025-01-20T21:27:07.86" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{3E35980D-20DB-4345-B9FE-BEA0317F7EBB}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="F4" dT="2025-01-20T20:26:40.91" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{A557D283-8D16-4ED2-AC97-8D87D241B088}">
+  <threadedComment ref="F5" dT="2025-01-20T20:26:40.91" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{A557D283-8D16-4ED2-AC97-8D87D241B088}">
     <text>Table 3 in https://www.sciencedirect.com/science/article/pii/S0021961419306883#f0030</text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
@@ -3881,7 +4020,7 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="F4" dT="2025-01-20T21:03:59.74" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{ED490485-EB49-40FD-819B-2FFEDC862A79}" parentId="{A557D283-8D16-4ED2-AC97-8D87D241B088}">
+  <threadedComment ref="F5" dT="2025-01-20T21:03:59.74" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{ED490485-EB49-40FD-819B-2FFEDC862A79}" parentId="{A557D283-8D16-4ED2-AC97-8D87D241B088}">
     <text>https://doi.org/10.1016/0022-0728(90)87217-8 101.6</text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
@@ -3890,61 +4029,22 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="I4" dT="2025-01-20T21:27:27.28" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{1983A994-3FCC-4917-A080-32AC954B27A3}">
-    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
-  </threadedComment>
-  <threadedComment ref="J4" dT="2025-01-20T21:27:42.09" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
-    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
-  </threadedComment>
-  <threadedComment ref="L4" dT="2025-01-20T21:27:55.05" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
-    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
-  </threadedComment>
-  <threadedComment ref="B5" dT="2025-01-20T21:26:28.19" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{918158CC-13D0-4406-9FA6-83AE98F2FB61}">
-    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
-  </threadedComment>
-  <threadedComment ref="C5" dT="2025-01-15T16:55:54.83" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
-    <text>https://businessanalytiq.com/procurementanalytics/index/dimethylformamide-dmf-price-index/</text>
+  <threadedComment ref="G5" dT="2025-02-27T00:07:09.07" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{82FB6557-34EB-402A-8FFE-EEA21AD195C0}">
+    <text>Schmelzer Farad Soc Trans 1990; Emerson manual https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf</text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>2903401631</xltc2:checksum>
-        <xltc2:hyperlink startIndex="0" length="90" url="https://businessanalytiq.com/procurementanalytics/index/dimethylformamide-dmf-price-index/"/>
+        <xltc2:checksum>2220198763</xltc2:checksum>
+        <xltc2:hyperlink startIndex="47" length="119" url="https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf"/>
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="C5" dT="2025-01-15T16:57:54.36" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{2116F162-FBCC-4461-8DF2-BA5FD59EB428}" parentId="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
-    <text>https://www.procurementresource.com/resource-center/dmf-dimethylformamide-price-trends</text>
-    <extLst>
-      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>3253514027</xltc2:checksum>
-        <xltc2:hyperlink startIndex="0" length="86" url="https://www.procurementresource.com/resource-center/dmf-dimethylformamide-price-trends"/>
-      </x:ext>
-    </extLst>
-  </threadedComment>
-  <threadedComment ref="C5" dT="2025-01-15T16:58:00.41" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{0F76214F-3170-4DB8-9A38-572C212649EE}" parentId="{5D6620EE-D7DA-4BD1-9DEC-F1DFA3B16F63}">
-    <text>Averaged the above roughly</text>
-  </threadedComment>
-  <threadedComment ref="D5" dT="2025-01-20T21:27:00.06" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{7EC05627-69D0-4FD7-BD41-0D34F6398A4A}">
+  <threadedComment ref="I5" dT="2025-01-20T21:27:27.28" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{1983A994-3FCC-4917-A080-32AC954B27A3}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="E5" dT="2025-01-20T21:27:11.44" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{86D5D7AE-BF34-4CC2-BAB5-EB71EAF53309}">
+  <threadedComment ref="J5" dT="2025-01-20T21:27:42.09" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{F163D6D5-0931-443B-A93F-1C0E825E55FE}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
-  <threadedComment ref="F5" dT="2025-01-20T21:04:12.01" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{3A5F5CB1-C285-495B-87E8-AE2A789DD37B}">
-    <text>https://doi.org/10.1016/0022-0728(90)87217-8 65.3</text>
-    <extLst>
-      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>693612592</xltc2:checksum>
-        <xltc2:hyperlink startIndex="0" length="44" url="https://doi.org/10.1016/0022-0728(90)87217-8"/>
-      </x:ext>
-    </extLst>
-  </threadedComment>
-  <threadedComment ref="I5" dT="2025-01-20T21:27:30.00" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{4E6C45D9-A547-4A85-8E31-46455E39B2F7}">
-    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
-  </threadedComment>
-  <threadedComment ref="J5" dT="2025-01-20T21:27:46.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{C9E7B65A-8DF8-424A-AFB0-85F34FB8C5A3}">
-    <text>CRC Handbook of Chem and Phys 105th Ed.</text>
-  </threadedComment>
-  <threadedComment ref="L5" dT="2025-01-20T21:27:59.71" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{699871B5-28D8-4F74-810A-11C06F2FFAC4}">
+  <threadedComment ref="L5" dT="2025-01-20T21:27:55.05" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{5EA6F35C-447A-4F92-B17C-594D64D62197}">
     <text>CRC Handbook of Chem and Phys 105th Ed.</text>
   </threadedComment>
 </ThreadedComments>
@@ -3964,8 +4064,23 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="D2" dT="2025-01-31T15:34:56.24" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{12C0EC02-9084-4697-8B56-C3293339F20B}">
-    <text>Darling Brushett Energy Env Sci 2014, 0.1 M, averaging all solvents</text>
+  <threadedComment ref="D2" dT="2025-02-26T22:01:55.36" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{43B59BBE-E29D-41F7-8430-AA47C246E708}">
+    <text>Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>1714132109</xltc2:checksum>
+        <xltc2:hyperlink startIndex="35" length="49" url="https://pubs.acs.org/doi/epdf/10.1021/j100845a068"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="E2" dT="2025-02-26T23:57:34.23" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{8D382F3B-8433-4D50-AD8B-3CDB4C5E2091}">
+    <text>Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>1714132109</xltc2:checksum>
+        <xltc2:hyperlink startIndex="35" length="49" url="https://pubs.acs.org/doi/epdf/10.1021/j100845a068"/>
+      </x:ext>
+    </extLst>
   </threadedComment>
   <threadedComment ref="C3" dT="2024-11-11T22:11:30.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{18ECACC2-E30B-407C-B2EF-2D02470F19E2}">
     <text>From Chen Hallett Green Chem 2014</text>
@@ -3980,16 +4095,22 @@
     </extLst>
   </threadedComment>
   <threadedComment ref="D3" dT="2025-01-31T16:11:12.25" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{224EC866-413C-4C24-91AC-D4B821D21361}">
-    <text>https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf - Pr4NClO4 in ACN</text>
+    <text>Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>3268516475</xltc2:checksum>
-        <xltc2:hyperlink startIndex="0" length="119" url="https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf"/>
+        <xltc2:checksum>1714132109</xltc2:checksum>
+        <xltc2:hyperlink startIndex="35" length="49" url="https://pubs.acs.org/doi/epdf/10.1021/j100845a068"/>
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="D3" dT="2025-01-31T16:24:29.22" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{70A94521-7CD4-4DC0-89E2-F5FAA609E1C2}" parentId="{224EC866-413C-4C24-91AC-D4B821D21361}">
-    <text>Factor of ⅗ to correct for multiple solvents being averaged</text>
+  <threadedComment ref="E3" dT="2025-02-26T23:57:39.00" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{99B3EF73-D9AF-4165-9BAA-2D78D6A936A3}">
+    <text>Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>1714132109</xltc2:checksum>
+        <xltc2:hyperlink startIndex="35" length="49" url="https://pubs.acs.org/doi/epdf/10.1021/j100845a068"/>
+      </x:ext>
+    </extLst>
   </threadedComment>
   <threadedComment ref="C4" dT="2024-11-11T22:11:30.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{2EA54DCB-79E7-4A67-94B1-01E68FDD14D9}">
     <text>From Chen Hallett Green Chem 2014</text>
@@ -4003,17 +4124,27 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="D4" dT="2025-01-31T16:11:12.25" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{24EDBDE4-89F6-4893-A249-65F70D6F4EB5}">
-    <text>https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf - Pr4NClO4 in ACN</text>
+  <threadedComment ref="D4" dT="2025-02-26T15:38:10.17" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{E8DB58D9-FECA-44B0-A45F-2D6CD01B8C82}">
+    <text>Ue Mori JECS 1994 - https://iopscience.iop.org/article/10.1149/1.2059270
+In DMF and ACN, 0.1 M: Shinkle Monroe J Power Sources 2014 -https://doi.org/10.1016/j.jpowsour.2013.10.034
+In PC, any concentration: Ue Mori JECS 1994 - https://iopscience.iop.org/article/10.1149/1.2059270</text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>3268516475</xltc2:checksum>
-        <xltc2:hyperlink startIndex="0" length="119" url="https://www.emerson.com/documents/automation/manual-conductance-data-for-commonly-used-chemicals-rosemount-en-68896.pdf"/>
+        <xltc2:checksum>2718014759</xltc2:checksum>
+        <xltc2:hyperlink startIndex="20" length="52" url="https://iopscience.iop.org/article/10.1149/1.2059270"/>
+        <xltc2:hyperlink startIndex="134" length="46" url="https://doi.org/10.1016/j.jpowsour.2013.10.034"/>
+        <xltc2:hyperlink startIndex="227" length="52" url="https://iopscience.iop.org/article/10.1149/1.2059270"/>
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="D4" dT="2025-01-31T16:24:32.22" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{C1CC95A5-4EB2-4EF1-8C44-0C3BD7C10A3B}" parentId="{24EDBDE4-89F6-4893-A249-65F70D6F4EB5}">
-    <text>Factor of ⅗ to correct for multiple solvents being averaged</text>
+  <threadedComment ref="E4" dT="2025-02-26T23:59:50.66" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{BCA5F20C-1DCE-4C25-8CA7-13042C65B6D7}">
+    <text>Gong Yan EES 2015 - https://doi.org/10.1039/C5EE02341F</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>99962891</xltc2:checksum>
+        <xltc2:hyperlink startIndex="20" length="34" url="https://doi.org/10.1039/C5EE02341F"/>
+      </x:ext>
+    </extLst>
   </threadedComment>
   <threadedComment ref="C5" dT="2024-11-11T22:11:30.12" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{FE69842F-8058-427E-A379-A3530412D42F}">
     <text>From Chen Hallett Green Chem 2014</text>
@@ -4039,6 +4170,15 @@
   <threadedComment ref="D5" dT="2025-01-31T16:24:36.23" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{8C32200A-9B0D-40A9-96BB-139CB0D54BF0}" parentId="{D8A725FE-F27F-4CE0-B881-3504A580D1E3}">
     <text>Factor of ⅗ to correct for multiple solvents being averaged</text>
   </threadedComment>
+  <threadedComment ref="E5" dT="2025-02-26T23:57:44.14" personId="{97EB442A-BA5A-4BA8-A59A-7061902B9186}" id="{47E6C014-E881-40B4-899B-38C111AE0A6F}">
+    <text>Mukherjee Boden J Phys Chem 1969 - https://pubs.acs.org/doi/epdf/10.1021/j100845a068</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>1714132109</xltc2:checksum>
+        <xltc2:hyperlink startIndex="35" length="49" url="https://pubs.acs.org/doi/epdf/10.1021/j100845a068"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -4046,8 +4186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="B30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4079,10 +4219,10 @@
     </row>
     <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="27">
         <v>1</v>
@@ -4095,10 +4235,10 @@
     </row>
     <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="C3" s="27">
         <v>0.3</v>
@@ -4136,7 +4276,7 @@
       <c r="B5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="41">
         <f>0.0145</f>
         <v>1.4500000000000001E-2</v>
       </c>
@@ -4168,49 +4308,49 @@
         <v>127</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" s="23">
         <f>1.3*950000*1.24*(800/444.2)*((1000)/(2160/(Solvents!H2*C19/1000)))^0.7</f>
         <v>57368.495093584941</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="23">
         <f>1.3*1989043*800/596.2</f>
         <v>3469648.9768534047</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -4227,16 +4367,16 @@
         <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="C10" s="8">
         <v>1000</v>
@@ -4268,9 +4408,9 @@
         <v>95</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="55">
+        <v>162</v>
+      </c>
+      <c r="C12" s="54">
         <v>0.3</v>
       </c>
       <c r="D12" s="38"/>
@@ -4549,16 +4689,16 @@
     </row>
     <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A30" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="B30" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="C30" s="46">
+      <c r="C30" s="45">
         <v>500</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="5"/>
@@ -4811,8 +4951,8 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H4" sqref="H4"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4873,10 +5013,10 @@
         <v>70</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>23</v>
@@ -4885,7 +5025,7 @@
         <v>59</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
@@ -4950,39 +5090,39 @@
       <c r="H3" s="10">
         <v>-0.06</v>
       </c>
-      <c r="I3" s="60">
+      <c r="I3" s="58">
         <f>-2.35-0.197-Products[[#This Row],[Standard potential, pH = 0 (V vs SHE)]]</f>
         <v>-2.4870000000000001</v>
       </c>
       <c r="J3" s="38">
         <v>-182</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="58">
         <v>1</v>
       </c>
       <c r="L3" s="10">
         <v>0.89</v>
       </c>
-      <c r="M3" s="58">
+      <c r="M3" s="63">
         <v>0.66700000000000004</v>
       </c>
-      <c r="N3" s="61">
+      <c r="N3" s="59">
         <v>198.8</v>
       </c>
       <c r="O3" s="22" t="s">
         <v>19</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="10">
         <v>90.03</v>
@@ -4993,7 +5133,7 @@
       <c r="E4" s="5">
         <v>2</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="57">
         <v>10000</v>
       </c>
       <c r="G4" s="9">
@@ -5002,7 +5142,7 @@
       <c r="H4" s="10">
         <v>-0.51</v>
       </c>
-      <c r="I4" s="60">
+      <c r="I4" s="58">
         <f>-1.8+0.197-Products[[#This Row],[Standard potential, pH = 0 (V vs SHE)]]</f>
         <v>-1.093</v>
       </c>
@@ -5010,34 +5150,34 @@
         <f>0.2*1000/(3.2-5.2)</f>
         <v>-100</v>
       </c>
-      <c r="K4" s="60">
+      <c r="K4" s="58">
         <v>5.6</v>
       </c>
       <c r="L4" s="6">
         <v>0.7</v>
       </c>
-      <c r="M4" s="58">
+      <c r="M4" s="63">
         <v>0.66700000000000004</v>
       </c>
-      <c r="N4" s="61">
+      <c r="N4" s="59">
         <v>168.6</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P4" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q4" s="22" t="s">
         <v>182</v>
-      </c>
-      <c r="Q4" s="22" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="34" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="C5" s="9">
         <v>46.024999999999999</v>
@@ -5048,7 +5188,7 @@
       <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="56">
+      <c r="F5" s="55">
         <v>5400</v>
       </c>
       <c r="G5" s="9">
@@ -5057,24 +5197,24 @@
       <c r="H5" s="10">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
       <c r="L5" s="6">
         <v>0.69</v>
       </c>
-      <c r="M5" s="58">
+      <c r="M5" s="63">
         <v>0.66700000000000004</v>
       </c>
-      <c r="N5" s="41"/>
+      <c r="N5" s="40"/>
       <c r="O5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="P5" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q5" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
@@ -5094,7 +5234,7 @@
         <v>63</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>68</v>
@@ -5113,7 +5253,7 @@
       </c>
       <c r="L6" s="25"/>
       <c r="M6" s="25"/>
-      <c r="N6" s="45"/>
+      <c r="N6" s="44"/>
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
       <c r="Q6" s="5"/>
@@ -5144,10 +5284,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4385D70-1AE4-4A35-988B-BBC4298D1C90}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5157,55 +5297,52 @@
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="74.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>155</v>
+    <row r="1" spans="1:12" ht="74.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>154</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>145</v>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>144</v>
       </c>
       <c r="B2" s="9">
         <v>41.052</v>
@@ -5223,8 +5360,8 @@
         <f>1/60.7</f>
         <v>1.6474464579901153E-2</v>
       </c>
-      <c r="G2" s="10">
-        <v>1</v>
+      <c r="G2" s="56">
+        <v>6.002662489076708</v>
       </c>
       <c r="H2" s="10">
         <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
@@ -5238,19 +5375,16 @@
         <f>11.9*1000</f>
         <v>11900</v>
       </c>
-      <c r="K2" s="63">
+      <c r="K2" s="60">
         <v>1E-4</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="M2" s="39" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
-        <v>160</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="B3" s="9">
         <v>102.089</v>
@@ -5269,8 +5403,7 @@
         <v>1.2180267965895251E-2</v>
       </c>
       <c r="G3" s="10">
-        <f>1.59/5.69</f>
-        <v>0.27943760984182775</v>
+        <v>1</v>
       </c>
       <c r="H3" s="10">
         <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
@@ -5284,139 +5417,121 @@
         <f>0.05*1000</f>
         <v>50</v>
       </c>
-      <c r="K3" s="63">
+      <c r="K3" s="60">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L3" s="57" t="s">
-        <v>195</v>
-      </c>
-      <c r="M3" s="39" t="s">
+      <c r="L3" s="56" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>161</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>177</v>
       </c>
       <c r="B4" s="9">
+        <v>73.093999999999994</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="29">
+        <v>944.5</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="F4" s="10">
+        <f>1/65.3</f>
+        <v>1.5313935681470138E-2</v>
+      </c>
+      <c r="G4" s="56">
+        <f>0.477748919953973*G2</f>
+        <v>2.8677655210046247</v>
+      </c>
+      <c r="H4" s="10">
+        <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
+        <v>0.17804541879244029</v>
+      </c>
+      <c r="I4" s="10">
+        <f>273.15+152.8</f>
+        <v>425.95</v>
+      </c>
+      <c r="J4" s="8">
+        <f>0.439*1000</f>
+        <v>439</v>
+      </c>
+      <c r="K4" s="60">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="9">
         <v>78.132999999999996</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C5" s="9">
         <v>2.66</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D5" s="29">
         <v>1101</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E5" s="10">
         <v>1.9870000000000001</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F5" s="10">
         <f>1/101.6</f>
         <v>9.8425196850393699E-3</v>
       </c>
-      <c r="G4" s="10">
-        <f>2.36/5.69</f>
-        <v>0.41476274165202104</v>
-      </c>
-      <c r="H4" s="10">
+      <c r="G5" s="56">
+        <f>2.36/5.69*G2</f>
+        <v>2.4896807511812002</v>
+      </c>
+      <c r="H5" s="10">
         <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
         <v>0.10758872701426347</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I5" s="10">
         <f>273.15+191.9</f>
         <v>465.04999999999995</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J5" s="8">
         <f>0.084*1000</f>
         <v>84</v>
       </c>
-      <c r="K4" s="63">
+      <c r="K5" s="60">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="M4" s="39" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="9">
-        <v>73.093999999999994</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="29">
-        <v>944.5</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="F5" s="10">
-        <f>1/65.3</f>
-        <v>1.5313935681470138E-2</v>
-      </c>
-      <c r="G5" s="10">
-        <f>3.34/5.69</f>
-        <v>0.58699472759226712</v>
-      </c>
-      <c r="H5" s="10">
-        <f>Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692/(1-Products6[[#This Row],[Henry''s constant at 298K, CO2 (mole fraction/atm)]]*9.8692)</f>
-        <v>0.17804541879244029</v>
-      </c>
-      <c r="I5" s="10">
-        <f>273.15+152.8</f>
-        <v>425.95</v>
-      </c>
-      <c r="J5" s="8">
-        <f>0.439*1000</f>
-        <v>439</v>
-      </c>
-      <c r="K5" s="63">
-        <v>1.0000000000000001E-5</v>
-      </c>
       <c r="L5" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="M5" s="39" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="57" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
-        <v>198</v>
-      </c>
-      <c r="I7" s="64"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I8" s="64"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I9" s="64"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I10" s="64"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" s="64"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I7" s="61"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I8" s="61"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I9" s="61"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="61"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I11" s="61"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="Izutsu (Wiley 2009)" xr:uid="{3CE65C60-DA75-4595-8CAA-88F2C9A358C9}"/>
-    <hyperlink ref="M3" r:id="rId2" display="Izutsu (Wiley 2009)" xr:uid="{6B0DA7F9-0782-4596-8B42-F9EBE5175294}"/>
-    <hyperlink ref="M4" r:id="rId3" display="Izutsu (Wiley 2009)" xr:uid="{55B29BD6-B10F-4DCF-93BE-7B2953D8D605}"/>
-    <hyperlink ref="M5" r:id="rId4" display="Izutsu (Wiley 2009)" xr:uid="{A3AEBAE1-B668-4BB3-9056-8F0FA6D1359D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5425,41 +5540,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8976AAB6-E21A-42F8-BEF8-70CDE446E133}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>157</v>
+    <row r="1" spans="1:7" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>156</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>199</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>196</v>
       </c>
       <c r="B2" s="9">
         <v>341.91</v>
@@ -5467,21 +5582,18 @@
       <c r="C2" s="9">
         <v>10</v>
       </c>
-      <c r="D2" s="58">
-        <f>5.69/1000</f>
-        <v>5.6900000000000006E-3</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="D2" s="65">
+        <v>1.0090104598197338E-2</v>
+      </c>
+      <c r="E2" s="65">
+        <v>28.17</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
-        <v>200</v>
+      <c r="A3" s="42" t="s">
+        <v>197</v>
       </c>
       <c r="B3" s="9">
         <v>229.74</v>
@@ -5489,15 +5601,16 @@
       <c r="C3" s="9">
         <v>10</v>
       </c>
-      <c r="D3" s="58">
-        <f>1000/1000000*0.3*172.3*(1-2.08*SQRT(0.3)+2.4*(0.3))</f>
-        <v>3.0018299685320562E-2</v>
-      </c>
-      <c r="E3" s="22"/>
+      <c r="D3" s="65">
+        <v>1.0002209009565739E-2</v>
+      </c>
+      <c r="E3" s="65">
+        <v>32.65</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>201</v>
+      <c r="A4" s="42" t="s">
+        <v>198</v>
       </c>
       <c r="B4" s="9">
         <v>329.27</v>
@@ -5505,16 +5618,17 @@
       <c r="C4" s="9">
         <v>10</v>
       </c>
-      <c r="D4" s="40">
-        <f>1000/1000000*0.3*172.3*(1-2.08*SQRT(0.3)+2.4*(0.3))</f>
-        <v>3.0018299685320562E-2</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="65"/>
+      <c r="D4" s="64">
+        <v>5.4603421645070798E-3</v>
+      </c>
+      <c r="E4" s="65">
+        <v>20.844999999999999</v>
+      </c>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
-        <v>197</v>
+      <c r="A5" s="42" t="s">
+        <v>195</v>
       </c>
       <c r="B5" s="9">
         <v>165.74</v>
@@ -5522,12 +5636,13 @@
       <c r="C5" s="9">
         <v>10</v>
       </c>
-      <c r="D5" s="58">
-        <f>1000/1000000*0.3*169.6*(1-2.1*SQRT(0.3)+10*(0.3))</f>
-        <v>0.14499694017568801</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="65"/>
+      <c r="D5" s="65">
+        <v>1.1860136423114074E-2</v>
+      </c>
+      <c r="E5" s="64">
+        <v>31.64</v>
+      </c>
+      <c r="F5" s="62"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -5544,15 +5659,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="49" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
@@ -5563,10 +5678,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5575,18 +5690,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="50">
         <v>2.4E-2</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="51">
         <v>50</v>
       </c>
       <c r="D3" s="28" t="s">
@@ -5603,10 +5718,10 @@
       <c r="A4" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="50">
         <v>2.4E-2</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="51">
         <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
@@ -5619,10 +5734,10 @@
       <c r="A5" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="50">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C5" s="52"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="28" t="s">
         <v>131</v>
       </c>
@@ -5631,11 +5746,11 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="50">
         <f>16.05/100</f>
         <v>0.1605</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="51">
         <v>230.93061430996579</v>
       </c>
       <c r="D6" s="28" t="s">
@@ -5646,26 +5761,26 @@
       <c r="A7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="50">
         <f>8.19/100</f>
         <v>8.1900000000000001E-2</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="51">
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B8" s="50">
         <f>2.22/kWh_per_mmBtu</f>
         <v>7.5691136219420956E-3</v>
       </c>
-      <c r="C8" s="52">
+      <c r="C8" s="51">
         <f>70.66/1000*kJ_per_kWh</f>
         <v>254.376</v>
       </c>
@@ -5677,29 +5792,29 @@
       <c r="A9" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="50">
         <v>0.03</v>
       </c>
-      <c r="C9" s="53"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="53"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="50">
         <f>B7</f>
         <v>8.1900000000000001E-2</v>
       </c>
-      <c r="C11" s="53">
+      <c r="C11" s="52">
         <f>C7</f>
         <v>414.10433834299573</v>
       </c>
@@ -5709,11 +5824,11 @@
       <c r="A12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="53">
         <f>B8</f>
         <v>7.5691136219420956E-3</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="52">
         <f>C8</f>
         <v>254.376</v>
       </c>
@@ -5721,18 +5836,18 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="51">
+      <c r="B14" s="50">
         <v>200</v>
       </c>
-      <c r="C14" s="53"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="32" t="s">
         <v>113</v>
       </c>

</xml_diff>